<commit_message>
Implementation of data for column extraction.
</commit_message>
<xml_diff>
--- a/data/LDH_attributes.xlsx
+++ b/data/LDH_attributes.xlsx
@@ -8,21 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chant\PycharmProjects\FUSE-V2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{192C16E1-B6CC-499D-A1ED-278F86171921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3650968-3AB8-46F6-8AFA-2A74E7C53305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="9" xr2:uid="{9D386D14-BB1A-49FB-A5CB-94A6FCCCA1F9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="5" activeTab="14" xr2:uid="{9D386D14-BB1A-49FB-A5CB-94A6FCCCA1F9}"/>
   </bookViews>
   <sheets>
-    <sheet name="chemicals" sheetId="2" r:id="rId1"/>
-    <sheet name="RMM" sheetId="9" r:id="rId2"/>
-    <sheet name="densities" sheetId="7" r:id="rId3"/>
-    <sheet name="heat capacities" sheetId="8" r:id="rId4"/>
-    <sheet name="reaction conditions" sheetId="3" r:id="rId5"/>
-    <sheet name="impeller" sheetId="4" r:id="rId6"/>
-    <sheet name="pump" sheetId="10" r:id="rId7"/>
-    <sheet name="water" sheetId="5" r:id="rId8"/>
-    <sheet name="costs" sheetId="11" r:id="rId9"/>
-    <sheet name="equipment" sheetId="6" r:id="rId10"/>
+    <sheet name="chemicals_sorbent_synthesis" sheetId="2" r:id="rId1"/>
+    <sheet name="washing" sheetId="12" r:id="rId2"/>
+    <sheet name="column" sheetId="17" r:id="rId3"/>
+    <sheet name="stripping" sheetId="13" r:id="rId4"/>
+    <sheet name="FO" sheetId="16" r:id="rId5"/>
+    <sheet name="densities" sheetId="7" r:id="rId6"/>
+    <sheet name="heat capacities" sheetId="8" r:id="rId7"/>
+    <sheet name="brine" sheetId="14" r:id="rId8"/>
+    <sheet name="plant" sheetId="15" r:id="rId9"/>
+    <sheet name="reaction conditions" sheetId="3" r:id="rId10"/>
+    <sheet name="impeller" sheetId="4" r:id="rId11"/>
+    <sheet name="pump" sheetId="10" r:id="rId12"/>
+    <sheet name="water" sheetId="5" r:id="rId13"/>
+    <sheet name="costs" sheetId="11" r:id="rId14"/>
+    <sheet name="equipment" sheetId="6" r:id="rId15"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="176">
   <si>
     <t>key</t>
   </si>
@@ -133,9 +138,6 @@
   </si>
   <si>
     <t>95 degree C</t>
-  </si>
-  <si>
-    <t>Paranthaman 2017</t>
   </si>
   <si>
     <t>Hammer mill</t>
@@ -248,15 +250,6 @@
     <t>J/(kg*K)</t>
   </si>
   <si>
-    <t>Pubchem</t>
-  </si>
-  <si>
-    <t>g/mol</t>
-  </si>
-  <si>
-    <t>LiCl</t>
-  </si>
-  <si>
     <t>Heating and stirring</t>
   </si>
   <si>
@@ -471,6 +464,120 @@
   </si>
   <si>
     <t>yield</t>
+  </si>
+  <si>
+    <t>Paranthaman 2017, Huang 2021</t>
+  </si>
+  <si>
+    <t>brine</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>sorbent</t>
+  </si>
+  <si>
+    <t>H2O_washing</t>
+  </si>
+  <si>
+    <t>per washing cycle</t>
+  </si>
+  <si>
+    <t>NaCl_conc</t>
+  </si>
+  <si>
+    <t>g/l</t>
+  </si>
+  <si>
+    <t>5 wt% solution</t>
+  </si>
+  <si>
+    <t>No_washing_cycles</t>
+  </si>
+  <si>
+    <t>H2O_stripping</t>
+  </si>
+  <si>
+    <t>No_stripping_cycles</t>
+  </si>
+  <si>
+    <t>Sorbent Synthesis</t>
+  </si>
+  <si>
+    <t>assuming density of water</t>
+  </si>
+  <si>
+    <t>brine_specific_enthalpy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> kJ/kg</t>
+  </si>
+  <si>
+    <t>brine_flow_day</t>
+  </si>
+  <si>
+    <t>m^3/day</t>
+  </si>
+  <si>
+    <t>h/year</t>
+  </si>
+  <si>
+    <t>years</t>
+  </si>
+  <si>
+    <t>LiCl_conc_brine</t>
+  </si>
+  <si>
+    <t>LiCl_conc_stripping</t>
+  </si>
+  <si>
+    <t>LiCl_sol_output</t>
+  </si>
+  <si>
+    <t>LiCl_conc_FO</t>
+  </si>
+  <si>
+    <t>plant_lifetime</t>
+  </si>
+  <si>
+    <t>plan_uptime</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>Huang 2021, Paranthaman 2017</t>
+  </si>
+  <si>
+    <t>Li_recovery</t>
+  </si>
+  <si>
+    <t>BV/h</t>
+  </si>
+  <si>
+    <t>BV = bed volume</t>
+  </si>
+  <si>
+    <t>brine_flow_rate</t>
+  </si>
+  <si>
+    <t>washing_flow_rate</t>
+  </si>
+  <si>
+    <t>stripping_flow_rate</t>
+  </si>
+  <si>
+    <t>Extraction column</t>
+  </si>
+  <si>
+    <t>FO unit</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>Membrane lifetime 500 h</t>
   </si>
 </sst>
 </file>
@@ -857,7 +964,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -867,7 +974,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -886,7 +993,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -894,18 +1001,18 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5">
         <v>0.7</v>
@@ -916,7 +1023,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -924,7 +1031,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -932,7 +1039,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -940,21 +1047,21 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" s="1">
         <v>50</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B11">
         <v>0.9</v>
@@ -967,586 +1074,11 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0624EAC2-56E2-4337-8D5D-42EAA0559452}">
-  <dimension ref="A1:M10"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" customWidth="1"/>
-    <col min="5" max="5" width="7.44140625" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G2" t="s">
-        <v>74</v>
-      </c>
-      <c r="H2" t="s">
-        <v>73</v>
-      </c>
-      <c r="I2" t="s">
-        <v>89</v>
-      </c>
-      <c r="J2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D3">
-        <v>37500</v>
-      </c>
-      <c r="E3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" t="s">
-        <v>78</v>
-      </c>
-      <c r="G3">
-        <v>3</v>
-      </c>
-      <c r="H3">
-        <v>0.5</v>
-      </c>
-      <c r="I3" t="s">
-        <v>90</v>
-      </c>
-      <c r="J3" t="s">
-        <v>71</v>
-      </c>
-      <c r="K3">
-        <v>0.53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4">
-        <v>230000</v>
-      </c>
-      <c r="E4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4" t="s">
-        <v>79</v>
-      </c>
-      <c r="G4">
-        <v>150</v>
-      </c>
-      <c r="H4">
-        <v>20</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="J4" t="s">
-        <v>15</v>
-      </c>
-      <c r="K4">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5">
-        <v>63000</v>
-      </c>
-      <c r="E5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" t="s">
-        <v>75</v>
-      </c>
-      <c r="G5">
-        <v>15</v>
-      </c>
-      <c r="H5">
-        <v>4</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="J5" t="s">
-        <v>76</v>
-      </c>
-      <c r="K5">
-        <v>0.81</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" t="s">
-        <v>82</v>
-      </c>
-      <c r="D6">
-        <v>9500</v>
-      </c>
-      <c r="E6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" t="s">
-        <v>75</v>
-      </c>
-      <c r="G6">
-        <v>23</v>
-      </c>
-      <c r="H6">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="J6" t="s">
-        <v>76</v>
-      </c>
-      <c r="K6">
-        <v>0.79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C7" t="s">
-        <v>86</v>
-      </c>
-      <c r="D7">
-        <v>4800</v>
-      </c>
-      <c r="E7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" t="s">
-        <v>84</v>
-      </c>
-      <c r="G7">
-        <v>7.5</v>
-      </c>
-      <c r="H7">
-        <v>2.54</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="J7" t="s">
-        <v>85</v>
-      </c>
-      <c r="K7">
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>101</v>
-      </c>
-      <c r="D8">
-        <v>80</v>
-      </c>
-      <c r="E8" t="s">
-        <v>95</v>
-      </c>
-      <c r="F8" t="s">
-        <v>84</v>
-      </c>
-      <c r="G8">
-        <v>15</v>
-      </c>
-      <c r="H8">
-        <v>20</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="J8" t="s">
-        <v>85</v>
-      </c>
-      <c r="K8">
-        <v>1.33</v>
-      </c>
-      <c r="L8">
-        <v>100</v>
-      </c>
-      <c r="M8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>139</v>
-      </c>
-      <c r="B10">
-        <v>650</v>
-      </c>
-      <c r="C10" t="s">
-        <v>88</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="I6" r:id="rId1" xr:uid="{7FC25CF3-66CB-4D0A-BB61-3B4475B2C819}"/>
-    <hyperlink ref="I5" r:id="rId2" xr:uid="{29B1090E-3E0E-4959-9517-01ECBE15B1E6}"/>
-    <hyperlink ref="I4" r:id="rId3" xr:uid="{699EF7F5-147A-4A45-9703-96F569E8802F}"/>
-    <hyperlink ref="I7" r:id="rId4" xr:uid="{292D848F-3DC3-42FF-B115-46148EDFD2A8}"/>
-    <hyperlink ref="I8" r:id="rId5" xr:uid="{CE857C8C-06BA-4606-B21B-E83F455C3B82}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{694DF68E-82AD-4767-96EA-71D620D0A7E2}">
-  <dimension ref="A1:C7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3">
-        <v>42</v>
-      </c>
-      <c r="C3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4">
-        <v>81.028000000000006</v>
-      </c>
-      <c r="C4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5">
-        <v>18.015000000000001</v>
-      </c>
-      <c r="C5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6">
-        <v>36.46</v>
-      </c>
-      <c r="C6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B7">
-        <v>42.4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB00B591-781D-4B14-8638-75E48C4EE83F}">
-  <dimension ref="A1:C7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3">
-        <v>2.54</v>
-      </c>
-      <c r="C3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4">
-        <v>1.51</v>
-      </c>
-      <c r="C4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5">
-        <v>2.42</v>
-      </c>
-      <c r="C5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6">
-        <f>1.639*10^-3</f>
-        <v>1.639E-3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FFA5140-DB51-449E-B884-903ABFBFFC40}">
-  <dimension ref="A1:F7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3">
-        <v>42.140040999999997</v>
-      </c>
-      <c r="C3">
-        <v>145.8434</v>
-      </c>
-      <c r="D3">
-        <v>-110.7379</v>
-      </c>
-      <c r="E3">
-        <v>32.62106</v>
-      </c>
-      <c r="F3">
-        <v>-0.48494700000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4">
-        <v>32.123919999999998</v>
-      </c>
-      <c r="C4">
-        <v>-13.45805</v>
-      </c>
-      <c r="D4">
-        <v>19.86852</v>
-      </c>
-      <c r="E4">
-        <v>-6.853936</v>
-      </c>
-      <c r="F4">
-        <v>-4.9672000000000001E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5">
-        <v>-203.60599999999999</v>
-      </c>
-      <c r="C5">
-        <v>1523.29</v>
-      </c>
-      <c r="D5">
-        <v>-3196.413</v>
-      </c>
-      <c r="E5">
-        <v>2474.4450000000002</v>
-      </c>
-      <c r="F5">
-        <v>3.8553259999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7">
-        <v>1193</v>
-      </c>
-      <c r="C7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A644868A-CA0D-4E33-AC4A-13C92D1F9685}">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1557,7 +1089,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1576,7 +1108,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>70</v>
+        <v>150</v>
+      </c>
+      <c r="D3" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1609,7 +1144,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -1637,7 +1172,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8">
         <v>6.3499999999999997E-3</v>
@@ -1651,7 +1186,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9">
         <v>3.7160000000000002</v>
@@ -1660,7 +1195,7 @@
         <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1669,12 +1204,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A0F109E-90BE-42A5-8DFF-EE3A7F8215F0}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1748,7 +1283,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7">
         <v>0.9</v>
@@ -1759,7 +1294,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB9B9DC-89ED-462F-B40D-72EC74E0973E}">
   <dimension ref="A1:D13"/>
   <sheetViews>
@@ -1774,7 +1309,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B1">
         <v>2016</v>
@@ -1791,12 +1326,12 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -1805,63 +1340,63 @@
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D6" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D8" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B10">
         <v>30</v>
@@ -1872,7 +1407,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B11">
         <v>0.2</v>
@@ -1883,13 +1418,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B12">
         <v>0.75</v>
       </c>
       <c r="D12" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1900,10 +1435,10 @@
         <v>9.81</v>
       </c>
       <c r="C13" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1911,7 +1446,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{489F410F-4873-4D81-A8B1-2DDFA51D15D5}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -1941,7 +1476,7 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1951,7 +1486,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B4">
         <v>1.5</v>
@@ -1960,7 +1495,7 @@
         <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1968,7 +1503,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F37A8F43-ECBD-4243-988B-AAA9A59B3D22}">
   <dimension ref="A2:E7"/>
   <sheetViews>
@@ -1986,57 +1521,57 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B3">
         <v>6.6600000000000006E-2</v>
       </c>
       <c r="D3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B4">
         <v>0.01</v>
       </c>
       <c r="D4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5">
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6">
         <v>0.3</v>
@@ -2045,15 +1580,15 @@
         <v>0.7</v>
       </c>
       <c r="D6" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7">
         <v>0.15</v>
@@ -2062,10 +1597,10 @@
         <v>0.45</v>
       </c>
       <c r="D7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E7" t="s">
         <v>130</v>
-      </c>
-      <c r="E7" t="s">
-        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -2075,4 +1610,1011 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0624EAC2-56E2-4337-8D5D-42EAA0559452}">
+  <dimension ref="A1:M13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" customWidth="1"/>
+    <col min="5" max="5" width="7.44140625" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3">
+        <v>37500</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>0.5</v>
+      </c>
+      <c r="I3" t="s">
+        <v>67</v>
+      </c>
+      <c r="J3" t="s">
+        <v>86</v>
+      </c>
+      <c r="K3">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4">
+        <v>230000</v>
+      </c>
+      <c r="E4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4">
+        <v>150</v>
+      </c>
+      <c r="H4">
+        <v>20</v>
+      </c>
+      <c r="I4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="K4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5">
+        <v>63000</v>
+      </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G5">
+        <v>15</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5" t="s">
+        <v>72</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K5">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6">
+        <v>9500</v>
+      </c>
+      <c r="E6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G6">
+        <v>23</v>
+      </c>
+      <c r="H6">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I6" t="s">
+        <v>72</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K6">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7">
+        <v>4800</v>
+      </c>
+      <c r="E7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" t="s">
+        <v>80</v>
+      </c>
+      <c r="G7">
+        <v>7.5</v>
+      </c>
+      <c r="H7">
+        <v>2.54</v>
+      </c>
+      <c r="I7" t="s">
+        <v>81</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="K7">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8">
+        <v>80</v>
+      </c>
+      <c r="E8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" t="s">
+        <v>80</v>
+      </c>
+      <c r="G8">
+        <v>15</v>
+      </c>
+      <c r="H8">
+        <v>20</v>
+      </c>
+      <c r="I8" t="s">
+        <v>81</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="K8">
+        <v>1.33</v>
+      </c>
+      <c r="L8">
+        <v>100</v>
+      </c>
+      <c r="M8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>172</v>
+      </c>
+      <c r="C9" t="s">
+        <v>175</v>
+      </c>
+      <c r="D9">
+        <v>380000</v>
+      </c>
+      <c r="E9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9">
+        <v>10</v>
+      </c>
+      <c r="H9">
+        <v>12</v>
+      </c>
+      <c r="J9" t="s">
+        <v>84</v>
+      </c>
+      <c r="K9">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>173</v>
+      </c>
+      <c r="D10">
+        <v>22000</v>
+      </c>
+      <c r="E10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" t="s">
+        <v>174</v>
+      </c>
+      <c r="G10">
+        <v>1600</v>
+      </c>
+      <c r="H10">
+        <v>3593</v>
+      </c>
+      <c r="I10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" t="s">
+        <v>84</v>
+      </c>
+      <c r="K10">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>135</v>
+      </c>
+      <c r="B13">
+        <v>650</v>
+      </c>
+      <c r="C13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J6" r:id="rId1" xr:uid="{7FC25CF3-66CB-4D0A-BB61-3B4475B2C819}"/>
+    <hyperlink ref="J5" r:id="rId2" xr:uid="{29B1090E-3E0E-4959-9517-01ECBE15B1E6}"/>
+    <hyperlink ref="J4" r:id="rId3" xr:uid="{699EF7F5-147A-4A45-9703-96F569E8802F}"/>
+    <hyperlink ref="J7" r:id="rId4" xr:uid="{292D848F-3DC3-42FF-B115-46148EDFD2A8}"/>
+    <hyperlink ref="J8" r:id="rId5" xr:uid="{CE857C8C-06BA-4606-B21B-E83F455C3B82}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{057E51FA-16AA-4EDB-95D7-E76738AA23C5}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B3">
+        <v>1383.46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B4">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="C4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B5">
+        <v>69.17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>140</v>
+      </c>
+      <c r="D6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>144</v>
+      </c>
+      <c r="B7">
+        <v>50</v>
+      </c>
+      <c r="C7" t="s">
+        <v>145</v>
+      </c>
+      <c r="D7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>147</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5B35FB0-FC35-4894-B852-40A6833023F4}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B3">
+        <v>2.5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4">
+        <v>0.1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B5">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>167</v>
+      </c>
+      <c r="D6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4E9EB40-91BA-4B28-833D-B3DB1EE1EE78}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B5">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B6">
+        <v>1.71</v>
+      </c>
+      <c r="C6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{285FC4B4-1D25-4960-A894-56724304077E}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B3">
+        <v>174</v>
+      </c>
+      <c r="C3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B4">
+        <v>1.54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB00B591-781D-4B14-8638-75E48C4EE83F}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3">
+        <v>2.54</v>
+      </c>
+      <c r="C3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4">
+        <v>1.51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5">
+        <v>2.42</v>
+      </c>
+      <c r="C5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6">
+        <f>1.639*10^-3</f>
+        <v>1.639E-3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FFA5140-DB51-449E-B884-903ABFBFFC40}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3">
+        <v>42.140040999999997</v>
+      </c>
+      <c r="C3">
+        <v>145.8434</v>
+      </c>
+      <c r="D3">
+        <v>-110.7379</v>
+      </c>
+      <c r="E3">
+        <v>32.62106</v>
+      </c>
+      <c r="F3">
+        <v>-0.48494700000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4">
+        <v>32.123919999999998</v>
+      </c>
+      <c r="C4">
+        <v>-13.45805</v>
+      </c>
+      <c r="D4">
+        <v>19.86852</v>
+      </c>
+      <c r="E4">
+        <v>-6.853936</v>
+      </c>
+      <c r="F4">
+        <v>-4.9672000000000001E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5">
+        <v>-203.60599999999999</v>
+      </c>
+      <c r="C5">
+        <v>1523.29</v>
+      </c>
+      <c r="D5">
+        <v>-3196.413</v>
+      </c>
+      <c r="E5">
+        <v>2474.4450000000002</v>
+      </c>
+      <c r="F5">
+        <v>3.8553259999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7">
+        <v>1193</v>
+      </c>
+      <c r="C7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C77679F-E498-462D-825B-EAF86D6734F3}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B3">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="C3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B4">
+        <v>1204.67</v>
+      </c>
+      <c r="C4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9896EE1E-7F56-45CB-B0FF-A4EB36B766F1}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B3">
+        <v>35000</v>
+      </c>
+      <c r="C3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B4">
+        <v>7920</v>
+      </c>
+      <c r="C4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implementation of opex for production of lithium carboante from brine
</commit_message>
<xml_diff>
--- a/data/LDH_attributes.xlsx
+++ b/data/LDH_attributes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chant\PycharmProjects\FUSE-V2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE2455D-D23E-4CD8-948E-C7468227169E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{697F1CE5-732F-4ED1-B7A2-11C36CE27463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="12" xr2:uid="{9D386D14-BB1A-49FB-A5CB-94A6FCCCA1F9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="8" activeTab="14" xr2:uid="{9D386D14-BB1A-49FB-A5CB-94A6FCCCA1F9}"/>
   </bookViews>
   <sheets>
     <sheet name="column" sheetId="17" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="234">
   <si>
     <t>key</t>
   </si>
@@ -396,9 +396,6 @@
     <t>https://www.alibaba.com/product-detail/Exporter-hot-sale-Hydrochloric-Acid-Factory_1600289913553.html?spm=a2700.galleryofferlist.normal_offer.d_title.3a8e2c51jUtwul&amp;s=p</t>
   </si>
   <si>
-    <t>https://www.alibaba.com/product-detail/Factory-supply-Industry-Grade-Price-Aluminum_1600101390190.html?spm=a2700.galleryofferlist.normal_offer.d_title.54ab1a51KPV513&amp;s=p</t>
-  </si>
-  <si>
     <t>electricity_industry</t>
   </si>
   <si>
@@ -526,9 +523,6 @@
   </si>
   <si>
     <t>lab scale</t>
-  </si>
-  <si>
-    <t>annual wage</t>
   </si>
   <si>
     <t>untis</t>
@@ -718,12 +712,85 @@
   <si>
     <t>LC_purification_washing</t>
   </si>
+  <si>
+    <t>bring reactants in aqueous solution</t>
+  </si>
+  <si>
+    <t>LC_processing_aq</t>
+  </si>
+  <si>
+    <t>l/g</t>
+  </si>
+  <si>
+    <t>CO2</t>
+  </si>
+  <si>
+    <t>https://www.alibaba.com/product-detail/high-quality-Soda-Ash-Dense-Na2CO3_62240433604.html?spm=a2700.galleryofferlist.0.0.4987214e22kx0L&amp;s=p</t>
+  </si>
+  <si>
+    <r>
+      <t>Na</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CO</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+  </si>
+  <si>
+    <t>https://sefindustry.en.alibaba.com/product/60759731750-803350891/68L_Co2_Gas_Cylinder_Widely_Used_For_Medical_Industry.html?spm=a2700.shop_plgr.41413.12.6add2cd2Se7L8y</t>
+  </si>
+  <si>
+    <t>lower if &gt; 450000</t>
+  </si>
+  <si>
+    <t>https://www.alibaba.com/product-detail/High-quality-flame-retardant-aluminum-hydroxide_1600269818787.html?spm=a2700.galleryofferlist.normal_offer.d_title.3be46679ztCxlv&amp;s=p</t>
+  </si>
+  <si>
+    <t>Date accessed 17/08/2021</t>
+  </si>
+  <si>
+    <t>annual_wage</t>
+  </si>
+  <si>
+    <t>supervision</t>
+  </si>
+  <si>
+    <t>Cost factors in % of operating labout</t>
+  </si>
+  <si>
+    <t>quality_control</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -774,6 +841,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -796,13 +870,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1131,7 +1206,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1150,7 +1225,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B3">
         <v>2.5</v>
@@ -1159,7 +1234,7 @@
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1173,12 +1248,12 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B5">
         <v>0.9</v>
@@ -1186,43 +1261,43 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B7">
         <v>8</v>
       </c>
       <c r="C7" t="s">
+        <v>151</v>
+      </c>
+      <c r="D7" t="s">
         <v>152</v>
-      </c>
-      <c r="D7" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B8">
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1245,7 +1320,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1259,23 +1334,23 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B4" s="1">
         <v>0.9</v>
@@ -1286,7 +1361,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B5" s="1">
         <v>0.8</v>
@@ -1297,32 +1372,32 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B6">
         <v>298.14999999999998</v>
       </c>
       <c r="C6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B7">
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B8" s="1">
         <v>2</v>
@@ -1336,7 +1411,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B9">
         <v>353</v>
@@ -1347,18 +1422,18 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
@@ -1414,13 +1489,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B15" s="1">
         <v>5000</v>
       </c>
       <c r="C15" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D15" t="s">
         <v>47</v>
@@ -1428,7 +1503,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B16">
         <v>0.8</v>
@@ -1436,13 +1511,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B17">
         <v>313.14999999999998</v>
       </c>
       <c r="D17" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -1695,10 +1770,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{489F410F-4873-4D81-A8B1-2DDFA51D15D5}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1707,12 +1782,12 @@
     <col min="2" max="2" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1723,53 +1798,78 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B3">
-        <v>1.5</v>
+        <f xml:space="preserve"> 1.5 * 10^(-3)</f>
+        <v>1.5E-3</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>222</v>
       </c>
       <c r="D3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>221</v>
       </c>
-      <c r="B4">
-        <v>10000</v>
+      <c r="B4" s="1">
+        <f>1*10^-3</f>
+        <v>1E-3</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>222</v>
+      </c>
+      <c r="D4" t="s">
+        <v>220</v>
+      </c>
+      <c r="H4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B5" s="1">
+        <f>1.5*10^-3</f>
+        <v>1.5E-3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>222</v>
+      </c>
+      <c r="H5" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F37A8F43-ECBD-4243-988B-AAA9A59B3D22}">
-  <dimension ref="A2:E7"/>
+  <dimension ref="A2:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1779,10 +1879,16 @@
       <c r="C2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B3">
         <v>6.6600000000000006E-2</v>
@@ -1790,11 +1896,11 @@
       <c r="D3" t="s">
         <v>110</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>111</v>
       </c>
@@ -1804,11 +1910,11 @@
       <c r="D4" t="s">
         <v>112</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>49</v>
       </c>
@@ -1818,28 +1924,28 @@
       <c r="D5" t="s">
         <v>113</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B6">
-        <v>0.3</v>
+        <v>0.51</v>
       </c>
       <c r="C6">
-        <v>0.7</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D6" t="s">
         <v>113</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -1852,25 +1958,68 @@
       <c r="D7" t="s">
         <v>113</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" s="2" t="s">
         <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B8">
+        <v>0.17</v>
+      </c>
+      <c r="C8">
+        <v>0.24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>113</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>223</v>
+      </c>
+      <c r="B9">
+        <f>30/45</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C9">
+        <f>190/45</f>
+        <v>4.2222222222222223</v>
+      </c>
+      <c r="D9" t="s">
+        <v>113</v>
+      </c>
+      <c r="E9" t="s">
+        <v>227</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>226</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E5" r:id="rId1" xr:uid="{C24F39EA-311C-4837-8AF3-5D85600B4F85}"/>
+    <hyperlink ref="F5" r:id="rId1" xr:uid="{C24F39EA-311C-4837-8AF3-5D85600B4F85}"/>
+    <hyperlink ref="F8" r:id="rId2" xr:uid="{BF3F774C-FF6C-4AEB-A9E4-FAFC8DEEC8C0}"/>
+    <hyperlink ref="F9" r:id="rId3" xr:uid="{046E4B52-F126-401E-8CFF-B220378AEB37}"/>
+    <hyperlink ref="F7" r:id="rId4" xr:uid="{ACAB8517-70FE-4BA5-9A1E-BE8833BF3BFC}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{2C6DF56B-0E94-4370-AA83-F48A81BF5478}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId6"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1330EF6F-438D-41F9-93CA-537B5AFAC263}">
-  <dimension ref="A2:H4"/>
+  <dimension ref="A2:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1886,12 +2035,15 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>163</v>
+        <v>161</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>162</v>
+        <v>230</v>
       </c>
       <c r="B3">
         <v>81890</v>
@@ -1900,21 +2052,45 @@
         <v>35</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>166</v>
-      </c>
-      <c r="B4">
+        <v>164</v>
+      </c>
+      <c r="B4" s="1">
         <v>45</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H4" t="s">
-        <v>167</v>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>231</v>
+      </c>
+      <c r="B6">
+        <v>0.2</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>233</v>
+      </c>
+      <c r="B7">
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>
@@ -1954,13 +2130,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C2" t="s">
         <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E2" t="s">
         <v>34</v>
@@ -1989,7 +2165,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -2067,7 +2243,7 @@
         <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E6">
         <v>63000</v>
@@ -2096,15 +2272,15 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E8">
         <v>380000</v>
@@ -2127,7 +2303,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E9">
         <v>22000</v>
@@ -2136,7 +2312,7 @@
         <v>35</v>
       </c>
       <c r="G9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H9">
         <v>1600</v>
@@ -2156,12 +2332,12 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -2176,78 +2352,78 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C16" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D16" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D17" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B18" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D18" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B19" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C19" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D19" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D20" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D21" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
@@ -2357,7 +2533,7 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B28">
         <v>650</v>
@@ -2413,29 +2589,29 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B3">
         <v>1383.46</v>
       </c>
       <c r="C3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B4">
         <v>0.19400000000000001</v>
       </c>
       <c r="C4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B5">
         <v>69.17</v>
@@ -2446,35 +2622,35 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B6">
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B7">
         <v>50</v>
       </c>
       <c r="C7" t="s">
+        <v>130</v>
+      </c>
+      <c r="D7" t="s">
         <v>131</v>
-      </c>
-      <c r="D7" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -2513,18 +2689,18 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B3">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -2532,24 +2708,24 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B5">
         <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B6">
         <v>1.71</v>
       </c>
       <c r="C6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -2596,24 +2772,24 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B4">
         <v>174</v>
       </c>
       <c r="C4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B5">
         <v>1.54</v>
       </c>
       <c r="C5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -2655,41 +2831,41 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B3">
         <v>0.19400000000000001</v>
       </c>
       <c r="C3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B4">
         <v>1204.67</v>
       </c>
       <c r="C4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -2728,35 +2904,35 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B3">
         <v>35000</v>
       </c>
       <c r="C3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B4">
         <v>7920</v>
       </c>
       <c r="C4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B5">
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -2779,7 +2955,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -2866,7 +3042,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B11">
         <v>0.9</v>
@@ -2883,7 +3059,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:K9"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2913,7 +3089,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D3" t="s">
         <v>53</v>
@@ -3024,7 +3200,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -3037,7 +3213,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3">
         <v>0.7</v>
@@ -3056,7 +3232,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B5" s="1">
         <v>2</v>

</xml_diff>

<commit_message>
Problem in opex file fixed and universal file path implemented for all files
</commit_message>
<xml_diff>
--- a/data/LDH_attributes.xlsx
+++ b/data/LDH_attributes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chant\PycharmProjects\FUSE-V2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{697F1CE5-732F-4ED1-B7A2-11C36CE27463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B161E05-5535-4CB4-ABD1-9882683D02A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="8" activeTab="14" xr2:uid="{9D386D14-BB1A-49FB-A5CB-94A6FCCCA1F9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="8" activeTab="15" xr2:uid="{9D386D14-BB1A-49FB-A5CB-94A6FCCCA1F9}"/>
   </bookViews>
   <sheets>
     <sheet name="column" sheetId="17" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="232">
   <si>
     <t>key</t>
   </si>
@@ -231,9 +231,6 @@
     <t>filter area</t>
   </si>
   <si>
-    <t>reactor with agitator</t>
-  </si>
-  <si>
     <t>centrifugal, AVS</t>
   </si>
   <si>
@@ -387,12 +384,6 @@
     <t>https://www.alibaba.com/product-detail/Battery-Grade-Lioh-Lithium-Hydroxide-Lithium_62267896947.html?spm=a2700.galleryofferlist.normal_offer.d_title.b1a0469axvBcL2&amp;s=p</t>
   </si>
   <si>
-    <t>value low</t>
-  </si>
-  <si>
-    <t>value high</t>
-  </si>
-  <si>
     <t>https://www.alibaba.com/product-detail/Exporter-hot-sale-Hydrochloric-Acid-Factory_1600289913553.html?spm=a2700.galleryofferlist.normal_offer.d_title.3a8e2c51jUtwul&amp;s=p</t>
   </si>
   <si>
@@ -595,9 +586,6 @@
   </si>
   <si>
     <t>Li2CO3 refinement</t>
-  </si>
-  <si>
-    <t>vessle  with agitator</t>
   </si>
   <si>
     <t>pressure vessle with agitator</t>
@@ -674,9 +662,6 @@
     <t>plant_uptime</t>
   </si>
   <si>
-    <t>impure Li2CO3 in aqueous solution</t>
-  </si>
-  <si>
     <t>yield_forward</t>
   </si>
   <si>
@@ -722,46 +707,15 @@
     <t>l/g</t>
   </si>
   <si>
+    <t>Na2CO3</t>
+  </si>
+  <si>
     <t>CO2</t>
   </si>
   <si>
     <t>https://www.alibaba.com/product-detail/high-quality-Soda-Ash-Dense-Na2CO3_62240433604.html?spm=a2700.galleryofferlist.0.0.4987214e22kx0L&amp;s=p</t>
   </si>
   <si>
-    <r>
-      <t>Na</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CO</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3</t>
-    </r>
-  </si>
-  <si>
     <t>https://sefindustry.en.alibaba.com/product/60759731750-803350891/68L_Co2_Gas_Cylinder_Widely_Used_For_Medical_Industry.html?spm=a2700.shop_plgr.41413.12.6add2cd2Se7L8y</t>
   </si>
   <si>
@@ -784,13 +738,22 @@
   </si>
   <si>
     <t>quality_control</t>
+  </si>
+  <si>
+    <t>value_high</t>
+  </si>
+  <si>
+    <t>value_low</t>
+  </si>
+  <si>
+    <t>see above</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -833,21 +796,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <vertAlign val="subscript"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -870,13 +818,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -1206,7 +1153,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1225,7 +1172,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B3">
         <v>2.5</v>
@@ -1234,12 +1181,12 @@
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B4">
         <v>0.1</v>
@@ -1248,12 +1195,12 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B5">
         <v>0.9</v>
@@ -1261,43 +1208,43 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B7">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B8">
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -1320,7 +1267,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1334,23 +1281,23 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B4" s="1">
         <v>0.9</v>
@@ -1361,7 +1308,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B5" s="1">
         <v>0.8</v>
@@ -1372,32 +1319,32 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B6">
         <v>298.14999999999998</v>
       </c>
       <c r="C6" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D6" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B7">
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B8" s="1">
         <v>2</v>
@@ -1411,7 +1358,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B9">
         <v>353</v>
@@ -1422,18 +1369,18 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
@@ -1484,18 +1431,18 @@
         <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B15" s="1">
         <v>5000</v>
       </c>
       <c r="C15" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D15" t="s">
         <v>47</v>
@@ -1503,7 +1450,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B16">
         <v>0.8</v>
@@ -1511,13 +1458,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B17">
         <v>313.14999999999998</v>
       </c>
       <c r="D17" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -1631,7 +1578,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B1">
         <v>2016</v>
@@ -1648,12 +1595,12 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -1662,63 +1609,63 @@
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" t="s">
         <v>90</v>
-      </c>
-      <c r="D4" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" t="s">
         <v>94</v>
-      </c>
-      <c r="D6" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" t="s">
         <v>96</v>
-      </c>
-      <c r="D7" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" t="s">
         <v>98</v>
-      </c>
-      <c r="D8" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B10">
         <v>30</v>
@@ -1729,7 +1676,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B11">
         <v>0.2</v>
@@ -1740,13 +1687,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B12">
         <v>0.75</v>
       </c>
       <c r="D12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1757,10 +1704,10 @@
         <v>9.81</v>
       </c>
       <c r="C13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1798,37 +1745,37 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B3">
         <f xml:space="preserve"> 1.5 * 10^(-3)</f>
         <v>1.5E-3</v>
       </c>
       <c r="C3" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B4" s="1">
         <f>1*10^-3</f>
         <v>1E-3</v>
       </c>
       <c r="C4" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D4" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="H4" t="s">
         <v>47</v>
@@ -1836,14 +1783,14 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B5" s="1">
         <f>1.5*10^-3</f>
         <v>1.5E-3</v>
       </c>
       <c r="C5" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="H5" t="s">
         <v>47</v>
@@ -1860,7 +1807,7 @@
   <dimension ref="A2:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1874,44 +1821,44 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>230</v>
       </c>
       <c r="C2" t="s">
-        <v>116</v>
+        <v>229</v>
       </c>
       <c r="E2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F2" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B3">
         <v>6.6600000000000006E-2</v>
       </c>
       <c r="D3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B4">
         <v>0.01</v>
       </c>
       <c r="D4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1922,10 +1869,10 @@
         <v>20</v>
       </c>
       <c r="D5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1939,10 +1886,10 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="D6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1956,15 +1903,15 @@
         <v>0.45</v>
       </c>
       <c r="D7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="B8">
         <v>0.17</v>
@@ -1973,15 +1920,15 @@
         <v>0.24</v>
       </c>
       <c r="D8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B9">
         <f>30/45</f>
@@ -1992,13 +1939,13 @@
         <v>4.2222222222222223</v>
       </c>
       <c r="D9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E9" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -2018,7 +1965,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1330EF6F-438D-41F9-93CA-537B5AFAC263}">
   <dimension ref="A2:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -2035,7 +1982,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -2043,7 +1990,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="B3">
         <v>81890</v>
@@ -2052,42 +1999,42 @@
         <v>35</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B4" s="1">
         <v>45</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H4" t="s">
         <v>162</v>
-      </c>
-      <c r="H4" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="B6">
         <v>0.2</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>0.2</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B7">
         <v>0.2</v>
@@ -2106,8 +2053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0624EAC2-56E2-4337-8D5D-42EAA0559452}">
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2118,11 +2065,13 @@
     <col min="4" max="4" width="34.33203125" customWidth="1"/>
     <col min="5" max="5" width="7.44140625" customWidth="1"/>
     <col min="6" max="6" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -2130,13 +2079,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C2" t="s">
         <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E2" t="s">
         <v>34</v>
@@ -2154,23 +2103,23 @@
         <v>7</v>
       </c>
       <c r="K2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L2" t="s">
         <v>36</v>
       </c>
       <c r="M2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>179</v>
       </c>
       <c r="B4" t="s">
         <v>26</v>
@@ -2197,7 +2146,7 @@
         <v>54</v>
       </c>
       <c r="K4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L4">
         <v>0.53</v>
@@ -2229,7 +2178,7 @@
         <v>15</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L5">
         <v>0.6</v>
@@ -2243,7 +2192,7 @@
         <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="E6">
         <v>63000</v>
@@ -2264,7 +2213,7 @@
         <v>59</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L6">
         <v>0.81</v>
@@ -2272,15 +2221,15 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C8" t="s">
         <v>156</v>
-      </c>
-      <c r="C8" t="s">
-        <v>159</v>
       </c>
       <c r="E8">
         <v>380000</v>
@@ -2295,7 +2244,7 @@
         <v>12</v>
       </c>
       <c r="K8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L8">
         <v>0.66</v>
@@ -2303,7 +2252,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E9">
         <v>22000</v>
@@ -2312,7 +2261,7 @@
         <v>35</v>
       </c>
       <c r="G9" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="H9">
         <v>1600</v>
@@ -2324,7 +2273,7 @@
         <v>15</v>
       </c>
       <c r="K9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L9">
         <v>0.85</v>
@@ -2332,17 +2281,44 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>182</v>
+        <v>179</v>
+      </c>
+      <c r="E10">
+        <v>37500</v>
+      </c>
+      <c r="F10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10">
+        <v>3</v>
+      </c>
+      <c r="I10">
+        <v>7.4</v>
+      </c>
+      <c r="J10" t="s">
+        <v>54</v>
+      </c>
+      <c r="K10" t="s">
+        <v>70</v>
+      </c>
+      <c r="L10">
+        <v>0.53</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>179</v>
+      </c>
+      <c r="C12" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -2352,89 +2328,105 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>207</v>
+      <c r="A15" t="s">
+        <v>182</v>
+      </c>
+      <c r="C15" t="s">
+        <v>183</v>
+      </c>
+      <c r="D15" t="s">
+        <v>188</v>
+      </c>
+      <c r="E15">
+        <v>75000</v>
+      </c>
+      <c r="F15" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15" t="s">
+        <v>61</v>
+      </c>
+      <c r="H15">
+        <v>3</v>
+      </c>
+      <c r="I15">
+        <v>7.4</v>
+      </c>
+      <c r="J15" t="s">
+        <v>54</v>
+      </c>
+      <c r="K15" t="s">
+        <v>70</v>
+      </c>
+      <c r="L15">
+        <v>0.53</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>186</v>
-      </c>
-      <c r="C16" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="D16" t="s">
-        <v>192</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>174</v>
       </c>
+      <c r="B17" t="s">
+        <v>184</v>
+      </c>
       <c r="D17" t="s">
-        <v>175</v>
+        <v>173</v>
+      </c>
+      <c r="K17" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B18" t="s">
-        <v>188</v>
+        <v>185</v>
+      </c>
+      <c r="C18" t="s">
+        <v>189</v>
       </c>
       <c r="D18" t="s">
-        <v>176</v>
-      </c>
-      <c r="K18" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>178</v>
-      </c>
-      <c r="B19" t="s">
-        <v>189</v>
-      </c>
-      <c r="C19" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="D19" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>201</v>
+        <v>176</v>
       </c>
       <c r="D20" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>179</v>
-      </c>
-      <c r="D21" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" t="s">
         <v>64</v>
-      </c>
-      <c r="C25" t="s">
-        <v>65</v>
       </c>
       <c r="D25">
         <v>9500</v>
@@ -2455,7 +2447,7 @@
         <v>59</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K25">
         <v>0.79</v>
@@ -2463,13 +2455,13 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D26">
         <v>4800</v>
@@ -2478,7 +2470,7 @@
         <v>35</v>
       </c>
       <c r="F26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G26">
         <v>7.5</v>
@@ -2487,10 +2479,10 @@
         <v>2.54</v>
       </c>
       <c r="I26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K26">
         <v>0.65</v>
@@ -2498,16 +2490,16 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D27">
         <v>80</v>
       </c>
       <c r="E27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G27">
         <v>15</v>
@@ -2516,10 +2508,10 @@
         <v>20</v>
       </c>
       <c r="I27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K27">
         <v>1.33</v>
@@ -2533,13 +2525,13 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B28">
         <v>650</v>
       </c>
       <c r="C28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2570,7 +2562,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -2584,34 +2576,34 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B3">
         <v>1383.46</v>
       </c>
       <c r="C3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B4">
         <v>0.19400000000000001</v>
       </c>
       <c r="C4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B5">
         <v>69.17</v>
@@ -2622,35 +2614,35 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B6">
         <v>10</v>
       </c>
       <c r="C6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D6" t="s">
         <v>125</v>
-      </c>
-      <c r="D6" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B7">
         <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D7" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -2676,7 +2668,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -2689,18 +2681,18 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B3">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -2708,24 +2700,24 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B5">
         <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B6">
         <v>1.71</v>
       </c>
       <c r="C6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -2748,7 +2740,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -2772,24 +2764,24 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B4">
         <v>174</v>
       </c>
       <c r="C4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B5">
         <v>1.54</v>
       </c>
       <c r="C5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -2812,7 +2804,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -2831,41 +2823,41 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B3">
         <v>0.19400000000000001</v>
       </c>
       <c r="C3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B4">
         <v>1204.67</v>
       </c>
       <c r="C4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="D5" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -2888,7 +2880,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -2904,35 +2896,35 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B3">
         <v>35000</v>
       </c>
       <c r="C3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B4">
         <v>7920</v>
       </c>
       <c r="C4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B5">
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2955,7 +2947,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -3042,7 +3034,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B11">
         <v>0.9</v>
@@ -3070,7 +3062,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -3089,7 +3081,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D3" t="s">
         <v>53</v>
@@ -3176,7 +3168,7 @@
         <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -3200,7 +3192,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -3213,7 +3205,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B3">
         <v>0.7</v>
@@ -3232,7 +3224,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B5" s="1">
         <v>2</v>
@@ -3283,7 +3275,7 @@
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change to forwards slash for universl file paths, additions to LDH_opex and implementation of capex
</commit_message>
<xml_diff>
--- a/data/LDH_attributes.xlsx
+++ b/data/LDH_attributes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chant\PycharmProjects\FUSE-V2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B161E05-5535-4CB4-ABD1-9882683D02A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D5106C3-8343-4D4A-BCA4-282BD0ACC339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="8" activeTab="15" xr2:uid="{9D386D14-BB1A-49FB-A5CB-94A6FCCCA1F9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="9" activeTab="15" xr2:uid="{9D386D14-BB1A-49FB-A5CB-94A6FCCCA1F9}"/>
   </bookViews>
   <sheets>
     <sheet name="column" sheetId="17" r:id="rId1"/>
@@ -26,9 +26,11 @@
     <sheet name="standard_impeller" sheetId="4" r:id="rId11"/>
     <sheet name="pump" sheetId="10" r:id="rId12"/>
     <sheet name="water" sheetId="5" r:id="rId13"/>
-    <sheet name="costs" sheetId="11" r:id="rId14"/>
-    <sheet name="worker" sheetId="18" r:id="rId15"/>
-    <sheet name="equipment" sheetId="6" r:id="rId16"/>
+    <sheet name="cost_chemicals" sheetId="11" r:id="rId14"/>
+    <sheet name="opex" sheetId="22" r:id="rId15"/>
+    <sheet name="worker" sheetId="18" r:id="rId16"/>
+    <sheet name="equipment" sheetId="6" r:id="rId17"/>
+    <sheet name="capex" sheetId="21" r:id="rId18"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="244">
   <si>
     <t>key</t>
   </si>
@@ -114,18 +116,6 @@
     <t>g</t>
   </si>
   <si>
-    <t>filter</t>
-  </si>
-  <si>
-    <t>grinder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stainless steel batch reactor </t>
-  </si>
-  <si>
-    <t>batch vacuum filter (leaf)</t>
-  </si>
-  <si>
     <t>Piccinno 2016, From laboratory scale to industrial scale: a scale-up framework for chemical processes in LCA studies</t>
   </si>
   <si>
@@ -138,12 +128,6 @@
     <t>95 degree C</t>
   </si>
   <si>
-    <t>Hammer mill</t>
-  </si>
-  <si>
-    <t xml:space="preserve">comment </t>
-  </si>
-  <si>
     <t>FOB</t>
   </si>
   <si>
@@ -222,33 +206,18 @@
     <t>kW</t>
   </si>
   <si>
-    <t>open tank</t>
-  </si>
-  <si>
     <t>working volume</t>
   </si>
   <si>
     <t>filter area</t>
   </si>
   <si>
-    <t>centrifugal, AVS</t>
-  </si>
-  <si>
-    <t>motor included, range 23-250</t>
-  </si>
-  <si>
-    <t>control valve</t>
-  </si>
-  <si>
     <t>diameter</t>
   </si>
   <si>
     <t>cm</t>
   </si>
   <si>
-    <t>excluding valve positioner, range 7.5 - 23</t>
-  </si>
-  <si>
     <t>washing before filtration</t>
   </si>
   <si>
@@ -285,15 +254,6 @@
     <t>https://www.alibaba.com/product-detail/Astm-a-53-carbon-schedule-40_60744718165.html?spm=a2700.7724857.normal_offer.d_title.384e4537n4GLw8</t>
   </si>
   <si>
-    <t>pump</t>
-  </si>
-  <si>
-    <t>valve</t>
-  </si>
-  <si>
-    <t>pipe</t>
-  </si>
-  <si>
     <t>amount</t>
   </si>
   <si>
@@ -396,9 +356,6 @@
     <t>CEPCI base</t>
   </si>
   <si>
-    <t>machine</t>
-  </si>
-  <si>
     <t>yield</t>
   </si>
   <si>
@@ -501,18 +458,9 @@
     <t>stripping_flow_rate</t>
   </si>
   <si>
-    <t>Extraction column</t>
-  </si>
-  <si>
-    <t>FO unit</t>
-  </si>
-  <si>
     <t>area</t>
   </si>
   <si>
-    <t>Membrane lifetime 500 h</t>
-  </si>
-  <si>
     <t>lab scale</t>
   </si>
   <si>
@@ -555,83 +503,9 @@
     <t>precipitation_pressure</t>
   </si>
   <si>
-    <t>Filter</t>
-  </si>
-  <si>
-    <t>removal of insoluble compounds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">removal of divalent and trivalent cations </t>
-  </si>
-  <si>
-    <t>ion exchange device</t>
-  </si>
-  <si>
-    <t>heating vessle for precipitation</t>
-  </si>
-  <si>
-    <t>drying apparatus</t>
-  </si>
-  <si>
     <t>https://www.purolite.com/product/s940</t>
   </si>
   <si>
-    <t>Column extraction and Forward Osmosis</t>
-  </si>
-  <si>
-    <t>vessle with agitator</t>
-  </si>
-  <si>
-    <t>Li2CO3 processing</t>
-  </si>
-  <si>
-    <t>Li2CO3 refinement</t>
-  </si>
-  <si>
-    <t>pressure vessle with agitator</t>
-  </si>
-  <si>
-    <t>with gas inlet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Purolite S940 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">precipitation </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">output size 150 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>μm (Paranthaman 2017)</t>
-    </r>
-  </si>
-  <si>
-    <t>reaction step</t>
-  </si>
-  <si>
-    <t>carbonatino ofaq Li2CO3</t>
-  </si>
-  <si>
-    <t>temp 60 - 95°C, 1 atm,</t>
-  </si>
-  <si>
-    <t>release of CO2 (possibility of recycling)</t>
-  </si>
-  <si>
-    <t>pure Li2CO3 recovery</t>
-  </si>
-  <si>
-    <t>drying of pure Li2CO3 filtration cake</t>
-  </si>
-  <si>
     <t xml:space="preserve">comments </t>
   </si>
   <si>
@@ -644,9 +518,6 @@
     <t>reaction_time</t>
   </si>
   <si>
-    <t>Filtration and centrifugation</t>
-  </si>
-  <si>
     <t>CO2_excess</t>
   </si>
   <si>
@@ -734,9 +605,6 @@
     <t>supervision</t>
   </si>
   <si>
-    <t>Cost factors in % of operating labout</t>
-  </si>
-  <si>
     <t>quality_control</t>
   </si>
   <si>
@@ -746,14 +614,173 @@
     <t>value_low</t>
   </si>
   <si>
-    <t>see above</t>
+    <t>resin volume</t>
+  </si>
+  <si>
+    <t>drying surface</t>
+  </si>
+  <si>
+    <t>https://www.alibaba.com/product-detail/Water-Treatment-Ion-Exchange-Resin-System_60196715429.html?spm=a2700.galleryofferlist.normal_offer.d_title.5d1cd423dNfMUX&amp;s=p</t>
+  </si>
+  <si>
+    <t>https://www.alibaba.com/product-detail/Distiller-s-Byproducts-Rotary-Dryer-DDGS_60163079081.html?spm=a2700.galleryofferlist.normal_offer.d_title.74477a8aDtXY0t&amp;s=p</t>
+  </si>
+  <si>
+    <t>taken from 1l volume (sharma 2020) and assumed to be the same for the 1000 l reaction vessle</t>
+  </si>
+  <si>
+    <t>Extraction_column</t>
+  </si>
+  <si>
+    <t>FO_unit</t>
+  </si>
+  <si>
+    <t>Reactor_1</t>
+  </si>
+  <si>
+    <t>Filter_1</t>
+  </si>
+  <si>
+    <t>Grinder</t>
+  </si>
+  <si>
+    <t>Reactor_2</t>
+  </si>
+  <si>
+    <t>Filter_2</t>
+  </si>
+  <si>
+    <t>Reactor_3</t>
+  </si>
+  <si>
+    <t>Ion_exchange_column</t>
+  </si>
+  <si>
+    <t>Ion_exchange_resin</t>
+  </si>
+  <si>
+    <t>Pumps</t>
+  </si>
+  <si>
+    <t>Valves</t>
+  </si>
+  <si>
+    <t>Pipes</t>
+  </si>
+  <si>
+    <t>Belt_Conveyor</t>
+  </si>
+  <si>
+    <t>Dryer</t>
+  </si>
+  <si>
+    <t>Installation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equipment </t>
+  </si>
+  <si>
+    <t>Instrumentation_and_control</t>
+  </si>
+  <si>
+    <t>Electric_equipment_and_materials</t>
+  </si>
+  <si>
+    <t>Buildings</t>
+  </si>
+  <si>
+    <t>Service_Facilities</t>
+  </si>
+  <si>
+    <t>Land</t>
+  </si>
+  <si>
+    <t>Facility_site_improvement</t>
+  </si>
+  <si>
+    <t>FCC_contingency</t>
+  </si>
+  <si>
+    <t>Depriciable + Non_Depreciable</t>
+  </si>
+  <si>
+    <t>Working_capital</t>
+  </si>
+  <si>
+    <t>FCC</t>
+  </si>
+  <si>
+    <t>Property_taxes</t>
+  </si>
+  <si>
+    <t>Insurance</t>
+  </si>
+  <si>
+    <t>Fringe_benefits</t>
+  </si>
+  <si>
+    <t>Operating labour and supervision</t>
+  </si>
+  <si>
+    <t>Direct and Indirect</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>Financing</t>
+  </si>
+  <si>
+    <t>TCI</t>
+  </si>
+  <si>
+    <t>R&amp;D</t>
+  </si>
+  <si>
+    <t>factor</t>
+  </si>
+  <si>
+    <t>cost</t>
+  </si>
+  <si>
+    <t>maintenance_labour</t>
+  </si>
+  <si>
+    <t>maintenance_material</t>
+  </si>
+  <si>
+    <t>operating_supplies</t>
+  </si>
+  <si>
+    <t>materials</t>
+  </si>
+  <si>
+    <t>remaining direct costs</t>
+  </si>
+  <si>
+    <t>contingency_1</t>
+  </si>
+  <si>
+    <t>contingency_2</t>
+  </si>
+  <si>
+    <t>operating labour</t>
+  </si>
+  <si>
+    <t>Overhead</t>
+  </si>
+  <si>
+    <t>Administrative</t>
+  </si>
+  <si>
+    <t>Cost factors of operating labort</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -767,12 +794,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -816,14 +837,14 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -1153,7 +1174,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1172,7 +1193,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="B3">
         <v>2.5</v>
@@ -1181,12 +1202,12 @@
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B4">
         <v>0.1</v>
@@ -1195,12 +1216,12 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="B5">
         <v>0.9</v>
@@ -1208,43 +1229,43 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>201</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="B7">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="D7" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="B8">
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -1267,7 +1288,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1281,70 +1302,70 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>193</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>198</v>
+        <v>158</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>194</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>203</v>
+        <v>163</v>
       </c>
       <c r="B4" s="1">
         <v>0.9</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>204</v>
+        <v>164</v>
       </c>
       <c r="B5" s="1">
         <v>0.8</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
       <c r="B6">
         <v>298.14999999999998</v>
       </c>
       <c r="C6" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
       <c r="D6" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
       <c r="B7">
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>199</v>
+        <v>159</v>
       </c>
       <c r="B8" s="1">
         <v>2</v>
@@ -1353,12 +1374,12 @@
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="B9">
         <v>353</v>
@@ -1369,18 +1390,18 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
@@ -1389,7 +1410,7 @@
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1408,7 +1429,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B13">
         <v>6.3499999999999997E-3</v>
@@ -1417,12 +1438,12 @@
         <v>15</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B14">
         <v>3.7160000000000002</v>
@@ -1431,26 +1452,26 @@
         <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>207</v>
+        <v>167</v>
       </c>
       <c r="B15" s="1">
         <v>5000</v>
       </c>
       <c r="C15" t="s">
-        <v>206</v>
+        <v>166</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>205</v>
+        <v>165</v>
       </c>
       <c r="B16">
         <v>0.8</v>
@@ -1458,13 +1479,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>208</v>
+        <v>168</v>
       </c>
       <c r="B17">
         <v>313.14999999999998</v>
       </c>
       <c r="D17" t="s">
-        <v>209</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -1488,7 +1509,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1513,7 +1534,7 @@
         <v>0.75</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1552,7 +1573,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B7">
         <v>0.9</v>
@@ -1578,7 +1599,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="B1">
         <v>2016</v>
@@ -1595,12 +1616,12 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -1609,63 +1630,63 @@
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="D4" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="D5" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="D6" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="D7" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="D8" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="B10">
         <v>30</v>
@@ -1676,7 +1697,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="B11">
         <v>0.2</v>
@@ -1687,13 +1708,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="B12">
         <v>0.75</v>
       </c>
       <c r="D12" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1704,10 +1725,10 @@
         <v>9.81</v>
       </c>
       <c r="C13" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="D13" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1745,55 +1766,55 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>210</v>
+        <v>170</v>
       </c>
       <c r="B3">
         <f xml:space="preserve"> 1.5 * 10^(-3)</f>
         <v>1.5E-3</v>
       </c>
       <c r="C3" t="s">
-        <v>217</v>
+        <v>177</v>
       </c>
       <c r="D3" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>216</v>
+        <v>176</v>
       </c>
       <c r="B4" s="1">
         <f>1*10^-3</f>
         <v>1E-3</v>
       </c>
       <c r="C4" t="s">
-        <v>217</v>
+        <v>177</v>
       </c>
       <c r="D4" t="s">
-        <v>215</v>
+        <v>175</v>
       </c>
       <c r="H4" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>214</v>
+        <v>174</v>
       </c>
       <c r="B5" s="1">
         <f>1.5*10^-3</f>
         <v>1.5E-3</v>
       </c>
       <c r="C5" t="s">
-        <v>217</v>
+        <v>177</v>
       </c>
       <c r="H5" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1804,15 +1825,15 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F37A8F43-ECBD-4243-988B-AAA9A59B3D22}">
-  <dimension ref="A2:F9"/>
+  <dimension ref="A2:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
     <col min="5" max="5" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1821,63 +1842,63 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>230</v>
+        <v>189</v>
       </c>
       <c r="C2" t="s">
-        <v>229</v>
+        <v>188</v>
       </c>
       <c r="E2" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="F2" t="s">
-        <v>224</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="B3">
         <v>6.6600000000000006E-2</v>
       </c>
       <c r="D3" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="F3" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="B4">
         <v>0.01</v>
       </c>
       <c r="D4" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="F4" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B5">
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B6">
         <v>0.51</v>
@@ -1886,15 +1907,15 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="D6" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>223</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B7">
         <v>0.15</v>
@@ -1903,15 +1924,15 @@
         <v>0.45</v>
       </c>
       <c r="D7" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>218</v>
+        <v>178</v>
       </c>
       <c r="B8">
         <v>0.17</v>
@@ -1920,15 +1941,15 @@
         <v>0.24</v>
       </c>
       <c r="D8" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>220</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>219</v>
+        <v>179</v>
       </c>
       <c r="B9">
         <f>30/45</f>
@@ -1939,14 +1960,23 @@
         <v>4.2222222222222223</v>
       </c>
       <c r="D9" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="E9" t="s">
-        <v>222</v>
+        <v>182</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>221</v>
-      </c>
+        <v>181</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1962,16 +1992,183 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1330EF6F-438D-41F9-93CA-537B5AFAC263}">
-  <dimension ref="A2:H7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24498815-2749-43E0-8B7E-EA1E475CA5F2}">
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="B3">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>235</v>
+      </c>
+      <c r="B4">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="B5">
+        <v>0.1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>239</v>
+      </c>
+      <c r="B6">
+        <v>0.25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>222</v>
+      </c>
+      <c r="B7">
+        <v>0.02</v>
+      </c>
+      <c r="C7" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>223</v>
+      </c>
+      <c r="B8">
+        <v>0.02</v>
+      </c>
+      <c r="C8" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>224</v>
+      </c>
+      <c r="B9">
+        <v>0.22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>241</v>
+      </c>
+      <c r="B10">
+        <v>0.5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>242</v>
+      </c>
+      <c r="B11">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>227</v>
+      </c>
+      <c r="B12">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="C12" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>228</v>
+      </c>
+      <c r="B13">
+        <v>0.08</v>
+      </c>
+      <c r="C13" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>230</v>
+      </c>
+      <c r="B14">
+        <v>5.7500000000000002E-2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>226</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1330EF6F-438D-41F9-93CA-537B5AFAC263}">
+  <dimension ref="A2:H8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -1982,7 +2179,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -1990,54 +2187,68 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>225</v>
+        <v>185</v>
       </c>
       <c r="B3">
         <v>81890</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
       <c r="B4" s="1">
         <v>45</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
       <c r="H4" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>227</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>226</v>
+        <v>186</v>
       </c>
       <c r="B6">
         <v>0.2</v>
       </c>
-      <c r="D6" s="5">
-        <v>0.2</v>
+      <c r="D6" s="5" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>228</v>
+        <v>187</v>
       </c>
       <c r="B7">
         <v>0.2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>233</v>
+      </c>
+      <c r="B8">
+        <v>2.7E-2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -2049,501 +2260,642 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0624EAC2-56E2-4337-8D5D-42EAA0559452}">
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.44140625" customWidth="1"/>
-    <col min="2" max="2" width="29.33203125" customWidth="1"/>
-    <col min="3" max="3" width="33.6640625" customWidth="1"/>
-    <col min="4" max="4" width="34.33203125" customWidth="1"/>
-    <col min="5" max="5" width="7.44140625" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" customWidth="1"/>
+    <col min="4" max="4" width="19.109375" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
     <col min="11" max="11" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>187</v>
+        <v>49</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>51</v>
+      </c>
+      <c r="F2" t="s">
+        <v>50</v>
       </c>
       <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B3">
+        <v>37500</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>0.5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" t="s">
+        <v>61</v>
+      </c>
+      <c r="I3">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>198</v>
+      </c>
+      <c r="B4">
+        <v>230000</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
         <v>55</v>
       </c>
-      <c r="H2" t="s">
+      <c r="E4">
+        <v>150</v>
+      </c>
+      <c r="F4">
+        <v>20</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>199</v>
+      </c>
+      <c r="B5">
+        <v>63000</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5">
+        <v>15</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I5">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>195</v>
+      </c>
+      <c r="B6">
+        <v>380000</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>12</v>
+      </c>
+      <c r="H6" t="s">
+        <v>59</v>
+      </c>
+      <c r="I6">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>196</v>
+      </c>
+      <c r="B7">
+        <v>22000</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>138</v>
+      </c>
+      <c r="E7">
+        <v>1600</v>
+      </c>
+      <c r="F7">
+        <v>3593</v>
+      </c>
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" t="s">
+        <v>59</v>
+      </c>
+      <c r="I7">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>200</v>
+      </c>
+      <c r="B8">
+        <v>37500</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+      <c r="G8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I8">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>201</v>
+      </c>
+      <c r="B9">
+        <v>230000</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9">
+        <v>150</v>
+      </c>
+      <c r="F9">
+        <v>100</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I9">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>202</v>
+      </c>
+      <c r="B10">
+        <v>75000</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="G10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" t="s">
+        <v>59</v>
+      </c>
+      <c r="I10">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>203</v>
+      </c>
+      <c r="B11">
+        <v>100000</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
+        <v>190</v>
+      </c>
+      <c r="E11">
+        <v>30</v>
+      </c>
+      <c r="F11">
+        <v>10</v>
+      </c>
+      <c r="G11" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" t="s">
+        <v>192</v>
+      </c>
+      <c r="I11">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>204</v>
+      </c>
+      <c r="B12">
+        <v>32.5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" t="s">
+        <v>190</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>10</v>
+      </c>
+      <c r="G12" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I12">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>209</v>
+      </c>
+      <c r="B13">
+        <v>238000</v>
+      </c>
+      <c r="C13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" t="s">
+        <v>191</v>
+      </c>
+      <c r="E13">
+        <v>10</v>
+      </c>
+      <c r="F13">
+        <v>60</v>
+      </c>
+      <c r="G13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" t="s">
+        <v>193</v>
+      </c>
+      <c r="I13">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B14">
+        <v>9500</v>
+      </c>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14">
+        <v>23</v>
+      </c>
+      <c r="F14">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G14" t="s">
+        <v>53</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="I14">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B15">
+        <v>4800</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15">
+        <v>7.5</v>
+      </c>
+      <c r="F15">
+        <v>2.54</v>
+      </c>
+      <c r="G15" t="s">
         <v>57</v>
       </c>
-      <c r="I2" t="s">
+      <c r="H15" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I15">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>207</v>
+      </c>
+      <c r="B16">
+        <v>80</v>
+      </c>
+      <c r="C16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" t="s">
         <v>56</v>
       </c>
-      <c r="J2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" t="s">
-        <v>71</v>
-      </c>
-      <c r="L2" t="s">
-        <v>36</v>
-      </c>
-      <c r="M2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>179</v>
-      </c>
-      <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E4">
-        <v>37500</v>
-      </c>
-      <c r="F4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" t="s">
-        <v>61</v>
-      </c>
-      <c r="H4">
-        <v>3</v>
-      </c>
-      <c r="I4">
-        <v>0.5</v>
-      </c>
-      <c r="J4" t="s">
-        <v>54</v>
-      </c>
-      <c r="K4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L4">
-        <v>0.53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5">
-        <v>230000</v>
-      </c>
-      <c r="F5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" t="s">
-        <v>62</v>
-      </c>
-      <c r="H5">
-        <v>150</v>
-      </c>
-      <c r="I5">
+      <c r="E16">
+        <v>15</v>
+      </c>
+      <c r="F16">
         <v>20</v>
       </c>
-      <c r="J5" t="s">
-        <v>15</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="L5">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" t="s">
-        <v>186</v>
-      </c>
-      <c r="E6">
-        <v>63000</v>
-      </c>
-      <c r="F6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" t="s">
-        <v>58</v>
-      </c>
-      <c r="H6">
-        <v>15</v>
-      </c>
-      <c r="I6">
-        <v>4</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="G16" t="s">
+        <v>57</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I16">
+        <v>1.33</v>
+      </c>
+      <c r="J16">
+        <v>100</v>
+      </c>
+      <c r="K16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>208</v>
+      </c>
+      <c r="B17">
+        <v>21000</v>
+      </c>
+      <c r="C17" t="s">
+        <v>29</v>
+      </c>
+      <c r="I17">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>103</v>
+      </c>
+      <c r="B19">
+        <v>650</v>
+      </c>
+      <c r="C19" t="s">
         <v>59</v>
       </c>
-      <c r="K6" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="L6">
-        <v>0.81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>153</v>
-      </c>
-      <c r="C8" t="s">
-        <v>156</v>
-      </c>
-      <c r="E8">
-        <v>380000</v>
-      </c>
-      <c r="F8" t="s">
-        <v>35</v>
-      </c>
-      <c r="H8">
-        <v>10</v>
-      </c>
-      <c r="I8">
-        <v>12</v>
-      </c>
-      <c r="K8" t="s">
-        <v>70</v>
-      </c>
-      <c r="L8">
-        <v>0.66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>154</v>
-      </c>
-      <c r="E9">
-        <v>22000</v>
-      </c>
-      <c r="F9" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" t="s">
-        <v>155</v>
-      </c>
-      <c r="H9">
-        <v>1600</v>
-      </c>
-      <c r="I9">
-        <v>3593</v>
-      </c>
-      <c r="J9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K9" t="s">
-        <v>70</v>
-      </c>
-      <c r="L9">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>179</v>
-      </c>
-      <c r="E10">
-        <v>37500</v>
-      </c>
-      <c r="F10" t="s">
-        <v>35</v>
-      </c>
-      <c r="G10" t="s">
-        <v>61</v>
-      </c>
-      <c r="H10">
-        <v>3</v>
-      </c>
-      <c r="I10">
-        <v>7.4</v>
-      </c>
-      <c r="J10" t="s">
-        <v>54</v>
-      </c>
-      <c r="K10" t="s">
-        <v>70</v>
-      </c>
-      <c r="L10">
-        <v>0.53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>179</v>
-      </c>
-      <c r="C12" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>182</v>
-      </c>
-      <c r="C15" t="s">
-        <v>183</v>
-      </c>
-      <c r="D15" t="s">
-        <v>188</v>
-      </c>
-      <c r="E15">
-        <v>75000</v>
-      </c>
-      <c r="F15" t="s">
-        <v>35</v>
-      </c>
-      <c r="G15" t="s">
-        <v>61</v>
-      </c>
-      <c r="H15">
-        <v>3</v>
-      </c>
-      <c r="I15">
-        <v>7.4</v>
-      </c>
-      <c r="J15" t="s">
-        <v>54</v>
-      </c>
-      <c r="K15" t="s">
-        <v>70</v>
-      </c>
-      <c r="L15">
-        <v>0.53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>171</v>
-      </c>
-      <c r="D16" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>174</v>
-      </c>
-      <c r="B17" t="s">
-        <v>184</v>
-      </c>
-      <c r="D17" t="s">
-        <v>173</v>
-      </c>
-      <c r="K17" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>175</v>
-      </c>
-      <c r="B18" t="s">
-        <v>185</v>
-      </c>
-      <c r="C18" t="s">
-        <v>189</v>
-      </c>
-      <c r="D18" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>197</v>
-      </c>
-      <c r="D19" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>176</v>
-      </c>
-      <c r="D20" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B25" t="s">
-        <v>63</v>
-      </c>
-      <c r="C25" t="s">
-        <v>64</v>
-      </c>
-      <c r="D25">
-        <v>9500</v>
-      </c>
-      <c r="E25" t="s">
-        <v>35</v>
-      </c>
-      <c r="F25" t="s">
-        <v>58</v>
-      </c>
-      <c r="G25">
-        <v>23</v>
-      </c>
-      <c r="H25">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="I25" t="s">
-        <v>59</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="K25">
-        <v>0.79</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B26" t="s">
-        <v>65</v>
-      </c>
-      <c r="C26" t="s">
-        <v>68</v>
-      </c>
-      <c r="D26">
-        <v>4800</v>
-      </c>
-      <c r="E26" t="s">
-        <v>35</v>
-      </c>
-      <c r="F26" t="s">
-        <v>66</v>
-      </c>
-      <c r="G26">
-        <v>7.5</v>
-      </c>
-      <c r="H26">
-        <v>2.54</v>
-      </c>
-      <c r="I26" t="s">
-        <v>67</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="K26">
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>83</v>
-      </c>
-      <c r="D27">
-        <v>80</v>
-      </c>
-      <c r="E27" t="s">
-        <v>77</v>
-      </c>
-      <c r="F27" t="s">
-        <v>66</v>
-      </c>
-      <c r="G27">
-        <v>15</v>
-      </c>
-      <c r="H27">
-        <v>20</v>
-      </c>
-      <c r="I27" t="s">
-        <v>67</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="K27">
-        <v>1.33</v>
-      </c>
-      <c r="L27">
-        <v>100</v>
-      </c>
-      <c r="M27" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>117</v>
-      </c>
-      <c r="B28">
-        <v>650</v>
-      </c>
-      <c r="C28" t="s">
-        <v>70</v>
-      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K6" r:id="rId1" xr:uid="{29B1090E-3E0E-4959-9517-01ECBE15B1E6}"/>
-    <hyperlink ref="K5" r:id="rId2" xr:uid="{699EF7F5-147A-4A45-9703-96F569E8802F}"/>
-    <hyperlink ref="J27" r:id="rId3" xr:uid="{CE857C8C-06BA-4606-B21B-E83F455C3B82}"/>
-    <hyperlink ref="J26" r:id="rId4" xr:uid="{292D848F-3DC3-42FF-B115-46148EDFD2A8}"/>
-    <hyperlink ref="J25" r:id="rId5" xr:uid="{7FC25CF3-66CB-4D0A-BB61-3B4475B2C819}"/>
+    <hyperlink ref="H5" r:id="rId1" xr:uid="{29B1090E-3E0E-4959-9517-01ECBE15B1E6}"/>
+    <hyperlink ref="H4" r:id="rId2" xr:uid="{699EF7F5-147A-4A45-9703-96F569E8802F}"/>
+    <hyperlink ref="H16" r:id="rId3" xr:uid="{CE857C8C-06BA-4606-B21B-E83F455C3B82}"/>
+    <hyperlink ref="H15" r:id="rId4" xr:uid="{292D848F-3DC3-42FF-B115-46148EDFD2A8}"/>
+    <hyperlink ref="H14" r:id="rId5" xr:uid="{7FC25CF3-66CB-4D0A-BB61-3B4475B2C819}"/>
+    <hyperlink ref="H9" r:id="rId6" xr:uid="{A5DFE124-6B6E-4D52-B2A1-E246DBD7A1E9}"/>
+    <hyperlink ref="H12" r:id="rId7" xr:uid="{5BA3537D-6CBE-495C-BAE1-48869200A390}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{285D6F2E-FA24-4D6E-BA33-9B8C5FFBA286}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B3">
+        <v>0.7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>212</v>
+      </c>
+      <c r="B4">
+        <v>0.18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>213</v>
+      </c>
+      <c r="B5">
+        <v>0.1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>214</v>
+      </c>
+      <c r="B6">
+        <v>0.38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>215</v>
+      </c>
+      <c r="B7">
+        <v>0.4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>216</v>
+      </c>
+      <c r="B8">
+        <v>0.06</v>
+      </c>
+      <c r="C8" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>217</v>
+      </c>
+      <c r="B9">
+        <v>0.1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>218</v>
+      </c>
+      <c r="B10">
+        <v>0.25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>220</v>
+      </c>
+      <c r="B11">
+        <v>0.2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>221</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -2562,7 +2914,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -2576,34 +2928,34 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="B3">
         <v>1383.46</v>
       </c>
       <c r="C3" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="B4">
         <v>0.19400000000000001</v>
       </c>
       <c r="C4" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="B5">
         <v>69.17</v>
@@ -2614,35 +2966,35 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="B6">
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="D6" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="B7">
         <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="D7" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -2658,7 +3010,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2668,7 +3020,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -2681,18 +3033,18 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="B3">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -2700,24 +3052,24 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="B5">
         <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="B6">
         <v>1.71</v>
       </c>
       <c r="C6" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -2740,7 +3092,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -2756,7 +3108,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B3">
         <v>0.9</v>
@@ -2764,24 +3116,24 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="B4">
         <v>174</v>
       </c>
       <c r="C4" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="B5">
         <v>1.54</v>
       </c>
       <c r="C5" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -2804,7 +3156,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -2823,41 +3175,41 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="B3">
         <v>0.19400000000000001</v>
       </c>
       <c r="C3" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="D3" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="B4">
         <v>1204.67</v>
       </c>
       <c r="C4" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>211</v>
+        <v>171</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>212</v>
+        <v>172</v>
       </c>
       <c r="D5" t="s">
-        <v>213</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -2880,7 +3232,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -2896,35 +3248,35 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="B3">
         <v>35000</v>
       </c>
       <c r="C3" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>202</v>
+        <v>162</v>
       </c>
       <c r="B4">
         <v>7920</v>
       </c>
       <c r="C4" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="B5">
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -2947,7 +3299,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -2966,7 +3318,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2974,18 +3326,18 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B5">
         <v>0.7</v>
@@ -2996,7 +3348,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3004,7 +3356,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3012,7 +3364,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3020,21 +3372,21 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B10" s="1">
         <v>50</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="B11">
         <v>0.9</v>
@@ -3051,7 +3403,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3062,7 +3414,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -3081,10 +3433,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -3098,7 +3450,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -3117,7 +3469,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -3145,7 +3497,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B8">
         <v>6.3499999999999997E-3</v>
@@ -3154,12 +3506,12 @@
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B9">
         <v>3.7160000000000002</v>
@@ -3168,7 +3520,7 @@
         <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -3182,7 +3534,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3192,7 +3544,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>195</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -3205,7 +3557,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="B3">
         <v>0.7</v>
@@ -3224,7 +3576,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>196</v>
+        <v>157</v>
       </c>
       <c r="B5" s="1">
         <v>2</v>
@@ -3233,7 +3585,7 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -3252,7 +3604,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B7">
         <v>6.3499999999999997E-3</v>
@@ -3261,12 +3613,12 @@
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B8">
         <v>3.7160000000000002</v>
@@ -3275,7 +3627,7 @@
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implementation of energy plot and rearrangement of LDH_attributes spreadsheet
</commit_message>
<xml_diff>
--- a/data/LDH_attributes.xlsx
+++ b/data/LDH_attributes.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chant\PycharmProjects\FUSE-V2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D5106C3-8343-4D4A-BCA4-282BD0ACC339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE760C4-F832-4B26-84FB-93A653C477B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="9" activeTab="15" xr2:uid="{9D386D14-BB1A-49FB-A5CB-94A6FCCCA1F9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="9" activeTab="10" xr2:uid="{9D386D14-BB1A-49FB-A5CB-94A6FCCCA1F9}"/>
   </bookViews>
   <sheets>
-    <sheet name="column" sheetId="17" r:id="rId1"/>
-    <sheet name="washing" sheetId="12" r:id="rId2"/>
-    <sheet name="stripping" sheetId="13" r:id="rId3"/>
-    <sheet name="FO" sheetId="16" r:id="rId4"/>
-    <sheet name="brine" sheetId="14" r:id="rId5"/>
-    <sheet name="plant" sheetId="15" r:id="rId6"/>
-    <sheet name="chemicals_sorbent_synthesis" sheetId="2" r:id="rId7"/>
-    <sheet name="sorbent_synthesis_reaction" sheetId="3" r:id="rId8"/>
+    <sheet name="chemicals_sorbent_synthesis" sheetId="2" r:id="rId1"/>
+    <sheet name="sorbent_synthesis_reaction" sheetId="3" r:id="rId2"/>
+    <sheet name="plant" sheetId="15" r:id="rId3"/>
+    <sheet name="brine" sheetId="14" r:id="rId4"/>
+    <sheet name="column" sheetId="17" r:id="rId5"/>
+    <sheet name="washing" sheetId="12" r:id="rId6"/>
+    <sheet name="stripping" sheetId="13" r:id="rId7"/>
+    <sheet name="FO" sheetId="16" r:id="rId8"/>
     <sheet name="Li2CO3_processing" sheetId="19" r:id="rId9"/>
     <sheet name="Li2CO3_purification" sheetId="20" r:id="rId10"/>
     <sheet name="standard_impeller" sheetId="4" r:id="rId11"/>
@@ -1160,21 +1160,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5B35FB0-FC35-4894-B852-40A6833023F4}">
-  <dimension ref="A1:D9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAA36DB8-B0B9-4A0A-8A56-527230CA91FC}">
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.21875" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>131</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1193,83 +1193,83 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>44</v>
       </c>
       <c r="B3">
-        <v>2.5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>139</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="B4">
-        <v>0.1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>139</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>132</v>
+        <v>37</v>
       </c>
       <c r="B5">
-        <v>0.9</v>
+        <v>0.7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>161</v>
+        <v>38</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>135</v>
+        <v>39</v>
       </c>
       <c r="B7">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>133</v>
-      </c>
-      <c r="D7" t="s">
-        <v>134</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>136</v>
+        <v>40</v>
       </c>
       <c r="B8">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>137</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-      <c r="C9" t="s">
-        <v>133</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="1">
+        <v>50</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B11">
+        <v>0.9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1498,7 +1498,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A0F109E-90BE-42A5-8DFF-EE3A7F8215F0}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -2162,7 +2162,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1330EF6F-438D-41F9-93CA-537B5AFAC263}">
   <dimension ref="A2:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -2900,505 +2900,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{057E51FA-16AA-4EDB-95D7-E76738AA23C5}">
-  <dimension ref="A1:D8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16.5546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B3">
-        <v>1383.46</v>
-      </c>
-      <c r="C3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>125</v>
-      </c>
-      <c r="B4">
-        <v>0.19400000000000001</v>
-      </c>
-      <c r="C4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B5">
-        <v>69.17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>109</v>
-      </c>
-      <c r="B6">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>111</v>
-      </c>
-      <c r="B7">
-        <v>50</v>
-      </c>
-      <c r="C7" t="s">
-        <v>112</v>
-      </c>
-      <c r="D7" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>114</v>
-      </c>
-      <c r="B8">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4E9EB40-91BA-4B28-833D-B3DB1EE1EE78}">
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>115</v>
-      </c>
-      <c r="B3">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>116</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>126</v>
-      </c>
-      <c r="B5">
-        <v>40</v>
-      </c>
-      <c r="C5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>127</v>
-      </c>
-      <c r="B6">
-        <v>1.71</v>
-      </c>
-      <c r="C6" t="s">
-        <v>107</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{285FC4B4-1D25-4960-A894-56724304077E}">
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16.5546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B4">
-        <v>174</v>
-      </c>
-      <c r="C4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>127</v>
-      </c>
-      <c r="B5">
-        <v>1.54</v>
-      </c>
-      <c r="C5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C77679F-E498-462D-825B-EAF86D6734F3}">
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="23.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>125</v>
-      </c>
-      <c r="B3">
-        <v>0.19400000000000001</v>
-      </c>
-      <c r="C3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>119</v>
-      </c>
-      <c r="B4">
-        <v>1204.67</v>
-      </c>
-      <c r="C4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>171</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>172</v>
-      </c>
-      <c r="D5" t="s">
-        <v>173</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9896EE1E-7F56-45CB-B0FF-A4EB36B766F1}">
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>121</v>
-      </c>
-      <c r="B3">
-        <v>35000</v>
-      </c>
-      <c r="C3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>162</v>
-      </c>
-      <c r="B4">
-        <v>7920</v>
-      </c>
-      <c r="C4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>129</v>
-      </c>
-      <c r="B5">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>124</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAA36DB8-B0B9-4A0A-8A56-527230CA91FC}">
-  <dimension ref="A1:D11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="32.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5">
-        <v>0.7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="1">
-        <v>50</v>
-      </c>
-      <c r="C10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>104</v>
-      </c>
-      <c r="B11">
-        <v>0.9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A644868A-CA0D-4E33-AC4A-13C92D1F9685}">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -3526,6 +3027,505 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9896EE1E-7F56-45CB-B0FF-A4EB36B766F1}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3">
+        <v>35000</v>
+      </c>
+      <c r="C3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B4">
+        <v>7920</v>
+      </c>
+      <c r="C4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C77679F-E498-462D-825B-EAF86D6734F3}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="C3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4">
+        <v>1204.67</v>
+      </c>
+      <c r="C4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>172</v>
+      </c>
+      <c r="D5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5B35FB0-FC35-4894-B852-40A6833023F4}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3">
+        <v>2.5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4">
+        <v>0.1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{057E51FA-16AA-4EDB-95D7-E76738AA23C5}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3">
+        <v>1383.46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="C4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5">
+        <v>69.17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7">
+        <v>50</v>
+      </c>
+      <c r="C7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4E9EB40-91BA-4B28-833D-B3DB1EE1EE78}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B5">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B6">
+        <v>1.71</v>
+      </c>
+      <c r="C6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{285FC4B4-1D25-4960-A894-56724304077E}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4">
+        <v>174</v>
+      </c>
+      <c r="C4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5">
+        <v>1.54</v>
+      </c>
+      <c r="C5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
made proces more efficient
</commit_message>
<xml_diff>
--- a/data/LDH_attributes.xlsx
+++ b/data/LDH_attributes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chant\PycharmProjects\FUSE-V2\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/Documents/University Work/summer work experience/Imperial College/FUSE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE760C4-F832-4B26-84FB-93A653C477B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C783357A-0391-BE41-B158-B22D3E86CDAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="9" activeTab="10" xr2:uid="{9D386D14-BB1A-49FB-A5CB-94A6FCCCA1F9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" firstSheet="9" activeTab="16" xr2:uid="{9D386D14-BB1A-49FB-A5CB-94A6FCCCA1F9}"/>
   </bookViews>
   <sheets>
     <sheet name="chemicals_sorbent_synthesis" sheetId="2" r:id="rId1"/>
@@ -32,10 +32,19 @@
     <sheet name="equipment" sheetId="6" r:id="rId17"/>
     <sheet name="capex" sheetId="21" r:id="rId18"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -194,12 +203,6 @@
     <t>size factor</t>
   </si>
   <si>
-    <t>size base</t>
-  </si>
-  <si>
-    <t>size ref</t>
-  </si>
-  <si>
     <t>drive power</t>
   </si>
   <si>
@@ -353,9 +356,6 @@
     <t xml:space="preserve"> comments</t>
   </si>
   <si>
-    <t>CEPCI base</t>
-  </si>
-  <si>
     <t>yield</t>
   </si>
   <si>
@@ -774,6 +774,15 @@
   </si>
   <si>
     <t>Cost factors of operating labort</t>
+  </si>
+  <si>
+    <t>size_ref</t>
+  </si>
+  <si>
+    <t>size_base</t>
+  </si>
+  <si>
+    <t>CEPCI_base</t>
   </si>
 </sst>
 </file>
@@ -1167,17 +1176,17 @@
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="32.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1191,7 +1200,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -1199,7 +1208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -1210,7 +1219,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -1221,7 +1230,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -1229,7 +1238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -1237,7 +1246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -1245,7 +1254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -1259,9 +1268,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B11">
         <v>0.9</v>
@@ -1281,17 +1290,17 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.5546875" customWidth="1"/>
+    <col min="1" max="1" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1302,23 +1311,23 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B4" s="1">
         <v>0.9</v>
@@ -1327,9 +1336,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B5" s="1">
         <v>0.8</v>
@@ -1338,34 +1347,34 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B6">
         <v>298.14999999999998</v>
       </c>
       <c r="C6" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D6" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B7">
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B8" s="1">
         <v>2</v>
@@ -1377,9 +1386,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B9">
         <v>353</v>
@@ -1388,20 +1397,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
@@ -1413,7 +1422,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
@@ -1427,7 +1436,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>45</v>
       </c>
@@ -1441,7 +1450,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>33</v>
       </c>
@@ -1452,40 +1461,40 @@
         <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B15" s="1">
         <v>5000</v>
       </c>
       <c r="C15" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D15" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B16">
         <v>0.8</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B17">
         <v>313.14999999999998</v>
       </c>
       <c r="D17" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -1498,21 +1507,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A0F109E-90BE-42A5-8DFF-EE3A7F8215F0}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.109375" customWidth="1"/>
+    <col min="1" max="1" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1526,7 +1535,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1537,7 +1546,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1548,7 +1557,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1559,7 +1568,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1571,7 +1580,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -1592,20 +1601,20 @@
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
+    <col min="1" max="1" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B1">
         <v>2016</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1616,12 +1625,12 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -1630,63 +1639,63 @@
         <v>16</v>
       </c>
       <c r="D3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>75</v>
-      </c>
-      <c r="D4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>77</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>79</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>81</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>83</v>
       </c>
-      <c r="D8" t="s">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>86</v>
       </c>
       <c r="B10">
         <v>30</v>
@@ -1695,9 +1704,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B11">
         <v>0.2</v>
@@ -1706,18 +1715,18 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B12">
         <v>0.75</v>
       </c>
       <c r="D12" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1725,10 +1734,10 @@
         <v>9.81</v>
       </c>
       <c r="C13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1744,18 +1753,18 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.77734375" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" customWidth="1"/>
+    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1766,52 +1775,52 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B3">
         <f xml:space="preserve"> 1.5 * 10^(-3)</f>
         <v>1.5E-3</v>
       </c>
       <c r="C3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B4" s="1">
         <f>1*10^-3</f>
         <v>1E-3</v>
       </c>
       <c r="C4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B5" s="1">
         <f>1.5*10^-3</f>
         <v>1.5E-3</v>
       </c>
       <c r="C5" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="H5" t="s">
         <v>41</v>
@@ -1831,58 +1840,58 @@
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" customWidth="1"/>
+    <col min="5" max="5" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B3">
         <v>6.6600000000000006E-2</v>
       </c>
       <c r="D3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>96</v>
       </c>
       <c r="B4">
         <v>0.01</v>
       </c>
       <c r="D4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>43</v>
       </c>
@@ -1890,13 +1899,13 @@
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>34</v>
       </c>
@@ -1907,13 +1916,13 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="D6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1924,15 +1933,15 @@
         <v>0.45</v>
       </c>
       <c r="D7" t="s">
+        <v>96</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B8">
         <v>0.17</v>
@@ -1941,15 +1950,15 @@
         <v>0.24</v>
       </c>
       <c r="D8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B9">
         <f>30/45</f>
@@ -1960,22 +1969,22 @@
         <v>4.2222222222222223</v>
       </c>
       <c r="D9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E9" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
     </row>
   </sheetData>
@@ -1999,158 +2008,158 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>231</v>
-      </c>
-      <c r="C2" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>234</v>
       </c>
       <c r="B3">
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="C3" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B4">
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C4" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B5">
         <v>0.1</v>
       </c>
       <c r="C5" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>236</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>239</v>
       </c>
       <c r="B6">
         <v>0.25</v>
       </c>
       <c r="C6" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B7">
         <v>0.02</v>
       </c>
       <c r="C7" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B8">
         <v>0.02</v>
       </c>
       <c r="C8" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>221</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>224</v>
       </c>
       <c r="B9">
         <v>0.22</v>
       </c>
       <c r="C9" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B10">
         <v>0.5</v>
       </c>
       <c r="C10" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B11">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="C11" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B12">
         <v>0.13500000000000001</v>
       </c>
       <c r="C12" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B13">
         <v>0.08</v>
       </c>
       <c r="C13" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B14">
         <v>5.7500000000000002E-2</v>
       </c>
       <c r="C14" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -2166,12 +2175,12 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2179,15 +2188,15 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B3">
         <v>81890</v>
@@ -2196,59 +2205,59 @@
         <v>29</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B4" s="1">
         <v>45</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="H4" t="s">
         <v>141</v>
       </c>
-      <c r="H4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B6">
         <v>0.2</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B7">
         <v>0.2</v>
       </c>
       <c r="D7" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B8">
         <v>2.7E-2</v>
       </c>
       <c r="D8" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -2264,29 +2273,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0624EAC2-56E2-4337-8D5D-42EAA0559452}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" customWidth="1"/>
+    <col min="1" max="1" width="26.5" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="8.6640625" customWidth="1"/>
-    <col min="4" max="4" width="19.109375" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" customWidth="1"/>
-    <col min="7" max="7" width="9.109375" customWidth="1"/>
+    <col min="4" max="4" width="19.1640625" customWidth="1"/>
+    <col min="5" max="5" width="8.5" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
     <col min="11" max="11" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2297,27 +2306,27 @@
         <v>49</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>241</v>
       </c>
       <c r="F2" t="s">
-        <v>50</v>
+        <v>242</v>
       </c>
       <c r="G2" t="s">
         <v>7</v>
       </c>
       <c r="H2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I2" t="s">
         <v>30</v>
       </c>
       <c r="J2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B3">
         <v>37500</v>
@@ -2326,7 +2335,7 @@
         <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E3">
         <v>3</v>
@@ -2338,15 +2347,15 @@
         <v>48</v>
       </c>
       <c r="H3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I3">
         <v>0.53</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B4">
         <v>230000</v>
@@ -2355,7 +2364,7 @@
         <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E4">
         <v>150</v>
@@ -2367,15 +2376,15 @@
         <v>15</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I4">
         <v>0.6</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B5">
         <v>63000</v>
@@ -2384,7 +2393,7 @@
         <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E5">
         <v>15</v>
@@ -2393,18 +2402,18 @@
         <v>4</v>
       </c>
       <c r="G5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I5">
         <v>0.81</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B6">
         <v>380000</v>
@@ -2419,15 +2428,15 @@
         <v>12</v>
       </c>
       <c r="H6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I6">
         <v>0.66</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B7">
         <v>22000</v>
@@ -2436,7 +2445,7 @@
         <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E7">
         <v>1600</v>
@@ -2448,15 +2457,15 @@
         <v>15</v>
       </c>
       <c r="H7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I7">
         <v>0.85</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B8">
         <v>37500</v>
@@ -2465,7 +2474,7 @@
         <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E8">
         <v>3</v>
@@ -2477,15 +2486,15 @@
         <v>48</v>
       </c>
       <c r="H8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I8">
         <v>0.53</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B9">
         <v>230000</v>
@@ -2494,7 +2503,7 @@
         <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E9">
         <v>150</v>
@@ -2506,15 +2515,15 @@
         <v>15</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I9">
         <v>0.6</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B10">
         <v>75000</v>
@@ -2523,7 +2532,7 @@
         <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E10">
         <v>3</v>
@@ -2535,15 +2544,15 @@
         <v>48</v>
       </c>
       <c r="H10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I10">
         <v>0.53</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B11">
         <v>100000</v>
@@ -2552,7 +2561,7 @@
         <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E11">
         <v>30</v>
@@ -2564,15 +2573,15 @@
         <v>48</v>
       </c>
       <c r="H11" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="I11">
         <v>0.67</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B12">
         <v>32.5</v>
@@ -2581,7 +2590,7 @@
         <v>29</v>
       </c>
       <c r="D12" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -2593,15 +2602,15 @@
         <v>48</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="I12">
         <v>0.95</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B13">
         <v>238000</v>
@@ -2610,7 +2619,7 @@
         <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E13">
         <v>10</v>
@@ -2622,15 +2631,15 @@
         <v>15</v>
       </c>
       <c r="H13" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="I13">
         <v>0.65</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B14">
         <v>9500</v>
@@ -2639,7 +2648,7 @@
         <v>29</v>
       </c>
       <c r="D14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E14">
         <v>23</v>
@@ -2648,18 +2657,18 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="G14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I14">
         <v>0.79</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B15">
         <v>4800</v>
@@ -2668,7 +2677,7 @@
         <v>29</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E15">
         <v>7.5</v>
@@ -2677,27 +2686,27 @@
         <v>2.54</v>
       </c>
       <c r="G15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I15">
         <v>0.65</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B16">
         <v>80</v>
       </c>
       <c r="C16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E16">
         <v>15</v>
@@ -2706,10 +2715,10 @@
         <v>20</v>
       </c>
       <c r="G16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I16">
         <v>1.33</v>
@@ -2721,9 +2730,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B17">
         <v>21000</v>
@@ -2735,18 +2744,18 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>103</v>
+        <v>243</v>
       </c>
       <c r="B19">
         <v>650</v>
       </c>
       <c r="C19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
     </row>
   </sheetData>
@@ -2772,126 +2781,126 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.33203125" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="11.77734375" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C2" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B3">
         <v>0.7</v>
       </c>
       <c r="C3" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B4">
         <v>0.18</v>
       </c>
       <c r="C4" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B5">
         <v>0.1</v>
       </c>
       <c r="C5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>211</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>214</v>
       </c>
       <c r="B6">
         <v>0.38</v>
       </c>
       <c r="C6" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B7">
         <v>0.4</v>
       </c>
       <c r="C7" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B8">
         <v>0.06</v>
       </c>
       <c r="C8" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B9">
         <v>0.1</v>
       </c>
       <c r="C9" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B10">
         <v>0.25</v>
       </c>
       <c r="C10" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B11">
         <v>0.2</v>
       </c>
       <c r="C11" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -2907,18 +2916,18 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.21875" customWidth="1"/>
+    <col min="1" max="1" width="27.1640625" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -2932,15 +2941,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -2954,7 +2963,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -2968,7 +2977,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>42</v>
       </c>
@@ -2982,7 +2991,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
@@ -2996,7 +3005,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>45</v>
       </c>
@@ -3007,10 +3016,10 @@
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>33</v>
       </c>
@@ -3021,7 +3030,7 @@
         <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -3038,17 +3047,17 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3059,37 +3068,37 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B3">
         <v>35000</v>
       </c>
       <c r="C3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B4">
         <v>7920</v>
       </c>
       <c r="C4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B5">
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -3105,17 +3114,17 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3129,43 +3138,43 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B3">
         <v>0.19400000000000001</v>
       </c>
       <c r="C3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B4">
         <v>1204.67</v>
       </c>
       <c r="C4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D5" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -3181,17 +3190,17 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.21875" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3205,9 +3214,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B3">
         <v>2.5</v>
@@ -3216,12 +3225,12 @@
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B4">
         <v>0.1</v>
@@ -3230,56 +3239,56 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B5">
         <v>0.9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B7">
         <v>8</v>
       </c>
       <c r="C7" t="s">
+        <v>130</v>
+      </c>
+      <c r="D7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>133</v>
-      </c>
-      <c r="D7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>136</v>
       </c>
       <c r="B8">
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -3295,17 +3304,17 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" customWidth="1"/>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3316,34 +3325,34 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B3">
         <v>1383.46</v>
       </c>
       <c r="C3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B4">
         <v>0.19400000000000001</v>
       </c>
       <c r="C4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B5">
         <v>69.17</v>
@@ -3352,37 +3361,37 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B6">
         <v>10</v>
       </c>
       <c r="C6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" t="s">
         <v>107</v>
       </c>
-      <c r="D6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B7">
         <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D7" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -3401,17 +3410,17 @@
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3419,45 +3428,45 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B3">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B5">
         <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B6">
         <v>1.71</v>
       </c>
       <c r="C6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -3473,17 +3482,17 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" customWidth="1"/>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3494,7 +3503,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -3502,26 +3511,26 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B4">
         <v>174</v>
       </c>
       <c r="C4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B5">
         <v>1.54</v>
       </c>
       <c r="C5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -3537,17 +3546,17 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3555,15 +3564,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B3">
         <v>0.7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -3574,9 +3583,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B5" s="1">
         <v>2</v>
@@ -3588,7 +3597,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -3602,7 +3611,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>45</v>
       </c>
@@ -3616,7 +3625,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>33</v>
       </c>
@@ -3627,7 +3636,7 @@
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Addition of belt conveyor and changes to LDH energy
</commit_message>
<xml_diff>
--- a/data/LDH_attributes.xlsx
+++ b/data/LDH_attributes.xlsx
@@ -8,29 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chant\PycharmProjects\FUSE-V2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE760C4-F832-4B26-84FB-93A653C477B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23FCA67E-2A59-4456-8451-89E8EABE448F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="9" activeTab="10" xr2:uid="{9D386D14-BB1A-49FB-A5CB-94A6FCCCA1F9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="12" activeTab="12" xr2:uid="{9D386D14-BB1A-49FB-A5CB-94A6FCCCA1F9}"/>
   </bookViews>
   <sheets>
-    <sheet name="chemicals_sorbent_synthesis" sheetId="2" r:id="rId1"/>
-    <sheet name="sorbent_synthesis_reaction" sheetId="3" r:id="rId2"/>
-    <sheet name="plant" sheetId="15" r:id="rId3"/>
-    <sheet name="brine" sheetId="14" r:id="rId4"/>
-    <sheet name="column" sheetId="17" r:id="rId5"/>
-    <sheet name="washing" sheetId="12" r:id="rId6"/>
-    <sheet name="stripping" sheetId="13" r:id="rId7"/>
-    <sheet name="FO" sheetId="16" r:id="rId8"/>
-    <sheet name="Li2CO3_processing" sheetId="19" r:id="rId9"/>
-    <sheet name="Li2CO3_purification" sheetId="20" r:id="rId10"/>
-    <sheet name="standard_impeller" sheetId="4" r:id="rId11"/>
-    <sheet name="pump" sheetId="10" r:id="rId12"/>
-    <sheet name="water" sheetId="5" r:id="rId13"/>
-    <sheet name="cost_chemicals" sheetId="11" r:id="rId14"/>
-    <sheet name="opex" sheetId="22" r:id="rId15"/>
-    <sheet name="worker" sheetId="18" r:id="rId16"/>
-    <sheet name="equipment" sheetId="6" r:id="rId17"/>
-    <sheet name="capex" sheetId="21" r:id="rId18"/>
+    <sheet name="Process overview" sheetId="23" r:id="rId1"/>
+    <sheet name="chemicals_sorbent_synthesis" sheetId="2" r:id="rId2"/>
+    <sheet name="sorbent_synthesis_reaction" sheetId="3" r:id="rId3"/>
+    <sheet name="plant" sheetId="15" r:id="rId4"/>
+    <sheet name="brine" sheetId="14" r:id="rId5"/>
+    <sheet name="column" sheetId="17" r:id="rId6"/>
+    <sheet name="washing" sheetId="12" r:id="rId7"/>
+    <sheet name="stripping" sheetId="13" r:id="rId8"/>
+    <sheet name="FO" sheetId="16" r:id="rId9"/>
+    <sheet name="Li2CO3_processing" sheetId="19" r:id="rId10"/>
+    <sheet name="Li2CO3_purification" sheetId="20" r:id="rId11"/>
+    <sheet name="standard_impeller" sheetId="4" r:id="rId12"/>
+    <sheet name="standard_belt_conveyor" sheetId="24" r:id="rId13"/>
+    <sheet name="pump" sheetId="10" r:id="rId14"/>
+    <sheet name="water" sheetId="5" r:id="rId15"/>
+    <sheet name="cost_chemicals" sheetId="11" r:id="rId16"/>
+    <sheet name="opex" sheetId="22" r:id="rId17"/>
+    <sheet name="worker" sheetId="18" r:id="rId18"/>
+    <sheet name="equipment" sheetId="6" r:id="rId19"/>
+    <sheet name="capex" sheetId="21" r:id="rId20"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="334">
   <si>
     <t>key</t>
   </si>
@@ -774,13 +776,336 @@
   </si>
   <si>
     <t>Cost factors of operating labort</t>
+  </si>
+  <si>
+    <t>Machine</t>
+  </si>
+  <si>
+    <t>Reaction step</t>
+  </si>
+  <si>
+    <t>Specification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Size </t>
+  </si>
+  <si>
+    <t>Amounts processed</t>
+  </si>
+  <si>
+    <t>Reaction</t>
+  </si>
+  <si>
+    <t>Reactor 1</t>
+  </si>
+  <si>
+    <t>Batch reactor</t>
+  </si>
+  <si>
+    <t>Volume: 500 l</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">LiOH*H2O + mAl(OH)3 + nH2O + HCl </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+        <charset val="2"/>
+      </rPr>
+      <t>à</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> LiCl*m[Al(OH)3]*nH2O + H2O</t>
+    </r>
+  </si>
+  <si>
+    <t>Open tank</t>
+  </si>
+  <si>
+    <t>Reaction in two steps</t>
+  </si>
+  <si>
+    <t>Jacketed with agitator</t>
+  </si>
+  <si>
+    <t>1. LiOH*H2O, Al(OH)3 and H20 are mixed together in the batch reactor at the given reaction temperature and stirred for reaction time 1</t>
+  </si>
+  <si>
+    <t>2. HCl is added to the mixture and the solution is stirred for reaction time 2</t>
+  </si>
+  <si>
+    <t>Filter 1</t>
+  </si>
+  <si>
+    <t>Batch vacuum (leaf) filter</t>
+  </si>
+  <si>
+    <t>Filter area: 20 m^2</t>
+  </si>
+  <si>
+    <t>Hammer mill</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">output size: 150 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>μm</t>
+    </r>
+  </si>
+  <si>
+    <t>Drive power: 4 kW</t>
+  </si>
+  <si>
+    <t>LDH column</t>
+  </si>
+  <si>
+    <t>Column extraction</t>
+  </si>
+  <si>
+    <t>Extraction column (from Huang 2021)</t>
+  </si>
+  <si>
+    <t>Input Brine: 1485.3 m^3/h</t>
+  </si>
+  <si>
+    <t>Outout LiCl sol: 6365.4795 l/h</t>
+  </si>
+  <si>
+    <t>Forward Osmisis unit</t>
+  </si>
+  <si>
+    <t>FO unit (from Huang 2021)</t>
+  </si>
+  <si>
+    <t>Filter area: 3593 m^2</t>
+  </si>
+  <si>
+    <t>Input LiCl sol: 6365.4795 l/h</t>
+  </si>
+  <si>
+    <t>Output: 1316.9958 l/h</t>
+  </si>
+  <si>
+    <t>Reactor 2</t>
+  </si>
+  <si>
+    <t>Li2CO3 processing</t>
+  </si>
+  <si>
+    <t>Batchr reactor</t>
+  </si>
+  <si>
+    <t>Volume: 5000 l</t>
+  </si>
+  <si>
+    <t>Input LiCl sol: 1316.9958 l/h</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2 LiCl (aq) +  Na2CO3 (aq) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+        <charset val="2"/>
+      </rPr>
+      <t>à</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Li2CO3 + 2 NaCl</t>
+    </r>
+  </si>
+  <si>
+    <t>Input Na2CO3: 286.414  kg/h</t>
+  </si>
+  <si>
+    <t>Output Li2CO3: 199.702 kg/h</t>
+  </si>
+  <si>
+    <t>Filter 2</t>
+  </si>
+  <si>
+    <t>Batch vaccum (leaf) filter</t>
+  </si>
+  <si>
+    <t>Filter area: 100 m^2</t>
+  </si>
+  <si>
+    <t>Reactor 3</t>
+  </si>
+  <si>
+    <t>Li2CO3 purification</t>
+  </si>
+  <si>
+    <t>Volume: 5000l</t>
+  </si>
+  <si>
+    <t>Input Li2CO3: 199.702 kg/h</t>
+  </si>
+  <si>
+    <t>Li2CO3 + H2O + CO2 --&gt; 2 LiHCO3</t>
+  </si>
+  <si>
+    <t>carbonation</t>
+  </si>
+  <si>
+    <t>Pressure vessel</t>
+  </si>
+  <si>
+    <t>Input H2O: 48.68 l/h</t>
+  </si>
+  <si>
+    <t>Input CO2 : 118.927 kg/h</t>
+  </si>
+  <si>
+    <t>gas inlet (CO2)</t>
+  </si>
+  <si>
+    <t>Output LiHCO3: 368.196 kg/h</t>
+  </si>
+  <si>
+    <t>same as filter 2</t>
+  </si>
+  <si>
+    <t>carboantion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ion exchange column </t>
+  </si>
+  <si>
+    <t>resin volume: 10m^3</t>
+  </si>
+  <si>
+    <t>Input LiHCO3: 368.196 kg/h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ion exchange resin </t>
+  </si>
+  <si>
+    <t>removal of divalent and trivalent ions</t>
+  </si>
+  <si>
+    <t>aminophosphonic acid groups</t>
+  </si>
+  <si>
+    <t>Reactor 4</t>
+  </si>
+  <si>
+    <t>same as Reactor 3</t>
+  </si>
+  <si>
+    <t>2 LiHCO3 --&gt; Li2CO3 + H2O + CO2</t>
+  </si>
+  <si>
+    <t>precipitation</t>
+  </si>
+  <si>
+    <t>Output H2O: 48.68 l/h</t>
+  </si>
+  <si>
+    <t>Output CO2 : 118.927 kg/h</t>
+  </si>
+  <si>
+    <t>Filter 4</t>
+  </si>
+  <si>
+    <t>same as Filter 2 and 3</t>
+  </si>
+  <si>
+    <t>rotary, horizontal (batch)</t>
+  </si>
+  <si>
+    <t>drying surface: 60 m^2</t>
+  </si>
+  <si>
+    <t>drying of pure Li2CO3 filter cake</t>
+  </si>
+  <si>
+    <t>Transportation (liquid)</t>
+  </si>
+  <si>
+    <t>centrifugal, AVS</t>
+  </si>
+  <si>
+    <t>Control valves</t>
+  </si>
+  <si>
+    <t>Belt conveyor</t>
+  </si>
+  <si>
+    <t>Transportation (solids)</t>
+  </si>
+  <si>
+    <t>Sheets: sorbents_syntehsis_reaction &amp; standard_impeller</t>
+  </si>
+  <si>
+    <t>Sheet: FO</t>
+  </si>
+  <si>
+    <t>Sheets: Li2CO3_processing &amp; standard_impeller</t>
+  </si>
+  <si>
+    <t>Sheets: Li2CO3_purification &amp; standard_impeller</t>
+  </si>
+  <si>
+    <t>Sheets: plant, brine, column, washing, stripping</t>
+  </si>
+  <si>
+    <t>ft/min</t>
+  </si>
+  <si>
+    <t>assumption</t>
+  </si>
+  <si>
+    <t>gradient</t>
+  </si>
+  <si>
+    <t>°</t>
+  </si>
+  <si>
+    <t>output</t>
+  </si>
+  <si>
+    <t>t/h</t>
+  </si>
+  <si>
+    <t>belt_speed</t>
+  </si>
+  <si>
+    <t>belt_length</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -817,6 +1142,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Wingdings"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -826,7 +1163,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -834,18 +1171,83 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -862,6 +1264,61 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>472440</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>100965</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86DC3DD0-C955-4405-98E9-858F7633F515}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15240" y="129540"/>
+          <a:ext cx="7772400" cy="23197185"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1160,21 +1617,484 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAA36DB8-B0B9-4A0A-8A56-527230CA91FC}">
-  <dimension ref="A1:D11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96F39DFA-2FDB-4EC9-BBFE-157F4FCC3560}">
+  <dimension ref="N2:T125"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" customWidth="1"/>
+    <col min="14" max="14" width="19" customWidth="1"/>
+    <col min="15" max="15" width="27.6640625" customWidth="1"/>
+    <col min="16" max="16" width="34.109375" customWidth="1"/>
+    <col min="17" max="17" width="19.6640625" customWidth="1"/>
+    <col min="18" max="18" width="28.77734375" customWidth="1"/>
+    <col min="19" max="19" width="62.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="14:20" x14ac:dyDescent="0.3">
+      <c r="N2" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="12" spans="14:20" x14ac:dyDescent="0.3">
+      <c r="N12" t="s">
+        <v>250</v>
+      </c>
+      <c r="O12" t="s">
+        <v>117</v>
+      </c>
+      <c r="P12" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>252</v>
+      </c>
+      <c r="S12" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="13" spans="14:20" x14ac:dyDescent="0.3">
+      <c r="P13" t="s">
+        <v>254</v>
+      </c>
+      <c r="S13" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="14" spans="14:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P14" t="s">
+        <v>256</v>
+      </c>
+      <c r="R14" s="6"/>
+      <c r="S14" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="T14" s="6"/>
+    </row>
+    <row r="15" spans="14:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P15" s="14" t="s">
+        <v>321</v>
+      </c>
+      <c r="R15" s="6"/>
+      <c r="S15" s="12"/>
+      <c r="T15" s="6"/>
+    </row>
+    <row r="16" spans="14:20" x14ac:dyDescent="0.3">
+      <c r="P16" s="14"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="T16" s="7"/>
+    </row>
+    <row r="19" spans="14:17" x14ac:dyDescent="0.3">
+      <c r="N19" t="s">
+        <v>259</v>
+      </c>
+      <c r="O19" t="s">
+        <v>117</v>
+      </c>
+      <c r="P19" t="s">
+        <v>260</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="25" spans="14:17" x14ac:dyDescent="0.3">
+      <c r="N25" t="s">
+        <v>199</v>
+      </c>
+      <c r="O25" t="s">
+        <v>117</v>
+      </c>
+      <c r="P25" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="26" spans="14:17" x14ac:dyDescent="0.3">
+      <c r="P26" t="s">
+        <v>263</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="39" spans="14:18" x14ac:dyDescent="0.3">
+      <c r="N39" t="s">
+        <v>265</v>
+      </c>
+      <c r="O39" t="s">
+        <v>266</v>
+      </c>
+      <c r="P39" t="s">
+        <v>267</v>
+      </c>
+      <c r="Q39">
+        <v>12</v>
+      </c>
+      <c r="R39" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="40" spans="14:18" x14ac:dyDescent="0.3">
+      <c r="P40" s="15" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="41" spans="14:18" x14ac:dyDescent="0.3">
+      <c r="P41" s="15"/>
+    </row>
+    <row r="42" spans="14:18" x14ac:dyDescent="0.3">
+      <c r="P42" s="10"/>
+      <c r="R42" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="52" spans="14:18" x14ac:dyDescent="0.3">
+      <c r="N52" t="s">
+        <v>270</v>
+      </c>
+      <c r="O52" t="s">
+        <v>266</v>
+      </c>
+      <c r="P52" t="s">
+        <v>271</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>272</v>
+      </c>
+      <c r="R52" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="53" spans="14:18" x14ac:dyDescent="0.3">
+      <c r="P53" t="s">
+        <v>322</v>
+      </c>
+      <c r="R53" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="70" spans="14:19" x14ac:dyDescent="0.3">
+      <c r="N70" t="s">
+        <v>275</v>
+      </c>
+      <c r="O70" t="s">
+        <v>276</v>
+      </c>
+      <c r="P70" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>278</v>
+      </c>
+      <c r="R70" t="s">
+        <v>279</v>
+      </c>
+      <c r="S70" s="9" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="71" spans="14:19" x14ac:dyDescent="0.3">
+      <c r="P71" t="s">
+        <v>254</v>
+      </c>
+      <c r="R71" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="72" spans="14:19" x14ac:dyDescent="0.3">
+      <c r="P72" t="s">
+        <v>256</v>
+      </c>
+      <c r="R72" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="73" spans="14:19" x14ac:dyDescent="0.3">
+      <c r="P73" s="14" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="74" spans="14:19" x14ac:dyDescent="0.3">
+      <c r="P74" s="14"/>
+    </row>
+    <row r="77" spans="14:19" x14ac:dyDescent="0.3">
+      <c r="N77" t="s">
+        <v>283</v>
+      </c>
+      <c r="O77" t="s">
+        <v>276</v>
+      </c>
+      <c r="P77" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q77" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="85" spans="14:19" x14ac:dyDescent="0.3">
+      <c r="N85" t="s">
+        <v>286</v>
+      </c>
+      <c r="O85" t="s">
+        <v>287</v>
+      </c>
+      <c r="P85" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q85" t="s">
+        <v>288</v>
+      </c>
+      <c r="R85" t="s">
+        <v>289</v>
+      </c>
+      <c r="S85" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="86" spans="14:19" x14ac:dyDescent="0.3">
+      <c r="O86" t="s">
+        <v>291</v>
+      </c>
+      <c r="P86" t="s">
+        <v>292</v>
+      </c>
+      <c r="R86" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="87" spans="14:19" x14ac:dyDescent="0.3">
+      <c r="P87" t="s">
+        <v>256</v>
+      </c>
+      <c r="R87" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="88" spans="14:19" x14ac:dyDescent="0.3">
+      <c r="P88" t="s">
+        <v>295</v>
+      </c>
+      <c r="R88" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="89" spans="14:19" x14ac:dyDescent="0.3">
+      <c r="P89" s="15" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="90" spans="14:19" x14ac:dyDescent="0.3">
+      <c r="P90" s="15"/>
+    </row>
+    <row r="94" spans="14:19" x14ac:dyDescent="0.3">
+      <c r="N94" t="s">
+        <v>283</v>
+      </c>
+      <c r="O94" t="s">
+        <v>287</v>
+      </c>
+      <c r="P94" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="95" spans="14:19" x14ac:dyDescent="0.3">
+      <c r="O95" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="100" spans="14:19" x14ac:dyDescent="0.3">
+      <c r="N100" t="s">
+        <v>299</v>
+      </c>
+      <c r="O100" t="s">
+        <v>287</v>
+      </c>
+      <c r="Q100" t="s">
+        <v>300</v>
+      </c>
+      <c r="R100" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="101" spans="14:19" x14ac:dyDescent="0.3">
+      <c r="N101" t="s">
+        <v>302</v>
+      </c>
+      <c r="O101" s="13" t="s">
+        <v>303</v>
+      </c>
+      <c r="P101" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q101" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="102" spans="14:19" x14ac:dyDescent="0.3">
+      <c r="O102" s="13"/>
+    </row>
+    <row r="104" spans="14:19" x14ac:dyDescent="0.3">
+      <c r="N104" t="s">
+        <v>305</v>
+      </c>
+      <c r="O104" t="s">
+        <v>287</v>
+      </c>
+      <c r="P104" t="s">
+        <v>306</v>
+      </c>
+      <c r="R104" t="s">
+        <v>301</v>
+      </c>
+      <c r="S104" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="105" spans="14:19" x14ac:dyDescent="0.3">
+      <c r="O105" t="s">
+        <v>308</v>
+      </c>
+      <c r="R105" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="106" spans="14:19" x14ac:dyDescent="0.3">
+      <c r="R106" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="107" spans="14:19" x14ac:dyDescent="0.3">
+      <c r="R107" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="109" spans="14:19" x14ac:dyDescent="0.3">
+      <c r="N109" t="s">
+        <v>311</v>
+      </c>
+      <c r="O109" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="110" spans="14:19" x14ac:dyDescent="0.3">
+      <c r="O110" t="s">
+        <v>308</v>
+      </c>
+      <c r="P110" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="116" spans="14:18" x14ac:dyDescent="0.3">
+      <c r="N116" t="s">
+        <v>209</v>
+      </c>
+      <c r="O116" t="s">
+        <v>287</v>
+      </c>
+      <c r="P116" t="s">
+        <v>313</v>
+      </c>
+      <c r="Q116" t="s">
+        <v>314</v>
+      </c>
+      <c r="R116" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="117" spans="14:18" x14ac:dyDescent="0.3">
+      <c r="O117" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="122" spans="14:18" x14ac:dyDescent="0.3">
+      <c r="N122" t="s">
+        <v>205</v>
+      </c>
+      <c r="O122" t="s">
+        <v>316</v>
+      </c>
+      <c r="P122" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="123" spans="14:18" x14ac:dyDescent="0.3">
+      <c r="N123" t="s">
+        <v>206</v>
+      </c>
+      <c r="O123" t="s">
+        <v>316</v>
+      </c>
+      <c r="P123" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="124" spans="14:18" x14ac:dyDescent="0.3">
+      <c r="N124" t="s">
+        <v>207</v>
+      </c>
+      <c r="O124" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="125" spans="14:18" x14ac:dyDescent="0.3">
+      <c r="N125" t="s">
+        <v>319</v>
+      </c>
+      <c r="O125" t="s">
+        <v>320</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="S14:S15"/>
+    <mergeCell ref="O101:O102"/>
+    <mergeCell ref="P15:P16"/>
+    <mergeCell ref="P73:P74"/>
+    <mergeCell ref="P89:P90"/>
+    <mergeCell ref="P40:P41"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43797486-FEB5-4613-A524-BCA6B61EB1F2}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>105</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1184,101 +2104,93 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>104</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>30</v>
+        <v>363.15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5">
-        <v>0.7</v>
+        <v>157</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>38</v>
+      <c r="A6" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>16.260000000000002</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>39</v>
+      <c r="A7" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>6.3499999999999997E-3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>40</v>
+      <c r="A8" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="B8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="1">
-        <v>50</v>
-      </c>
-      <c r="C10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>104</v>
-      </c>
-      <c r="B11">
-        <v>0.9</v>
+        <v>3.7160000000000002</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC77B64C-CA76-4811-9820-2E72F61B9A29}">
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1494,11 +2406,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A0F109E-90BE-42A5-8DFF-EE3A7F8215F0}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -1584,7 +2496,95 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39F5853C-7EBD-44C3-B44F-35BFE47CA7B2}">
+  <dimension ref="A2:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>332</v>
+      </c>
+      <c r="B3" s="1">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
+        <v>326</v>
+      </c>
+      <c r="D3" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>333</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>328</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>330</v>
+      </c>
+      <c r="B6">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7">
+        <v>0.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB9B9DC-89ED-462F-B40D-72EC74E0973E}">
   <dimension ref="A1:D13"/>
   <sheetViews>
@@ -1736,7 +2736,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{489F410F-4873-4D81-A8B1-2DDFA51D15D5}">
   <dimension ref="A1:H5"/>
   <sheetViews>
@@ -1823,7 +2823,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F37A8F43-ECBD-4243-988B-AAA9A59B3D22}">
   <dimension ref="A2:F14"/>
   <sheetViews>
@@ -1991,7 +2991,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24498815-2749-43E0-8B7E-EA1E475CA5F2}">
   <dimension ref="A1:C14"/>
   <sheetViews>
@@ -2158,7 +3158,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1330EF6F-438D-41F9-93CA-537B5AFAC263}">
   <dimension ref="A2:H8"/>
   <sheetViews>
@@ -2260,7 +3260,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0624EAC2-56E2-4337-8D5D-42EAA0559452}">
   <dimension ref="A1:K22"/>
   <sheetViews>
@@ -2764,7 +3764,121 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAA36DB8-B0B9-4A0A-8A56-527230CA91FC}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5">
+        <v>0.7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="1">
+        <v>50</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B11">
+        <v>0.9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{285D6F2E-FA24-4D6E-BA33-9B8C5FFBA286}">
   <dimension ref="A1:C11"/>
   <sheetViews>
@@ -2899,7 +4013,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A644868A-CA0D-4E33-AC4A-13C92D1F9685}">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -3030,7 +4144,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9896EE1E-7F56-45CB-B0FF-A4EB36B766F1}">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -3097,7 +4211,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C77679F-E498-462D-825B-EAF86D6734F3}">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -3173,7 +4287,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5B35FB0-FC35-4894-B852-40A6833023F4}">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -3287,7 +4401,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{057E51FA-16AA-4EDB-95D7-E76738AA23C5}">
   <dimension ref="A1:D8"/>
   <sheetViews>
@@ -3393,7 +4507,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4E9EB40-91BA-4B28-833D-B3DB1EE1EE78}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -3465,7 +4579,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{285FC4B4-1D25-4960-A894-56724304077E}">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -3527,110 +4641,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43797486-FEB5-4613-A524-BCA6B61EB1F2}">
-  <dimension ref="A1:D8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B3">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>363.15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>157</v>
-      </c>
-      <c r="B5" s="1">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6">
-        <v>16.260000000000002</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7">
-        <v>6.3499999999999997E-3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8">
-        <v>3.7160000000000002</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
made a plot function converted costs into a data frame for more consistent file handling
</commit_message>
<xml_diff>
--- a/data/LDH_attributes.xlsx
+++ b/data/LDH_attributes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chant\PycharmProjects\FUSE-V2\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/Documents/University Work/summer work experience/Imperial College/FUSE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE613855-CBD3-4431-A4DF-9E5DE1AB0784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63DDCA66-8F36-3040-B892-7A2B08B04474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="12" activeTab="18" xr2:uid="{9D386D14-BB1A-49FB-A5CB-94A6FCCCA1F9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" firstSheet="12" activeTab="18" xr2:uid="{9D386D14-BB1A-49FB-A5CB-94A6FCCCA1F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Process overview" sheetId="23" r:id="rId1"/>
@@ -34,10 +34,19 @@
     <sheet name="equipment" sheetId="6" r:id="rId19"/>
     <sheet name="capex" sheetId="21" r:id="rId20"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -347,9 +356,6 @@
   </si>
   <si>
     <t xml:space="preserve"> comments</t>
-  </si>
-  <si>
-    <t>CEPCI base</t>
   </si>
   <si>
     <t>yield</t>
@@ -1099,6 +1105,9 @@
   </si>
   <si>
     <t>size_base</t>
+  </si>
+  <si>
+    <t>CEPCI_base</t>
   </si>
 </sst>
 </file>
@@ -1624,445 +1633,445 @@
       <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="14" max="14" width="19" customWidth="1"/>
     <col min="15" max="15" width="27.6640625" customWidth="1"/>
-    <col min="16" max="16" width="34.109375" customWidth="1"/>
+    <col min="16" max="16" width="34.1640625" customWidth="1"/>
     <col min="17" max="17" width="19.6640625" customWidth="1"/>
-    <col min="18" max="18" width="28.77734375" customWidth="1"/>
-    <col min="19" max="19" width="62.44140625" customWidth="1"/>
+    <col min="18" max="18" width="28.83203125" customWidth="1"/>
+    <col min="19" max="19" width="62.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="14:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="14:20" x14ac:dyDescent="0.2">
       <c r="N2" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="O2" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="Q2" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="R2" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="S2" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="S2" s="4" t="s">
+    </row>
+    <row r="12" spans="14:20" x14ac:dyDescent="0.2">
+      <c r="N12" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="12" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N12" t="s">
+      <c r="O12" t="s">
+        <v>114</v>
+      </c>
+      <c r="P12" t="s">
         <v>248</v>
       </c>
-      <c r="O12" t="s">
-        <v>115</v>
-      </c>
-      <c r="P12" t="s">
+      <c r="Q12" t="s">
         <v>249</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="S12" t="s">
         <v>250</v>
       </c>
-      <c r="S12" t="s">
+    </row>
+    <row r="13" spans="14:20" x14ac:dyDescent="0.2">
+      <c r="P13" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="13" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="P13" t="s">
+      <c r="S13" t="s">
         <v>252</v>
       </c>
-      <c r="S13" t="s">
+    </row>
+    <row r="14" spans="14:20" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P14" t="s">
         <v>253</v>
-      </c>
-    </row>
-    <row r="14" spans="14:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="P14" t="s">
-        <v>254</v>
       </c>
       <c r="R14" s="6"/>
       <c r="S14" s="11" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="T14" s="6"/>
     </row>
-    <row r="15" spans="14:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="14:20" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="P15" s="14" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="R15" s="6"/>
       <c r="S15" s="12"/>
       <c r="T15" s="6"/>
     </row>
-    <row r="16" spans="14:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="14:20" x14ac:dyDescent="0.2">
       <c r="P16" s="14"/>
       <c r="R16" s="7"/>
       <c r="S16" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="T16" s="7"/>
+    </row>
+    <row r="19" spans="14:17" x14ac:dyDescent="0.2">
+      <c r="N19" t="s">
         <v>256</v>
       </c>
-      <c r="T16" s="7"/>
-    </row>
-    <row r="19" spans="14:17" x14ac:dyDescent="0.3">
-      <c r="N19" t="s">
+      <c r="O19" t="s">
+        <v>114</v>
+      </c>
+      <c r="P19" t="s">
         <v>257</v>
       </c>
-      <c r="O19" t="s">
-        <v>115</v>
-      </c>
-      <c r="P19" t="s">
+      <c r="Q19" t="s">
         <v>258</v>
       </c>
-      <c r="Q19" t="s">
+    </row>
+    <row r="25" spans="14:17" x14ac:dyDescent="0.2">
+      <c r="N25" t="s">
+        <v>196</v>
+      </c>
+      <c r="O25" t="s">
+        <v>114</v>
+      </c>
+      <c r="P25" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="25" spans="14:17" x14ac:dyDescent="0.3">
-      <c r="N25" t="s">
-        <v>197</v>
-      </c>
-      <c r="O25" t="s">
-        <v>115</v>
-      </c>
-      <c r="P25" t="s">
+    <row r="26" spans="14:17" x14ac:dyDescent="0.2">
+      <c r="P26" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="26" spans="14:17" x14ac:dyDescent="0.3">
-      <c r="P26" t="s">
+      <c r="Q26" t="s">
         <v>261</v>
       </c>
-      <c r="Q26" t="s">
+    </row>
+    <row r="39" spans="14:18" x14ac:dyDescent="0.2">
+      <c r="N39" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="39" spans="14:18" x14ac:dyDescent="0.3">
-      <c r="N39" t="s">
+      <c r="O39" t="s">
         <v>263</v>
       </c>
-      <c r="O39" t="s">
+      <c r="P39" t="s">
         <v>264</v>
-      </c>
-      <c r="P39" t="s">
-        <v>265</v>
       </c>
       <c r="Q39">
         <v>12</v>
       </c>
       <c r="R39" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="40" spans="14:18" x14ac:dyDescent="0.3">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="40" spans="14:18" x14ac:dyDescent="0.2">
       <c r="P40" s="15" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="41" spans="14:18" x14ac:dyDescent="0.3">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="41" spans="14:18" x14ac:dyDescent="0.2">
       <c r="P41" s="15"/>
     </row>
-    <row r="42" spans="14:18" x14ac:dyDescent="0.3">
+    <row r="42" spans="14:18" x14ac:dyDescent="0.2">
       <c r="P42" s="10"/>
       <c r="R42" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="52" spans="14:18" x14ac:dyDescent="0.2">
+      <c r="N52" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="52" spans="14:18" x14ac:dyDescent="0.3">
-      <c r="N52" t="s">
+      <c r="O52" t="s">
+        <v>263</v>
+      </c>
+      <c r="P52" t="s">
         <v>268</v>
       </c>
-      <c r="O52" t="s">
-        <v>264</v>
-      </c>
-      <c r="P52" t="s">
+      <c r="Q52" t="s">
         <v>269</v>
       </c>
-      <c r="Q52" t="s">
+      <c r="R52" t="s">
         <v>270</v>
       </c>
-      <c r="R52" t="s">
+    </row>
+    <row r="53" spans="14:18" x14ac:dyDescent="0.2">
+      <c r="P53" t="s">
+        <v>319</v>
+      </c>
+      <c r="R53" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="53" spans="14:18" x14ac:dyDescent="0.3">
-      <c r="P53" t="s">
+    <row r="70" spans="14:19" x14ac:dyDescent="0.2">
+      <c r="N70" t="s">
+        <v>272</v>
+      </c>
+      <c r="O70" t="s">
+        <v>273</v>
+      </c>
+      <c r="P70" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>275</v>
+      </c>
+      <c r="R70" t="s">
+        <v>276</v>
+      </c>
+      <c r="S70" s="9" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="71" spans="14:19" x14ac:dyDescent="0.2">
+      <c r="P71" t="s">
+        <v>251</v>
+      </c>
+      <c r="R71" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="72" spans="14:19" x14ac:dyDescent="0.2">
+      <c r="P72" t="s">
+        <v>253</v>
+      </c>
+      <c r="R72" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="73" spans="14:19" x14ac:dyDescent="0.2">
+      <c r="P73" s="14" t="s">
         <v>320</v>
       </c>
-      <c r="R53" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="70" spans="14:19" x14ac:dyDescent="0.3">
-      <c r="N70" t="s">
+    </row>
+    <row r="74" spans="14:19" x14ac:dyDescent="0.2">
+      <c r="P74" s="14"/>
+    </row>
+    <row r="77" spans="14:19" x14ac:dyDescent="0.2">
+      <c r="N77" t="s">
+        <v>280</v>
+      </c>
+      <c r="O77" t="s">
         <v>273</v>
       </c>
-      <c r="O70" t="s">
-        <v>274</v>
-      </c>
-      <c r="P70" t="s">
-        <v>275</v>
-      </c>
-      <c r="Q70" t="s">
-        <v>276</v>
-      </c>
-      <c r="R70" t="s">
-        <v>277</v>
-      </c>
-      <c r="S70" s="9" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="71" spans="14:19" x14ac:dyDescent="0.3">
-      <c r="P71" t="s">
-        <v>252</v>
-      </c>
-      <c r="R71" t="s">
+      <c r="P77" t="s">
+        <v>281</v>
+      </c>
+      <c r="Q77" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="85" spans="14:19" x14ac:dyDescent="0.2">
+      <c r="N85" t="s">
+        <v>283</v>
+      </c>
+      <c r="O85" t="s">
+        <v>284</v>
+      </c>
+      <c r="P85" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q85" t="s">
+        <v>285</v>
+      </c>
+      <c r="R85" t="s">
+        <v>286</v>
+      </c>
+      <c r="S85" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="86" spans="14:19" x14ac:dyDescent="0.2">
+      <c r="O86" t="s">
+        <v>288</v>
+      </c>
+      <c r="P86" t="s">
+        <v>289</v>
+      </c>
+      <c r="R86" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="87" spans="14:19" x14ac:dyDescent="0.2">
+      <c r="P87" t="s">
+        <v>253</v>
+      </c>
+      <c r="R87" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="88" spans="14:19" x14ac:dyDescent="0.2">
+      <c r="P88" t="s">
+        <v>292</v>
+      </c>
+      <c r="R88" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="89" spans="14:19" x14ac:dyDescent="0.2">
+      <c r="P89" s="15" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="90" spans="14:19" x14ac:dyDescent="0.2">
+      <c r="P90" s="15"/>
+    </row>
+    <row r="94" spans="14:19" x14ac:dyDescent="0.2">
+      <c r="N94" t="s">
+        <v>280</v>
+      </c>
+      <c r="O94" t="s">
+        <v>284</v>
+      </c>
+      <c r="P94" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="95" spans="14:19" x14ac:dyDescent="0.2">
+      <c r="O95" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="100" spans="14:19" x14ac:dyDescent="0.2">
+      <c r="N100" t="s">
+        <v>296</v>
+      </c>
+      <c r="O100" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q100" t="s">
+        <v>297</v>
+      </c>
+      <c r="R100" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="101" spans="14:19" x14ac:dyDescent="0.2">
+      <c r="N101" t="s">
+        <v>299</v>
+      </c>
+      <c r="O101" s="13" t="s">
+        <v>300</v>
+      </c>
+      <c r="P101" t="s">
+        <v>301</v>
+      </c>
+      <c r="Q101" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="102" spans="14:19" x14ac:dyDescent="0.2">
+      <c r="O102" s="13"/>
+    </row>
+    <row r="104" spans="14:19" x14ac:dyDescent="0.2">
+      <c r="N104" t="s">
+        <v>302</v>
+      </c>
+      <c r="O104" t="s">
+        <v>284</v>
+      </c>
+      <c r="P104" t="s">
+        <v>303</v>
+      </c>
+      <c r="R104" t="s">
+        <v>298</v>
+      </c>
+      <c r="S104" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="105" spans="14:19" x14ac:dyDescent="0.2">
+      <c r="O105" t="s">
+        <v>305</v>
+      </c>
+      <c r="R105" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="72" spans="14:19" x14ac:dyDescent="0.3">
-      <c r="P72" t="s">
-        <v>254</v>
-      </c>
-      <c r="R72" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="73" spans="14:19" x14ac:dyDescent="0.3">
-      <c r="P73" s="14" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="74" spans="14:19" x14ac:dyDescent="0.3">
-      <c r="P74" s="14"/>
-    </row>
-    <row r="77" spans="14:19" x14ac:dyDescent="0.3">
-      <c r="N77" t="s">
-        <v>281</v>
-      </c>
-      <c r="O77" t="s">
-        <v>274</v>
-      </c>
-      <c r="P77" t="s">
-        <v>282</v>
-      </c>
-      <c r="Q77" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="85" spans="14:19" x14ac:dyDescent="0.3">
-      <c r="N85" t="s">
+    <row r="106" spans="14:19" x14ac:dyDescent="0.2">
+      <c r="R106" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="107" spans="14:19" x14ac:dyDescent="0.2">
+      <c r="R107" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="109" spans="14:19" x14ac:dyDescent="0.2">
+      <c r="N109" t="s">
+        <v>308</v>
+      </c>
+      <c r="O109" t="s">
         <v>284</v>
       </c>
-      <c r="O85" t="s">
-        <v>285</v>
-      </c>
-      <c r="P85" t="s">
-        <v>249</v>
-      </c>
-      <c r="Q85" t="s">
+    </row>
+    <row r="110" spans="14:19" x14ac:dyDescent="0.2">
+      <c r="O110" t="s">
+        <v>305</v>
+      </c>
+      <c r="P110" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="116" spans="14:18" x14ac:dyDescent="0.2">
+      <c r="N116" t="s">
+        <v>206</v>
+      </c>
+      <c r="O116" t="s">
+        <v>284</v>
+      </c>
+      <c r="P116" t="s">
+        <v>310</v>
+      </c>
+      <c r="Q116" t="s">
+        <v>311</v>
+      </c>
+      <c r="R116" t="s">
         <v>286</v>
       </c>
-      <c r="R85" t="s">
-        <v>287</v>
-      </c>
-      <c r="S85" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="86" spans="14:19" x14ac:dyDescent="0.3">
-      <c r="O86" t="s">
-        <v>289</v>
-      </c>
-      <c r="P86" t="s">
-        <v>290</v>
-      </c>
-      <c r="R86" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="87" spans="14:19" x14ac:dyDescent="0.3">
-      <c r="P87" t="s">
-        <v>254</v>
-      </c>
-      <c r="R87" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="88" spans="14:19" x14ac:dyDescent="0.3">
-      <c r="P88" t="s">
-        <v>293</v>
-      </c>
-      <c r="R88" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="89" spans="14:19" x14ac:dyDescent="0.3">
-      <c r="P89" s="15" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="90" spans="14:19" x14ac:dyDescent="0.3">
-      <c r="P90" s="15"/>
-    </row>
-    <row r="94" spans="14:19" x14ac:dyDescent="0.3">
-      <c r="N94" t="s">
-        <v>281</v>
-      </c>
-      <c r="O94" t="s">
-        <v>285</v>
-      </c>
-      <c r="P94" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="95" spans="14:19" x14ac:dyDescent="0.3">
-      <c r="O95" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="100" spans="14:19" x14ac:dyDescent="0.3">
-      <c r="N100" t="s">
-        <v>297</v>
-      </c>
-      <c r="O100" t="s">
-        <v>285</v>
-      </c>
-      <c r="Q100" t="s">
-        <v>298</v>
-      </c>
-      <c r="R100" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="101" spans="14:19" x14ac:dyDescent="0.3">
-      <c r="N101" t="s">
-        <v>300</v>
-      </c>
-      <c r="O101" s="13" t="s">
-        <v>301</v>
-      </c>
-      <c r="P101" t="s">
-        <v>302</v>
-      </c>
-      <c r="Q101" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="102" spans="14:19" x14ac:dyDescent="0.3">
-      <c r="O102" s="13"/>
-    </row>
-    <row r="104" spans="14:19" x14ac:dyDescent="0.3">
-      <c r="N104" t="s">
-        <v>303</v>
-      </c>
-      <c r="O104" t="s">
-        <v>285</v>
-      </c>
-      <c r="P104" t="s">
-        <v>304</v>
-      </c>
-      <c r="R104" t="s">
-        <v>299</v>
-      </c>
-      <c r="S104" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="105" spans="14:19" x14ac:dyDescent="0.3">
-      <c r="O105" t="s">
-        <v>306</v>
-      </c>
-      <c r="R105" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="106" spans="14:19" x14ac:dyDescent="0.3">
-      <c r="R106" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="107" spans="14:19" x14ac:dyDescent="0.3">
-      <c r="R107" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="109" spans="14:19" x14ac:dyDescent="0.3">
-      <c r="N109" t="s">
-        <v>309</v>
-      </c>
-      <c r="O109" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="110" spans="14:19" x14ac:dyDescent="0.3">
-      <c r="O110" t="s">
-        <v>306</v>
-      </c>
-      <c r="P110" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="116" spans="14:18" x14ac:dyDescent="0.3">
-      <c r="N116" t="s">
-        <v>207</v>
-      </c>
-      <c r="O116" t="s">
-        <v>285</v>
-      </c>
-      <c r="P116" t="s">
-        <v>311</v>
-      </c>
-      <c r="Q116" t="s">
+    </row>
+    <row r="117" spans="14:18" x14ac:dyDescent="0.2">
+      <c r="O117" t="s">
         <v>312</v>
       </c>
-      <c r="R116" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="117" spans="14:18" x14ac:dyDescent="0.3">
-      <c r="O117" t="s">
+    </row>
+    <row r="122" spans="14:18" x14ac:dyDescent="0.2">
+      <c r="N122" t="s">
+        <v>202</v>
+      </c>
+      <c r="O122" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="122" spans="14:18" x14ac:dyDescent="0.3">
-      <c r="N122" t="s">
+      <c r="P122" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="123" spans="14:18" x14ac:dyDescent="0.2">
+      <c r="N123" t="s">
         <v>203</v>
       </c>
-      <c r="O122" t="s">
-        <v>314</v>
-      </c>
-      <c r="P122" t="s">
+      <c r="O123" t="s">
+        <v>313</v>
+      </c>
+      <c r="P123" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="123" spans="14:18" x14ac:dyDescent="0.3">
-      <c r="N123" t="s">
+    <row r="124" spans="14:18" x14ac:dyDescent="0.2">
+      <c r="N124" t="s">
         <v>204</v>
       </c>
-      <c r="O123" t="s">
-        <v>314</v>
-      </c>
-      <c r="P123" t="s">
+      <c r="O124" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="125" spans="14:18" x14ac:dyDescent="0.2">
+      <c r="N125" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="124" spans="14:18" x14ac:dyDescent="0.3">
-      <c r="N124" t="s">
-        <v>205</v>
-      </c>
-      <c r="O124" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="125" spans="14:18" x14ac:dyDescent="0.3">
-      <c r="N125" t="s">
+      <c r="O125" t="s">
         <v>317</v>
-      </c>
-      <c r="O125" t="s">
-        <v>318</v>
       </c>
     </row>
   </sheetData>
@@ -2087,17 +2096,17 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2105,15 +2114,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3">
         <v>0.7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -2124,9 +2133,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B5" s="1">
         <v>2</v>
@@ -2138,7 +2147,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -2152,7 +2161,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>45</v>
       </c>
@@ -2166,7 +2175,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>33</v>
       </c>
@@ -2193,17 +2202,17 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.5546875" customWidth="1"/>
+    <col min="1" max="1" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2214,23 +2223,23 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B4" s="1">
         <v>0.9</v>
@@ -2239,9 +2248,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B5" s="1">
         <v>0.8</v>
@@ -2250,34 +2259,34 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B6">
         <v>298.14999999999998</v>
       </c>
       <c r="C6" t="s">
+        <v>145</v>
+      </c>
+      <c r="D6" t="s">
         <v>146</v>
       </c>
-      <c r="D6" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>147</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>148</v>
       </c>
       <c r="B7">
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B8" s="1">
         <v>2</v>
@@ -2289,9 +2298,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B9">
         <v>353</v>
@@ -2300,20 +2309,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
@@ -2325,7 +2334,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
@@ -2339,7 +2348,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>45</v>
       </c>
@@ -2353,7 +2362,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>33</v>
       </c>
@@ -2367,37 +2376,37 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B15" s="1">
         <v>5000</v>
       </c>
       <c r="C15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D15" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B16">
         <v>0.8</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B17">
         <v>313.14999999999998</v>
       </c>
       <c r="D17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -2414,17 +2423,17 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.109375" customWidth="1"/>
+    <col min="1" max="1" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2438,7 +2447,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -2449,7 +2458,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -2460,7 +2469,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -2471,7 +2480,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -2483,7 +2492,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -2504,12 +2513,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.109375" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2523,54 +2532,54 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B3" s="1">
         <v>50</v>
       </c>
       <c r="C3" t="s">
+        <v>323</v>
+      </c>
+      <c r="D3" t="s">
         <v>324</v>
       </c>
-      <c r="D3" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B4">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>327</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>328</v>
       </c>
       <c r="B6">
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -2592,12 +2601,12 @@
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
+    <col min="1" max="1" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>69</v>
       </c>
@@ -2605,7 +2614,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2619,7 +2628,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -2633,7 +2642,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -2641,7 +2650,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -2655,7 +2664,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>77</v>
       </c>
@@ -2663,7 +2672,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>79</v>
       </c>
@@ -2671,7 +2680,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>81</v>
       </c>
@@ -2679,12 +2688,12 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>84</v>
       </c>
@@ -2695,7 +2704,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>85</v>
       </c>
@@ -2706,7 +2715,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>87</v>
       </c>
@@ -2717,7 +2726,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -2744,18 +2753,18 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.77734375" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" customWidth="1"/>
+    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2769,49 +2778,49 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B3">
         <f xml:space="preserve"> 1.5 * 10^(-3)</f>
         <v>1.5E-3</v>
       </c>
       <c r="C3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B4" s="1">
         <f>1*10^-3</f>
         <v>1E-3</v>
       </c>
       <c r="C4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B5" s="1">
         <f>1.5*10^-3</f>
         <v>1.5E-3</v>
       </c>
       <c r="C5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H5" t="s">
         <v>41</v>
@@ -2831,30 +2840,30 @@
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" customWidth="1"/>
+    <col min="5" max="5" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E2" t="s">
         <v>71</v>
       </c>
       <c r="F2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>99</v>
       </c>
@@ -2868,7 +2877,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>94</v>
       </c>
@@ -2882,7 +2891,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>43</v>
       </c>
@@ -2896,7 +2905,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>34</v>
       </c>
@@ -2910,10 +2919,10 @@
         <v>96</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -2930,9 +2939,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B8">
         <v>0.17</v>
@@ -2944,12 +2953,12 @@
         <v>96</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B9">
         <f>30/45</f>
@@ -2963,19 +2972,19 @@
         <v>96</v>
       </c>
       <c r="E9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
     </row>
   </sheetData>
@@ -2999,158 +3008,158 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C2" t="s">
         <v>229</v>
       </c>
-      <c r="C2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B3">
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="C3" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B4">
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C4" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B5">
         <v>0.1</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B6">
         <v>0.25</v>
       </c>
       <c r="C6" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B7">
         <v>0.02</v>
       </c>
       <c r="C7" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B8">
         <v>0.02</v>
       </c>
       <c r="C8" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B9">
         <v>0.22</v>
       </c>
       <c r="C9" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B10">
         <v>0.5</v>
       </c>
       <c r="C10" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B11">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="C11" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>224</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>225</v>
       </c>
       <c r="B12">
         <v>0.13500000000000001</v>
       </c>
       <c r="C12" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B13">
         <v>0.08</v>
       </c>
       <c r="C13" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>227</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>228</v>
       </c>
       <c r="B14">
         <v>5.7500000000000002E-2</v>
       </c>
       <c r="C14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -3166,12 +3175,12 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3179,15 +3188,15 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B3">
         <v>81890</v>
@@ -3196,59 +3205,59 @@
         <v>29</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>140</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>141</v>
       </c>
       <c r="B4" s="1">
         <v>45</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B6">
         <v>0.2</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B7">
         <v>0.2</v>
       </c>
       <c r="D7" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B8">
         <v>2.7E-2</v>
       </c>
       <c r="D8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -3265,28 +3274,28 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" customWidth="1"/>
+    <col min="1" max="1" width="26.5" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="8.6640625" customWidth="1"/>
-    <col min="4" max="4" width="19.109375" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" customWidth="1"/>
-    <col min="7" max="7" width="9.109375" customWidth="1"/>
+    <col min="4" max="4" width="19.1640625" customWidth="1"/>
+    <col min="5" max="5" width="8.5" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
     <col min="11" max="11" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3297,10 +3306,10 @@
         <v>49</v>
       </c>
       <c r="E2" t="s">
+        <v>331</v>
+      </c>
+      <c r="F2" t="s">
         <v>332</v>
-      </c>
-      <c r="F2" t="s">
-        <v>333</v>
       </c>
       <c r="G2" t="s">
         <v>7</v>
@@ -3315,9 +3324,9 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B3">
         <v>37500</v>
@@ -3344,9 +3353,9 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B4">
         <v>230000</v>
@@ -3373,9 +3382,9 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B5">
         <v>63000</v>
@@ -3402,9 +3411,9 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B6">
         <v>380000</v>
@@ -3425,9 +3434,9 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B7">
         <v>22000</v>
@@ -3436,7 +3445,7 @@
         <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E7">
         <v>1600</v>
@@ -3454,9 +3463,9 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B8">
         <v>37500</v>
@@ -3483,9 +3492,9 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B9">
         <v>230000</v>
@@ -3512,9 +3521,9 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B10">
         <v>75000</v>
@@ -3541,9 +3550,9 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B11">
         <v>100000</v>
@@ -3552,7 +3561,7 @@
         <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E11">
         <v>30</v>
@@ -3564,15 +3573,15 @@
         <v>48</v>
       </c>
       <c r="H11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I11">
         <v>0.67</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B12">
         <v>32.5</v>
@@ -3581,7 +3590,7 @@
         <v>29</v>
       </c>
       <c r="D12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -3593,15 +3602,15 @@
         <v>48</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I12">
         <v>0.95</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B13">
         <v>238000</v>
@@ -3610,7 +3619,7 @@
         <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E13">
         <v>10</v>
@@ -3622,15 +3631,15 @@
         <v>15</v>
       </c>
       <c r="H13" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I13">
         <v>0.65</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B14">
         <v>9500</v>
@@ -3657,9 +3666,9 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B15">
         <v>4800</v>
@@ -3686,9 +3695,9 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B16">
         <v>80</v>
@@ -3721,9 +3730,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B17">
         <v>21000</v>
@@ -3735,9 +3744,9 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>101</v>
+        <v>333</v>
       </c>
       <c r="B19">
         <v>650</v>
@@ -3746,7 +3755,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
     </row>
   </sheetData>
@@ -3772,17 +3781,17 @@
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="32.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3796,7 +3805,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -3804,7 +3813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -3815,7 +3824,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -3826,7 +3835,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -3834,7 +3843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -3842,7 +3851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -3850,7 +3859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -3864,9 +3873,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B11">
         <v>0.9</v>
@@ -3886,126 +3895,126 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.33203125" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="11.77734375" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C2" t="s">
         <v>229</v>
       </c>
-      <c r="C2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B3">
         <v>0.7</v>
       </c>
       <c r="C3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>209</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>210</v>
       </c>
       <c r="B4">
         <v>0.18</v>
       </c>
       <c r="C4" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B5">
         <v>0.1</v>
       </c>
       <c r="C5" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B6">
         <v>0.38</v>
       </c>
       <c r="C6" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B7">
         <v>0.4</v>
       </c>
       <c r="C7" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B8">
         <v>0.06</v>
       </c>
       <c r="C8" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B9">
         <v>0.1</v>
       </c>
       <c r="C9" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B10">
         <v>0.25</v>
       </c>
       <c r="C10" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>217</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>218</v>
       </c>
       <c r="B11">
         <v>0.2</v>
       </c>
       <c r="C11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -4021,18 +4030,18 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.21875" customWidth="1"/>
+    <col min="1" max="1" width="27.1640625" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -4046,15 +4055,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -4068,7 +4077,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -4082,7 +4091,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>42</v>
       </c>
@@ -4096,7 +4105,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
@@ -4110,7 +4119,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>45</v>
       </c>
@@ -4121,10 +4130,10 @@
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>33</v>
       </c>
@@ -4152,17 +4161,17 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4173,37 +4182,37 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B3">
         <v>35000</v>
       </c>
       <c r="C3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B4">
         <v>7920</v>
       </c>
       <c r="C4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B5">
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -4219,17 +4228,17 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4243,43 +4252,43 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3">
         <v>0.19400000000000001</v>
       </c>
       <c r="C3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>116</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>117</v>
       </c>
       <c r="B4">
         <v>1204.67</v>
       </c>
       <c r="C4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D5" t="s">
         <v>170</v>
-      </c>
-      <c r="D5" t="s">
-        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -4295,17 +4304,17 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.21875" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4319,9 +4328,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B3">
         <v>2.5</v>
@@ -4330,10 +4339,10 @@
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -4344,56 +4353,56 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B5">
         <v>0.9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B7">
         <v>8</v>
       </c>
       <c r="C7" t="s">
+        <v>130</v>
+      </c>
+      <c r="D7" t="s">
         <v>131</v>
       </c>
-      <c r="D7" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B8">
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -4409,17 +4418,17 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" customWidth="1"/>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4433,31 +4442,31 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B3">
         <v>1383.46</v>
       </c>
       <c r="C3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B4">
         <v>0.19400000000000001</v>
       </c>
       <c r="C4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B5">
         <v>69.17</v>
@@ -4466,37 +4475,37 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B6">
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>108</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>109</v>
       </c>
       <c r="B7">
         <v>50</v>
       </c>
       <c r="C7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" t="s">
         <v>110</v>
       </c>
-      <c r="D7" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>111</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>112</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -4515,17 +4524,17 @@
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4533,45 +4542,45 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B3">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B5">
         <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B6">
         <v>1.71</v>
       </c>
       <c r="C6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -4587,17 +4596,17 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" customWidth="1"/>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4608,7 +4617,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -4616,26 +4625,26 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B4">
         <v>174</v>
       </c>
       <c r="C4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5">
         <v>1.54</v>
       </c>
       <c r="C5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixing problems in LDH_plots and LDH_opex, changes to LDH_energy
</commit_message>
<xml_diff>
--- a/data/LDH_attributes.xlsx
+++ b/data/LDH_attributes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/Documents/University Work/summer work experience/Imperial College/FUSE/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chant\PycharmProjects\FUSE-V2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63DDCA66-8F36-3040-B892-7A2B08B04474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2FD848-7D3B-4CE5-967B-2BFE123482CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" firstSheet="12" activeTab="18" xr2:uid="{9D386D14-BB1A-49FB-A5CB-94A6FCCCA1F9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="10" activeTab="12" xr2:uid="{9D386D14-BB1A-49FB-A5CB-94A6FCCCA1F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Process overview" sheetId="23" r:id="rId1"/>
@@ -34,26 +34,17 @@
     <sheet name="equipment" sheetId="6" r:id="rId19"/>
     <sheet name="capex" sheetId="21" r:id="rId20"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="335">
   <si>
     <t>key</t>
   </si>
@@ -1108,6 +1099,9 @@
   </si>
   <si>
     <t>CEPCI_base</t>
+  </si>
+  <si>
+    <t>ft</t>
   </si>
 </sst>
 </file>
@@ -1280,22 +1274,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>472440</xdr:colOff>
-      <xdr:row>127</xdr:row>
-      <xdr:rowOff>100965</xdr:rowOff>
+      <xdr:colOff>1082040</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>5338</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86DC3DD0-C955-4405-98E9-858F7633F515}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3AB4C2F5-25E1-4947-BF52-84C9265C5400}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1317,8 +1311,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15240" y="129540"/>
-          <a:ext cx="7772400" cy="23197185"/>
+          <a:off x="0" y="0"/>
+          <a:ext cx="8641080" cy="23413978"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1629,21 +1623,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96F39DFA-2FDB-4EC9-BBFE-157F4FCC3560}">
   <dimension ref="N2:T125"/>
   <sheetViews>
-    <sheetView topLeftCell="K60" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="12" max="12" width="13.6640625" customWidth="1"/>
+    <col min="13" max="13" width="16.109375" customWidth="1"/>
     <col min="14" max="14" width="19" customWidth="1"/>
     <col min="15" max="15" width="27.6640625" customWidth="1"/>
-    <col min="16" max="16" width="34.1640625" customWidth="1"/>
+    <col min="16" max="16" width="34.109375" customWidth="1"/>
     <col min="17" max="17" width="19.6640625" customWidth="1"/>
-    <col min="18" max="18" width="28.83203125" customWidth="1"/>
-    <col min="19" max="19" width="62.5" customWidth="1"/>
+    <col min="18" max="18" width="28.77734375" customWidth="1"/>
+    <col min="19" max="19" width="62.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="14:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N2" s="4" t="s">
         <v>241</v>
       </c>
@@ -1663,7 +1659,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="12" spans="14:20" x14ac:dyDescent="0.2">
+    <row r="12" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N12" t="s">
         <v>247</v>
       </c>
@@ -1680,7 +1676,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="13" spans="14:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="14:20" x14ac:dyDescent="0.3">
       <c r="P13" t="s">
         <v>251</v>
       </c>
@@ -1688,7 +1684,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="14" spans="14:20" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="14:20" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="P14" t="s">
         <v>253</v>
       </c>
@@ -1698,7 +1694,7 @@
       </c>
       <c r="T14" s="6"/>
     </row>
-    <row r="15" spans="14:20" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="14:20" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="P15" s="14" t="s">
         <v>318</v>
       </c>
@@ -1706,7 +1702,7 @@
       <c r="S15" s="12"/>
       <c r="T15" s="6"/>
     </row>
-    <row r="16" spans="14:20" x14ac:dyDescent="0.2">
+    <row r="16" spans="14:20" x14ac:dyDescent="0.3">
       <c r="P16" s="14"/>
       <c r="R16" s="7"/>
       <c r="S16" s="8" t="s">
@@ -1714,7 +1710,7 @@
       </c>
       <c r="T16" s="7"/>
     </row>
-    <row r="19" spans="14:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="14:17" x14ac:dyDescent="0.3">
       <c r="N19" t="s">
         <v>256</v>
       </c>
@@ -1728,7 +1724,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="25" spans="14:17" x14ac:dyDescent="0.2">
+    <row r="25" spans="14:17" x14ac:dyDescent="0.3">
       <c r="N25" t="s">
         <v>196</v>
       </c>
@@ -1739,7 +1735,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="26" spans="14:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="14:17" x14ac:dyDescent="0.3">
       <c r="P26" t="s">
         <v>260</v>
       </c>
@@ -1747,7 +1743,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="39" spans="14:18" x14ac:dyDescent="0.2">
+    <row r="39" spans="14:18" x14ac:dyDescent="0.3">
       <c r="N39" t="s">
         <v>262</v>
       </c>
@@ -1764,21 +1760,21 @@
         <v>265</v>
       </c>
     </row>
-    <row r="40" spans="14:18" x14ac:dyDescent="0.2">
+    <row r="40" spans="14:18" x14ac:dyDescent="0.3">
       <c r="P40" s="15" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="41" spans="14:18" x14ac:dyDescent="0.2">
+    <row r="41" spans="14:18" x14ac:dyDescent="0.3">
       <c r="P41" s="15"/>
     </row>
-    <row r="42" spans="14:18" x14ac:dyDescent="0.2">
+    <row r="42" spans="14:18" x14ac:dyDescent="0.3">
       <c r="P42" s="10"/>
       <c r="R42" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="52" spans="14:18" x14ac:dyDescent="0.2">
+    <row r="52" spans="14:18" x14ac:dyDescent="0.3">
       <c r="N52" t="s">
         <v>267</v>
       </c>
@@ -1795,7 +1791,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="53" spans="14:18" x14ac:dyDescent="0.2">
+    <row r="53" spans="14:18" x14ac:dyDescent="0.3">
       <c r="P53" t="s">
         <v>319</v>
       </c>
@@ -1803,7 +1799,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="70" spans="14:19" x14ac:dyDescent="0.2">
+    <row r="70" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N70" t="s">
         <v>272</v>
       </c>
@@ -1823,7 +1819,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="71" spans="14:19" x14ac:dyDescent="0.2">
+    <row r="71" spans="14:19" x14ac:dyDescent="0.3">
       <c r="P71" t="s">
         <v>251</v>
       </c>
@@ -1831,7 +1827,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="72" spans="14:19" x14ac:dyDescent="0.2">
+    <row r="72" spans="14:19" x14ac:dyDescent="0.3">
       <c r="P72" t="s">
         <v>253</v>
       </c>
@@ -1839,15 +1835,15 @@
         <v>279</v>
       </c>
     </row>
-    <row r="73" spans="14:19" x14ac:dyDescent="0.2">
+    <row r="73" spans="14:19" x14ac:dyDescent="0.3">
       <c r="P73" s="14" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="74" spans="14:19" x14ac:dyDescent="0.2">
+    <row r="74" spans="14:19" x14ac:dyDescent="0.3">
       <c r="P74" s="14"/>
     </row>
-    <row r="77" spans="14:19" x14ac:dyDescent="0.2">
+    <row r="77" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N77" t="s">
         <v>280</v>
       </c>
@@ -1861,7 +1857,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="85" spans="14:19" x14ac:dyDescent="0.2">
+    <row r="85" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N85" t="s">
         <v>283</v>
       </c>
@@ -1881,7 +1877,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="86" spans="14:19" x14ac:dyDescent="0.2">
+    <row r="86" spans="14:19" x14ac:dyDescent="0.3">
       <c r="O86" t="s">
         <v>288</v>
       </c>
@@ -1892,7 +1888,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="87" spans="14:19" x14ac:dyDescent="0.2">
+    <row r="87" spans="14:19" x14ac:dyDescent="0.3">
       <c r="P87" t="s">
         <v>253</v>
       </c>
@@ -1900,7 +1896,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="88" spans="14:19" x14ac:dyDescent="0.2">
+    <row r="88" spans="14:19" x14ac:dyDescent="0.3">
       <c r="P88" t="s">
         <v>292</v>
       </c>
@@ -1908,15 +1904,15 @@
         <v>293</v>
       </c>
     </row>
-    <row r="89" spans="14:19" x14ac:dyDescent="0.2">
+    <row r="89" spans="14:19" x14ac:dyDescent="0.3">
       <c r="P89" s="15" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="90" spans="14:19" x14ac:dyDescent="0.2">
+    <row r="90" spans="14:19" x14ac:dyDescent="0.3">
       <c r="P90" s="15"/>
     </row>
-    <row r="94" spans="14:19" x14ac:dyDescent="0.2">
+    <row r="94" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N94" t="s">
         <v>280</v>
       </c>
@@ -1927,12 +1923,12 @@
         <v>294</v>
       </c>
     </row>
-    <row r="95" spans="14:19" x14ac:dyDescent="0.2">
+    <row r="95" spans="14:19" x14ac:dyDescent="0.3">
       <c r="O95" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="100" spans="14:19" x14ac:dyDescent="0.2">
+    <row r="100" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N100" t="s">
         <v>296</v>
       </c>
@@ -1946,7 +1942,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="101" spans="14:19" x14ac:dyDescent="0.2">
+    <row r="101" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N101" t="s">
         <v>299</v>
       </c>
@@ -1960,10 +1956,10 @@
         <v>297</v>
       </c>
     </row>
-    <row r="102" spans="14:19" x14ac:dyDescent="0.2">
+    <row r="102" spans="14:19" x14ac:dyDescent="0.3">
       <c r="O102" s="13"/>
     </row>
-    <row r="104" spans="14:19" x14ac:dyDescent="0.2">
+    <row r="104" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N104" t="s">
         <v>302</v>
       </c>
@@ -1980,7 +1976,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="105" spans="14:19" x14ac:dyDescent="0.2">
+    <row r="105" spans="14:19" x14ac:dyDescent="0.3">
       <c r="O105" t="s">
         <v>305</v>
       </c>
@@ -1988,17 +1984,17 @@
         <v>279</v>
       </c>
     </row>
-    <row r="106" spans="14:19" x14ac:dyDescent="0.2">
+    <row r="106" spans="14:19" x14ac:dyDescent="0.3">
       <c r="R106" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="107" spans="14:19" x14ac:dyDescent="0.2">
+    <row r="107" spans="14:19" x14ac:dyDescent="0.3">
       <c r="R107" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="109" spans="14:19" x14ac:dyDescent="0.2">
+    <row r="109" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N109" t="s">
         <v>308</v>
       </c>
@@ -2006,7 +2002,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="110" spans="14:19" x14ac:dyDescent="0.2">
+    <row r="110" spans="14:19" x14ac:dyDescent="0.3">
       <c r="O110" t="s">
         <v>305</v>
       </c>
@@ -2014,7 +2010,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="116" spans="14:18" x14ac:dyDescent="0.2">
+    <row r="116" spans="14:18" x14ac:dyDescent="0.3">
       <c r="N116" t="s">
         <v>206</v>
       </c>
@@ -2031,12 +2027,12 @@
         <v>286</v>
       </c>
     </row>
-    <row r="117" spans="14:18" x14ac:dyDescent="0.2">
+    <row r="117" spans="14:18" x14ac:dyDescent="0.3">
       <c r="O117" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="122" spans="14:18" x14ac:dyDescent="0.2">
+    <row r="122" spans="14:18" x14ac:dyDescent="0.3">
       <c r="N122" t="s">
         <v>202</v>
       </c>
@@ -2047,7 +2043,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="123" spans="14:18" x14ac:dyDescent="0.2">
+    <row r="123" spans="14:18" x14ac:dyDescent="0.3">
       <c r="N123" t="s">
         <v>203</v>
       </c>
@@ -2058,7 +2054,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="124" spans="14:18" x14ac:dyDescent="0.2">
+    <row r="124" spans="14:18" x14ac:dyDescent="0.3">
       <c r="N124" t="s">
         <v>204</v>
       </c>
@@ -2066,7 +2062,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="125" spans="14:18" x14ac:dyDescent="0.2">
+    <row r="125" spans="14:18" x14ac:dyDescent="0.3">
       <c r="N125" t="s">
         <v>316</v>
       </c>
@@ -2096,17 +2092,17 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2114,7 +2110,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>101</v>
       </c>
@@ -2122,7 +2118,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -2133,7 +2129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>154</v>
       </c>
@@ -2147,7 +2143,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -2161,7 +2157,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>45</v>
       </c>
@@ -2175,7 +2171,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>33</v>
       </c>
@@ -2202,17 +2198,17 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.5" customWidth="1"/>
+    <col min="1" max="1" width="27.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2226,7 +2222,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>155</v>
       </c>
@@ -2237,7 +2233,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>160</v>
       </c>
@@ -2248,7 +2244,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>161</v>
       </c>
@@ -2259,7 +2255,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>144</v>
       </c>
@@ -2273,7 +2269,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>147</v>
       </c>
@@ -2284,7 +2280,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>156</v>
       </c>
@@ -2298,7 +2294,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>142</v>
       </c>
@@ -2309,7 +2305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>149</v>
       </c>
@@ -2320,7 +2316,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>157</v>
       </c>
@@ -2334,7 +2330,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
@@ -2348,7 +2344,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>45</v>
       </c>
@@ -2362,7 +2358,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>33</v>
       </c>
@@ -2376,7 +2372,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>164</v>
       </c>
@@ -2390,7 +2386,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>162</v>
       </c>
@@ -2398,7 +2394,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>165</v>
       </c>
@@ -2423,17 +2419,17 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.1640625" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2447,7 +2443,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -2458,7 +2454,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -2469,7 +2465,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -2480,7 +2476,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -2492,7 +2488,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -2509,16 +2505,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39F5853C-7EBD-44C3-B44F-35BFE47CA7B2}">
   <dimension ref="A2:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.1640625" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2532,12 +2528,12 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>329</v>
       </c>
       <c r="B3" s="1">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="C3" t="s">
         <v>323</v>
@@ -2546,7 +2542,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>330</v>
       </c>
@@ -2554,10 +2550,10 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>325</v>
       </c>
@@ -2568,7 +2564,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>327</v>
       </c>
@@ -2579,7 +2575,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -2601,12 +2597,12 @@
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.83203125" customWidth="1"/>
+    <col min="1" max="1" width="19.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>69</v>
       </c>
@@ -2614,7 +2610,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2628,7 +2624,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -2642,7 +2638,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -2650,7 +2646,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -2664,7 +2660,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>77</v>
       </c>
@@ -2672,7 +2668,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>79</v>
       </c>
@@ -2680,7 +2676,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>81</v>
       </c>
@@ -2688,12 +2684,12 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>84</v>
       </c>
@@ -2704,7 +2700,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>85</v>
       </c>
@@ -2715,7 +2711,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>87</v>
       </c>
@@ -2726,7 +2722,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -2753,18 +2749,18 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" customWidth="1"/>
+    <col min="1" max="1" width="20.77734375" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2778,7 +2774,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>167</v>
       </c>
@@ -2793,7 +2789,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>173</v>
       </c>
@@ -2811,7 +2807,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>171</v>
       </c>
@@ -2840,13 +2836,13 @@
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="5" max="5" width="17.5" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2863,7 +2859,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>99</v>
       </c>
@@ -2877,7 +2873,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>94</v>
       </c>
@@ -2891,7 +2887,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>43</v>
       </c>
@@ -2905,7 +2901,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>34</v>
       </c>
@@ -2922,7 +2918,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -2939,7 +2935,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>175</v>
       </c>
@@ -2956,7 +2952,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>176</v>
       </c>
@@ -2978,13 +2974,13 @@
         <v>178</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
     </row>
   </sheetData>
@@ -3008,18 +3004,18 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3030,7 +3026,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>231</v>
       </c>
@@ -3041,7 +3037,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>232</v>
       </c>
@@ -3052,7 +3048,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>235</v>
       </c>
@@ -3063,7 +3059,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>236</v>
       </c>
@@ -3074,7 +3070,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>219</v>
       </c>
@@ -3085,7 +3081,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>220</v>
       </c>
@@ -3096,7 +3092,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>221</v>
       </c>
@@ -3107,7 +3103,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>238</v>
       </c>
@@ -3118,7 +3114,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>239</v>
       </c>
@@ -3129,7 +3125,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>224</v>
       </c>
@@ -3140,7 +3136,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>225</v>
       </c>
@@ -3151,7 +3147,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>227</v>
       </c>
@@ -3175,12 +3171,12 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3194,7 +3190,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>182</v>
       </c>
@@ -3208,7 +3204,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>140</v>
       </c>
@@ -3222,12 +3218,12 @@
         <v>141</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>183</v>
       </c>
@@ -3238,7 +3234,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>184</v>
       </c>
@@ -3249,7 +3245,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>230</v>
       </c>
@@ -3273,29 +3269,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0624EAC2-56E2-4337-8D5D-42EAA0559452}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.5" customWidth="1"/>
+    <col min="1" max="1" width="26.44140625" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="8.6640625" customWidth="1"/>
-    <col min="4" max="4" width="19.1640625" customWidth="1"/>
-    <col min="5" max="5" width="8.5" customWidth="1"/>
-    <col min="6" max="6" width="10.1640625" customWidth="1"/>
-    <col min="7" max="7" width="9.1640625" customWidth="1"/>
+    <col min="4" max="4" width="19.109375" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
     <col min="11" max="11" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3324,7 +3320,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>194</v>
       </c>
@@ -3353,7 +3349,7 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>195</v>
       </c>
@@ -3382,7 +3378,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>196</v>
       </c>
@@ -3411,7 +3407,7 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>192</v>
       </c>
@@ -3434,7 +3430,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>193</v>
       </c>
@@ -3463,7 +3459,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>197</v>
       </c>
@@ -3492,7 +3488,7 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>198</v>
       </c>
@@ -3521,7 +3517,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>199</v>
       </c>
@@ -3550,7 +3546,7 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>200</v>
       </c>
@@ -3579,7 +3575,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>201</v>
       </c>
@@ -3608,7 +3604,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>206</v>
       </c>
@@ -3637,7 +3633,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>202</v>
       </c>
@@ -3666,7 +3662,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>203</v>
       </c>
@@ -3695,7 +3691,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>204</v>
       </c>
@@ -3730,7 +3726,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>205</v>
       </c>
@@ -3744,7 +3740,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>333</v>
       </c>
@@ -3755,7 +3751,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
     </row>
   </sheetData>
@@ -3781,17 +3777,17 @@
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3805,7 +3801,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -3813,7 +3809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -3824,7 +3820,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -3835,7 +3831,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -3843,7 +3839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -3851,7 +3847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -3859,7 +3855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -3873,7 +3869,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>101</v>
       </c>
@@ -3895,19 +3891,19 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30.33203125" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3918,7 +3914,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>207</v>
       </c>
@@ -3929,7 +3925,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>209</v>
       </c>
@@ -3940,7 +3936,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>210</v>
       </c>
@@ -3951,7 +3947,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>211</v>
       </c>
@@ -3962,7 +3958,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>212</v>
       </c>
@@ -3973,7 +3969,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>213</v>
       </c>
@@ -3984,7 +3980,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>214</v>
       </c>
@@ -3995,7 +3991,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>215</v>
       </c>
@@ -4006,7 +4002,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>217</v>
       </c>
@@ -4030,18 +4026,18 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.1640625" customWidth="1"/>
+    <col min="1" max="1" width="27.109375" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -4055,7 +4051,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>114</v>
       </c>
@@ -4063,7 +4059,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -4077,7 +4073,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -4091,7 +4087,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>42</v>
       </c>
@@ -4105,7 +4101,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
@@ -4119,7 +4115,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>45</v>
       </c>
@@ -4133,7 +4129,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>33</v>
       </c>
@@ -4161,17 +4157,17 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4182,7 +4178,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>118</v>
       </c>
@@ -4193,7 +4189,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>159</v>
       </c>
@@ -4204,7 +4200,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>126</v>
       </c>
@@ -4228,17 +4224,17 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4252,7 +4248,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>122</v>
       </c>
@@ -4266,7 +4262,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -4277,7 +4273,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>168</v>
       </c>
@@ -4304,17 +4300,17 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4328,7 +4324,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>127</v>
       </c>
@@ -4342,7 +4338,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -4356,7 +4352,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>129</v>
       </c>
@@ -4364,12 +4360,12 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>132</v>
       </c>
@@ -4383,7 +4379,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>133</v>
       </c>
@@ -4394,7 +4390,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>134</v>
       </c>
@@ -4418,17 +4414,17 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5" customWidth="1"/>
+    <col min="1" max="1" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4442,7 +4438,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>103</v>
       </c>
@@ -4453,7 +4449,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>122</v>
       </c>
@@ -4464,7 +4460,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>105</v>
       </c>
@@ -4475,7 +4471,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>106</v>
       </c>
@@ -4489,7 +4485,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>108</v>
       </c>
@@ -4503,7 +4499,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>111</v>
       </c>
@@ -4524,17 +4520,17 @@
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" customWidth="1"/>
+    <col min="1" max="1" width="18.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4542,7 +4538,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>112</v>
       </c>
@@ -4553,7 +4549,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>113</v>
       </c>
@@ -4561,7 +4557,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>123</v>
       </c>
@@ -4572,7 +4568,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>124</v>
       </c>
@@ -4596,17 +4592,17 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5" customWidth="1"/>
+    <col min="1" max="1" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4617,7 +4613,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -4625,7 +4621,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>125</v>
       </c>
@@ -4636,7 +4632,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>124</v>
       </c>

</xml_diff>

<commit_message>
Implementation of SorbentSynthesis (partly taken from Sor_Syn_Chemicals, addition of definitions of methods, implementation of stirring energy for column washing, adjustments to give amounts of water required in l
</commit_message>
<xml_diff>
--- a/data/LDH_attributes.xlsx
+++ b/data/LDH_attributes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chant\PycharmProjects\FUSE-V2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2FD848-7D3B-4CE5-967B-2BFE123482CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0BE7DD8-659E-4C76-8357-27B8AA960536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="10" activeTab="12" xr2:uid="{9D386D14-BB1A-49FB-A5CB-94A6FCCCA1F9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="9" xr2:uid="{9D386D14-BB1A-49FB-A5CB-94A6FCCCA1F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Process overview" sheetId="23" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="335">
   <si>
     <t>key</t>
   </si>
@@ -142,9 +142,6 @@
     <t>mass_sorbent</t>
   </si>
   <si>
-    <t>kg/year</t>
-  </si>
-  <si>
     <t>surface_area</t>
   </si>
   <si>
@@ -355,13 +352,7 @@
     <t>Paranthaman 2017, Huang 2021</t>
   </si>
   <si>
-    <t>brine</t>
-  </si>
-  <si>
     <t>l</t>
-  </si>
-  <si>
-    <t>sorbent</t>
   </si>
   <si>
     <t>H2O_washing</t>
@@ -1102,6 +1093,15 @@
   </si>
   <si>
     <t>ft</t>
+  </si>
+  <si>
+    <t>Li 2018 (Lithium Recovery from Aqueous Resources and Batteries: A Brief Review)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">guess </t>
+  </si>
+  <si>
+    <t>tonnes/year</t>
   </si>
 </sst>
 </file>
@@ -1216,7 +1216,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -1251,6 +1251,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1623,7 +1625,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96F39DFA-2FDB-4EC9-BBFE-157F4FCC3560}">
   <dimension ref="N2:T125"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
@@ -1641,62 +1643,62 @@
   <sheetData>
     <row r="2" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N2" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="Q2" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="R2" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="S2" s="4" t="s">
         <v>243</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="12" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N12" t="s">
+        <v>244</v>
+      </c>
+      <c r="O12" t="s">
+        <v>111</v>
+      </c>
+      <c r="P12" t="s">
+        <v>245</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>246</v>
+      </c>
+      <c r="S12" t="s">
         <v>247</v>
-      </c>
-      <c r="O12" t="s">
-        <v>114</v>
-      </c>
-      <c r="P12" t="s">
-        <v>248</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>249</v>
-      </c>
-      <c r="S12" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="13" spans="14:20" x14ac:dyDescent="0.3">
       <c r="P13" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="S13" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="14" spans="14:20" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="P14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="R14" s="6"/>
       <c r="S14" s="11" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="T14" s="6"/>
     </row>
     <row r="15" spans="14:20" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="P15" s="14" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="R15" s="6"/>
       <c r="S15" s="12"/>
@@ -1706,63 +1708,63 @@
       <c r="P16" s="14"/>
       <c r="R16" s="7"/>
       <c r="S16" s="8" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="T16" s="7"/>
     </row>
     <row r="19" spans="14:17" x14ac:dyDescent="0.3">
       <c r="N19" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="O19" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="P19" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="Q19" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="25" spans="14:17" x14ac:dyDescent="0.3">
       <c r="N25" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="O25" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="P25" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="26" spans="14:17" x14ac:dyDescent="0.3">
       <c r="P26" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="Q26" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="39" spans="14:18" x14ac:dyDescent="0.3">
       <c r="N39" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="O39" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="P39" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="Q39">
         <v>12</v>
       </c>
       <c r="R39" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="40" spans="14:18" x14ac:dyDescent="0.3">
       <c r="P40" s="15" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="41" spans="14:18" x14ac:dyDescent="0.3">
@@ -1771,73 +1773,73 @@
     <row r="42" spans="14:18" x14ac:dyDescent="0.3">
       <c r="P42" s="10"/>
       <c r="R42" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="52" spans="14:18" x14ac:dyDescent="0.3">
       <c r="N52" t="s">
+        <v>264</v>
+      </c>
+      <c r="O52" t="s">
+        <v>260</v>
+      </c>
+      <c r="P52" t="s">
+        <v>265</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>266</v>
+      </c>
+      <c r="R52" t="s">
         <v>267</v>
-      </c>
-      <c r="O52" t="s">
-        <v>263</v>
-      </c>
-      <c r="P52" t="s">
-        <v>268</v>
-      </c>
-      <c r="Q52" t="s">
-        <v>269</v>
-      </c>
-      <c r="R52" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="53" spans="14:18" x14ac:dyDescent="0.3">
       <c r="P53" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="R53" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="70" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N70" t="s">
+        <v>269</v>
+      </c>
+      <c r="O70" t="s">
+        <v>270</v>
+      </c>
+      <c r="P70" t="s">
+        <v>271</v>
+      </c>
+      <c r="Q70" t="s">
         <v>272</v>
       </c>
-      <c r="O70" t="s">
+      <c r="R70" t="s">
         <v>273</v>
       </c>
-      <c r="P70" t="s">
+      <c r="S70" s="9" t="s">
         <v>274</v>
-      </c>
-      <c r="Q70" t="s">
-        <v>275</v>
-      </c>
-      <c r="R70" t="s">
-        <v>276</v>
-      </c>
-      <c r="S70" s="9" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="71" spans="14:19" x14ac:dyDescent="0.3">
       <c r="P71" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="R71" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="72" spans="14:19" x14ac:dyDescent="0.3">
       <c r="P72" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="R72" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="73" spans="14:19" x14ac:dyDescent="0.3">
       <c r="P73" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="74" spans="14:19" x14ac:dyDescent="0.3">
@@ -1845,68 +1847,68 @@
     </row>
     <row r="77" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N77" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="O77" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="P77" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="Q77" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="85" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N85" t="s">
+        <v>280</v>
+      </c>
+      <c r="O85" t="s">
+        <v>281</v>
+      </c>
+      <c r="P85" t="s">
+        <v>245</v>
+      </c>
+      <c r="Q85" t="s">
+        <v>282</v>
+      </c>
+      <c r="R85" t="s">
         <v>283</v>
       </c>
-      <c r="O85" t="s">
+      <c r="S85" t="s">
         <v>284</v>
-      </c>
-      <c r="P85" t="s">
-        <v>248</v>
-      </c>
-      <c r="Q85" t="s">
-        <v>285</v>
-      </c>
-      <c r="R85" t="s">
-        <v>286</v>
-      </c>
-      <c r="S85" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="86" spans="14:19" x14ac:dyDescent="0.3">
       <c r="O86" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="P86" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="R86" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="87" spans="14:19" x14ac:dyDescent="0.3">
       <c r="P87" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="R87" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="88" spans="14:19" x14ac:dyDescent="0.3">
       <c r="P88" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="R88" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="89" spans="14:19" x14ac:dyDescent="0.3">
       <c r="P89" s="15" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="90" spans="14:19" x14ac:dyDescent="0.3">
@@ -1914,46 +1916,46 @@
     </row>
     <row r="94" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N94" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="O94" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="P94" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="95" spans="14:19" x14ac:dyDescent="0.3">
       <c r="O95" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="100" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N100" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="O100" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="Q100" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="R100" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="101" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N101" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="O101" s="13" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="P101" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="Q101" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="102" spans="14:19" x14ac:dyDescent="0.3">
@@ -1961,113 +1963,113 @@
     </row>
     <row r="104" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N104" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="O104" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="P104" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="R104" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="S104" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="105" spans="14:19" x14ac:dyDescent="0.3">
       <c r="O105" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="R105" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="106" spans="14:19" x14ac:dyDescent="0.3">
       <c r="R106" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="107" spans="14:19" x14ac:dyDescent="0.3">
       <c r="R107" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="109" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N109" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="O109" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="110" spans="14:19" x14ac:dyDescent="0.3">
       <c r="O110" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="P110" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="116" spans="14:18" x14ac:dyDescent="0.3">
       <c r="N116" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="O116" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="P116" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="Q116" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="R116" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="117" spans="14:18" x14ac:dyDescent="0.3">
       <c r="O117" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="122" spans="14:18" x14ac:dyDescent="0.3">
       <c r="N122" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="O122" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="P122" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="123" spans="14:18" x14ac:dyDescent="0.3">
       <c r="N123" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="O123" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="P123" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="124" spans="14:18" x14ac:dyDescent="0.3">
       <c r="N124" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="O124" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="125" spans="14:18" x14ac:dyDescent="0.3">
       <c r="N125" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="O125" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -2088,7 +2090,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43797486-FEB5-4613-A524-BCA6B61EB1F2}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -2099,7 +2101,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -2112,7 +2114,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B3">
         <v>0.7</v>
@@ -2131,7 +2133,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B5" s="1">
         <v>2</v>
@@ -2140,7 +2142,7 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -2159,7 +2161,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7">
         <v>6.3499999999999997E-3</v>
@@ -2173,7 +2175,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8">
         <v>3.7160000000000002</v>
@@ -2182,7 +2184,7 @@
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2195,7 +2197,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2205,7 +2207,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -2219,70 +2221,70 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B4" s="1">
         <v>0.9</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B5" s="1">
         <v>0.8</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B6">
         <v>298.14999999999998</v>
       </c>
       <c r="C6" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D6" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B7">
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B8" s="1">
         <v>2</v>
@@ -2291,12 +2293,12 @@
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B9">
         <v>353</v>
@@ -2307,18 +2309,18 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
@@ -2327,7 +2329,7 @@
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -2346,7 +2348,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13">
         <v>6.3499999999999997E-3</v>
@@ -2360,7 +2362,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14">
         <v>3.7160000000000002</v>
@@ -2369,26 +2371,26 @@
         <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B15" s="1">
         <v>5000</v>
       </c>
       <c r="C15" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D15" t="s">
-        <v>41</v>
+        <v>333</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B16">
         <v>0.8</v>
@@ -2396,13 +2398,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B17">
         <v>313.14999999999998</v>
       </c>
       <c r="D17" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -2490,7 +2492,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7">
         <v>0.9</v>
@@ -2505,8 +2507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39F5853C-7EBD-44C3-B44F-35BFE47CA7B2}">
   <dimension ref="A2:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2525,59 +2527,59 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>329</v>
-      </c>
-      <c r="B3" s="1">
+        <v>326</v>
+      </c>
+      <c r="B3" s="16">
         <v>100</v>
       </c>
       <c r="C3" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D3" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>330</v>
-      </c>
-      <c r="B4">
-        <v>5</v>
+        <v>327</v>
+      </c>
+      <c r="B4" s="17">
+        <v>200</v>
       </c>
       <c r="C4" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B6">
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7">
         <v>0.8</v>
@@ -2604,7 +2606,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B1">
         <v>2016</v>
@@ -2621,12 +2623,12 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -2635,63 +2637,63 @@
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" t="s">
         <v>73</v>
-      </c>
-      <c r="D4" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" t="s">
         <v>77</v>
-      </c>
-      <c r="D6" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" t="s">
         <v>79</v>
-      </c>
-      <c r="D7" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" t="s">
         <v>81</v>
-      </c>
-      <c r="D8" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B10">
         <v>30</v>
@@ -2702,7 +2704,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B11">
         <v>0.2</v>
@@ -2713,13 +2715,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B12">
         <v>0.75</v>
       </c>
       <c r="D12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -2730,10 +2732,10 @@
         <v>9.81</v>
       </c>
       <c r="C13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -2771,55 +2773,55 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B3">
         <f xml:space="preserve"> 1.5 * 10^(-3)</f>
         <v>1.5E-3</v>
       </c>
       <c r="C3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B4" s="1">
         <f>1*10^-3</f>
         <v>1E-3</v>
       </c>
       <c r="C4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D4" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B5" s="1">
         <f>1.5*10^-3</f>
         <v>1.5E-3</v>
       </c>
       <c r="C5" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -2847,63 +2849,63 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B3">
         <v>6.6600000000000006E-2</v>
       </c>
       <c r="D3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B4">
         <v>0.01</v>
       </c>
       <c r="D4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5">
         <v>20</v>
       </c>
       <c r="D5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6">
         <v>0.51</v>
@@ -2912,15 +2914,15 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="D6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7">
         <v>0.15</v>
@@ -2929,15 +2931,15 @@
         <v>0.45</v>
       </c>
       <c r="D7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B8">
         <v>0.17</v>
@@ -2946,15 +2948,15 @@
         <v>0.24</v>
       </c>
       <c r="D8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B9">
         <f>30/45</f>
@@ -2965,13 +2967,13 @@
         <v>4.2222222222222223</v>
       </c>
       <c r="D9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E9" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -3012,7 +3014,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -3020,142 +3022,142 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B3">
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="C3" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B4">
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C4" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B5">
         <v>0.1</v>
       </c>
       <c r="C5" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B6">
         <v>0.25</v>
       </c>
       <c r="C6" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B7">
         <v>0.02</v>
       </c>
       <c r="C7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B8">
         <v>0.02</v>
       </c>
       <c r="C8" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B9">
         <v>0.22</v>
       </c>
       <c r="C9" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B10">
         <v>0.5</v>
       </c>
       <c r="C10" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B11">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="C11" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B12">
         <v>0.13500000000000001</v>
       </c>
       <c r="C12" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B13">
         <v>0.08</v>
       </c>
       <c r="C13" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B14">
         <v>5.7500000000000002E-2</v>
       </c>
       <c r="C14" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -3168,7 +3170,7 @@
   <dimension ref="A2:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3184,7 +3186,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -3192,7 +3194,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B3">
         <v>81890</v>
@@ -3201,59 +3203,59 @@
         <v>29</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>140</v>
-      </c>
-      <c r="B4" s="1">
+        <v>137</v>
+      </c>
+      <c r="B4" s="3">
         <v>45</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="H4" t="s">
         <v>138</v>
-      </c>
-      <c r="H4" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B6">
         <v>0.2</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B7">
         <v>0.2</v>
       </c>
       <c r="D7" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B8">
         <v>2.7E-2</v>
       </c>
       <c r="D8" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -3288,7 +3290,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -3299,30 +3301,30 @@
         <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E2" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="F2" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="G2" t="s">
         <v>7</v>
       </c>
       <c r="H2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I2" t="s">
         <v>30</v>
       </c>
       <c r="J2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B3">
         <v>37500</v>
@@ -3331,7 +3333,7 @@
         <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E3">
         <v>3</v>
@@ -3340,10 +3342,10 @@
         <v>0.5</v>
       </c>
       <c r="G3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I3">
         <v>0.53</v>
@@ -3351,7 +3353,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B4">
         <v>230000</v>
@@ -3360,7 +3362,7 @@
         <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E4">
         <v>150</v>
@@ -3372,7 +3374,7 @@
         <v>15</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I4">
         <v>0.6</v>
@@ -3380,7 +3382,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B5">
         <v>63000</v>
@@ -3389,7 +3391,7 @@
         <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E5">
         <v>15</v>
@@ -3398,10 +3400,10 @@
         <v>4</v>
       </c>
       <c r="G5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I5">
         <v>0.81</v>
@@ -3409,7 +3411,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B6">
         <v>380000</v>
@@ -3424,7 +3426,7 @@
         <v>12</v>
       </c>
       <c r="H6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I6">
         <v>0.66</v>
@@ -3432,7 +3434,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B7">
         <v>22000</v>
@@ -3441,7 +3443,7 @@
         <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E7">
         <v>1600</v>
@@ -3453,7 +3455,7 @@
         <v>15</v>
       </c>
       <c r="H7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I7">
         <v>0.85</v>
@@ -3461,7 +3463,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B8">
         <v>37500</v>
@@ -3470,7 +3472,7 @@
         <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E8">
         <v>3</v>
@@ -3479,10 +3481,10 @@
         <v>5</v>
       </c>
       <c r="G8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I8">
         <v>0.53</v>
@@ -3490,7 +3492,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B9">
         <v>230000</v>
@@ -3499,7 +3501,7 @@
         <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E9">
         <v>150</v>
@@ -3511,7 +3513,7 @@
         <v>15</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I9">
         <v>0.6</v>
@@ -3519,7 +3521,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B10">
         <v>75000</v>
@@ -3528,7 +3530,7 @@
         <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E10">
         <v>3</v>
@@ -3537,10 +3539,10 @@
         <v>5</v>
       </c>
       <c r="G10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I10">
         <v>0.53</v>
@@ -3548,7 +3550,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B11">
         <v>100000</v>
@@ -3557,7 +3559,7 @@
         <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E11">
         <v>30</v>
@@ -3566,10 +3568,10 @@
         <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H11" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="I11">
         <v>0.67</v>
@@ -3577,7 +3579,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B12">
         <v>32.5</v>
@@ -3586,7 +3588,7 @@
         <v>29</v>
       </c>
       <c r="D12" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -3595,10 +3597,10 @@
         <v>10</v>
       </c>
       <c r="G12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="I12">
         <v>0.95</v>
@@ -3606,7 +3608,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B13">
         <v>238000</v>
@@ -3615,7 +3617,7 @@
         <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E13">
         <v>10</v>
@@ -3627,7 +3629,7 @@
         <v>15</v>
       </c>
       <c r="H13" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="I13">
         <v>0.65</v>
@@ -3635,7 +3637,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B14">
         <v>9500</v>
@@ -3644,7 +3646,7 @@
         <v>29</v>
       </c>
       <c r="D14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E14">
         <v>23</v>
@@ -3653,10 +3655,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="G14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I14">
         <v>0.79</v>
@@ -3664,7 +3666,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B15">
         <v>4800</v>
@@ -3673,7 +3675,7 @@
         <v>29</v>
       </c>
       <c r="D15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E15">
         <v>7.5</v>
@@ -3682,10 +3684,10 @@
         <v>2.54</v>
       </c>
       <c r="G15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I15">
         <v>0.65</v>
@@ -3693,16 +3695,16 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B16">
         <v>80</v>
       </c>
       <c r="C16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E16">
         <v>15</v>
@@ -3711,10 +3713,10 @@
         <v>20</v>
       </c>
       <c r="G16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I16">
         <v>1.33</v>
@@ -3728,7 +3730,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B17">
         <v>21000</v>
@@ -3742,13 +3744,13 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="B19">
         <v>650</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
@@ -3774,17 +3776,18 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -3803,7 +3806,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3811,7 +3814,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -3822,7 +3825,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5">
         <v>0.7</v>
@@ -3833,7 +3836,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3841,7 +3844,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3849,7 +3852,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3859,19 +3862,19 @@
       <c r="A10" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="1">
-        <v>50</v>
+      <c r="B10" s="3">
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>334</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>332</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B11">
         <v>0.9</v>
@@ -3900,7 +3903,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -3908,109 +3911,109 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B3">
         <v>0.7</v>
       </c>
       <c r="C3" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B4">
         <v>0.18</v>
       </c>
       <c r="C4" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B5">
         <v>0.1</v>
       </c>
       <c r="C5" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B6">
         <v>0.38</v>
       </c>
       <c r="C6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B7">
         <v>0.4</v>
       </c>
       <c r="C7" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B8">
         <v>0.06</v>
       </c>
       <c r="C8" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B9">
         <v>0.1</v>
       </c>
       <c r="C9" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B10">
         <v>0.25</v>
       </c>
       <c r="C10" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B11">
         <v>0.2</v>
       </c>
       <c r="C11" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -4034,7 +4037,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -4053,10 +4056,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -4089,7 +4092,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -4117,7 +4120,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8">
         <v>6.3499999999999997E-3</v>
@@ -4126,12 +4129,12 @@
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9">
         <v>3.7160000000000002</v>
@@ -4140,7 +4143,7 @@
         <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -4164,7 +4167,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -4180,35 +4183,35 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B3">
         <v>35000</v>
       </c>
       <c r="C3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B4">
         <v>7920</v>
       </c>
       <c r="C4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B5">
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -4231,7 +4234,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -4250,41 +4253,41 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B3">
         <v>0.19400000000000001</v>
       </c>
       <c r="C3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B4">
         <v>1204.67</v>
       </c>
       <c r="C4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -4307,7 +4310,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -4326,7 +4329,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B3">
         <v>2.5</v>
@@ -4335,12 +4338,12 @@
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4">
         <v>0.1</v>
@@ -4349,12 +4352,12 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B5">
         <v>0.9</v>
@@ -4362,43 +4365,43 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B7">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D7" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B8">
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -4408,10 +4411,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{057E51FA-16AA-4EDB-95D7-E76738AA23C5}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4421,7 +4424,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -4435,29 +4438,32 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="B3">
-        <v>1383.46</v>
+        <v>0.19400000000000001</v>
       </c>
       <c r="C3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="B4">
-        <v>0.19400000000000001</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>109</v>
+        <v>102</v>
+      </c>
+      <c r="D4" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -4465,46 +4471,35 @@
         <v>105</v>
       </c>
       <c r="B5">
-        <v>69.17</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>106</v>
+      </c>
+      <c r="D5" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B6">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>104</v>
-      </c>
-      <c r="D6" t="s">
-        <v>107</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>108</v>
-      </c>
-      <c r="B7">
-        <v>50</v>
+        <v>20</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.5</v>
       </c>
       <c r="C7" t="s">
-        <v>109</v>
+        <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>111</v>
-      </c>
-      <c r="B8">
-        <v>4</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -4527,7 +4522,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -4540,18 +4535,18 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B3">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -4559,24 +4554,24 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B5">
         <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B6">
         <v>1.71</v>
       </c>
       <c r="C6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -4599,7 +4594,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -4615,7 +4610,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3">
         <v>0.9</v>
@@ -4623,24 +4618,24 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B4">
         <v>174</v>
       </c>
       <c r="C4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B5">
         <v>1.54</v>
       </c>
       <c r="C5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implementation of Belt conveyor in Equipment and LDH_capex; changes to plot to get energy in kWh/tonnes
</commit_message>
<xml_diff>
--- a/data/LDH_attributes.xlsx
+++ b/data/LDH_attributes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chant\PycharmProjects\FUSE-V2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0BE7DD8-659E-4C76-8357-27B8AA960536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A58A07F8-3A9E-41C6-A2FD-9AD582ACE822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="9" xr2:uid="{9D386D14-BB1A-49FB-A5CB-94A6FCCCA1F9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="11" activeTab="18" xr2:uid="{9D386D14-BB1A-49FB-A5CB-94A6FCCCA1F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Process overview" sheetId="23" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="337">
   <si>
     <t>key</t>
   </si>
@@ -1102,6 +1102,12 @@
   </si>
   <si>
     <t>tonnes/year</t>
+  </si>
+  <si>
+    <t>solid capacity * (length)^2.5</t>
+  </si>
+  <si>
+    <t>(t*m^2.5)/h</t>
   </si>
 </sst>
 </file>
@@ -1236,6 +1242,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1251,8 +1259,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1691,21 +1697,21 @@
         <v>250</v>
       </c>
       <c r="R14" s="6"/>
-      <c r="S14" s="11" t="s">
+      <c r="S14" s="13" t="s">
         <v>251</v>
       </c>
       <c r="T14" s="6"/>
     </row>
     <row r="15" spans="14:20" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="P15" s="14" t="s">
+      <c r="P15" s="16" t="s">
         <v>315</v>
       </c>
       <c r="R15" s="6"/>
-      <c r="S15" s="12"/>
+      <c r="S15" s="14"/>
       <c r="T15" s="6"/>
     </row>
     <row r="16" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="P16" s="14"/>
+      <c r="P16" s="16"/>
       <c r="R16" s="7"/>
       <c r="S16" s="8" t="s">
         <v>252</v>
@@ -1763,12 +1769,12 @@
       </c>
     </row>
     <row r="40" spans="14:18" x14ac:dyDescent="0.3">
-      <c r="P40" s="15" t="s">
+      <c r="P40" s="17" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="41" spans="14:18" x14ac:dyDescent="0.3">
-      <c r="P41" s="15"/>
+      <c r="P41" s="17"/>
     </row>
     <row r="42" spans="14:18" x14ac:dyDescent="0.3">
       <c r="P42" s="10"/>
@@ -1838,12 +1844,12 @@
       </c>
     </row>
     <row r="73" spans="14:19" x14ac:dyDescent="0.3">
-      <c r="P73" s="14" t="s">
+      <c r="P73" s="16" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="74" spans="14:19" x14ac:dyDescent="0.3">
-      <c r="P74" s="14"/>
+      <c r="P74" s="16"/>
     </row>
     <row r="77" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N77" t="s">
@@ -1907,12 +1913,12 @@
       </c>
     </row>
     <row r="89" spans="14:19" x14ac:dyDescent="0.3">
-      <c r="P89" s="15" t="s">
+      <c r="P89" s="17" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="90" spans="14:19" x14ac:dyDescent="0.3">
-      <c r="P90" s="15"/>
+      <c r="P90" s="17"/>
     </row>
     <row r="94" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N94" t="s">
@@ -1948,7 +1954,7 @@
       <c r="N101" t="s">
         <v>296</v>
       </c>
-      <c r="O101" s="13" t="s">
+      <c r="O101" s="15" t="s">
         <v>297</v>
       </c>
       <c r="P101" t="s">
@@ -1959,7 +1965,7 @@
       </c>
     </row>
     <row r="102" spans="14:19" x14ac:dyDescent="0.3">
-      <c r="O102" s="13"/>
+      <c r="O102" s="15"/>
     </row>
     <row r="104" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N104" t="s">
@@ -2090,7 +2096,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43797486-FEB5-4613-A524-BCA6B61EB1F2}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -2534,7 +2540,7 @@
       <c r="A3" t="s">
         <v>326</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3" s="11">
         <v>100</v>
       </c>
       <c r="C3" t="s">
@@ -2548,7 +2554,7 @@
       <c r="A4" t="s">
         <v>327</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="12">
         <v>200</v>
       </c>
       <c r="C4" t="s">
@@ -3271,8 +3277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0624EAC2-56E2-4337-8D5D-42EAA0559452}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3280,7 +3286,7 @@
     <col min="1" max="1" width="26.44140625" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="8.6640625" customWidth="1"/>
-    <col min="4" max="4" width="19.109375" customWidth="1"/>
+    <col min="4" max="4" width="25.44140625" customWidth="1"/>
     <col min="5" max="5" width="8.44140625" customWidth="1"/>
     <col min="6" max="6" width="10.109375" customWidth="1"/>
     <col min="7" max="7" width="9.109375" customWidth="1"/>
@@ -3623,7 +3629,7 @@
         <v>10</v>
       </c>
       <c r="F13">
-        <v>60</v>
+        <v>8</v>
       </c>
       <c r="G13" t="s">
         <v>15</v>
@@ -3737,6 +3743,20 @@
       </c>
       <c r="C17" t="s">
         <v>29</v>
+      </c>
+      <c r="D17" t="s">
+        <v>335</v>
+      </c>
+      <c r="E17">
+        <f>10^6</f>
+        <v>1000000</v>
+      </c>
+      <c r="F17">
+        <f>(standard_belt_conveyor!B6*(standard_belt_conveyor!B4*0.3048)^2.5)</f>
+        <v>435214.799238206</v>
+      </c>
+      <c r="G17" t="s">
+        <v>336</v>
       </c>
       <c r="I17">
         <v>0.2</v>

</xml_diff>

<commit_message>
correction of units of Li2CO3, implementation of belt conveyor to LDH energy
</commit_message>
<xml_diff>
--- a/data/LDH_attributes.xlsx
+++ b/data/LDH_attributes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chant\PycharmProjects\FUSE-V2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A58A07F8-3A9E-41C6-A2FD-9AD582ACE822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F4A90FB-A27F-4678-AE41-B1CF1C764BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="11" activeTab="18" xr2:uid="{9D386D14-BB1A-49FB-A5CB-94A6FCCCA1F9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{9D386D14-BB1A-49FB-A5CB-94A6FCCCA1F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Process overview" sheetId="23" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="336">
   <si>
     <t>key</t>
   </si>
@@ -551,9 +551,6 @@
   </si>
   <si>
     <t>LC_purification_washing</t>
-  </si>
-  <si>
-    <t>bring reactants in aqueous solution</t>
   </si>
   <si>
     <t>LC_processing_aq</t>
@@ -1092,9 +1089,6 @@
     <t>CEPCI_base</t>
   </si>
   <si>
-    <t>ft</t>
-  </si>
-  <si>
     <t>Li 2018 (Lithium Recovery from Aqueous Resources and Batteries: A Brief Review)</t>
   </si>
   <si>
@@ -1108,6 +1102,9 @@
   </si>
   <si>
     <t>(t*m^2.5)/h</t>
+  </si>
+  <si>
+    <t>20 wt% soda ash sol (Ehren, Patent no: WO 2013/036983 Al)</t>
   </si>
 </sst>
 </file>
@@ -1649,62 +1646,62 @@
   <sheetData>
     <row r="2" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N2" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="O2" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="Q2" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="R2" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="S2" s="4" t="s">
         <v>242</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="12" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O12" t="s">
         <v>111</v>
       </c>
       <c r="P12" t="s">
+        <v>244</v>
+      </c>
+      <c r="Q12" t="s">
         <v>245</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="S12" t="s">
         <v>246</v>
-      </c>
-      <c r="S12" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="13" spans="14:20" x14ac:dyDescent="0.3">
       <c r="P13" t="s">
+        <v>247</v>
+      </c>
+      <c r="S13" t="s">
         <v>248</v>
-      </c>
-      <c r="S13" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="14" spans="14:20" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="P14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="R14" s="6"/>
       <c r="S14" s="13" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="T14" s="6"/>
     </row>
     <row r="15" spans="14:20" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="P15" s="16" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="R15" s="6"/>
       <c r="S15" s="14"/>
@@ -1714,63 +1711,63 @@
       <c r="P16" s="16"/>
       <c r="R16" s="7"/>
       <c r="S16" s="8" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="T16" s="7"/>
     </row>
     <row r="19" spans="14:17" x14ac:dyDescent="0.3">
       <c r="N19" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O19" t="s">
         <v>111</v>
       </c>
       <c r="P19" t="s">
+        <v>253</v>
+      </c>
+      <c r="Q19" t="s">
         <v>254</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="25" spans="14:17" x14ac:dyDescent="0.3">
       <c r="N25" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O25" t="s">
         <v>111</v>
       </c>
       <c r="P25" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="26" spans="14:17" x14ac:dyDescent="0.3">
       <c r="P26" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q26" t="s">
         <v>257</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="39" spans="14:18" x14ac:dyDescent="0.3">
       <c r="N39" t="s">
+        <v>258</v>
+      </c>
+      <c r="O39" t="s">
         <v>259</v>
       </c>
-      <c r="O39" t="s">
+      <c r="P39" t="s">
         <v>260</v>
-      </c>
-      <c r="P39" t="s">
-        <v>261</v>
       </c>
       <c r="Q39">
         <v>12</v>
       </c>
       <c r="R39" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="40" spans="14:18" x14ac:dyDescent="0.3">
       <c r="P40" s="17" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="41" spans="14:18" x14ac:dyDescent="0.3">
@@ -1779,73 +1776,73 @@
     <row r="42" spans="14:18" x14ac:dyDescent="0.3">
       <c r="P42" s="10"/>
       <c r="R42" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="52" spans="14:18" x14ac:dyDescent="0.3">
       <c r="N52" t="s">
+        <v>263</v>
+      </c>
+      <c r="O52" t="s">
+        <v>259</v>
+      </c>
+      <c r="P52" t="s">
         <v>264</v>
       </c>
-      <c r="O52" t="s">
-        <v>260</v>
-      </c>
-      <c r="P52" t="s">
+      <c r="Q52" t="s">
         <v>265</v>
       </c>
-      <c r="Q52" t="s">
+      <c r="R52" t="s">
         <v>266</v>
-      </c>
-      <c r="R52" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="53" spans="14:18" x14ac:dyDescent="0.3">
       <c r="P53" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="R53" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="70" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N70" t="s">
+        <v>268</v>
+      </c>
+      <c r="O70" t="s">
         <v>269</v>
       </c>
-      <c r="O70" t="s">
+      <c r="P70" t="s">
         <v>270</v>
       </c>
-      <c r="P70" t="s">
+      <c r="Q70" t="s">
         <v>271</v>
       </c>
-      <c r="Q70" t="s">
+      <c r="R70" t="s">
         <v>272</v>
       </c>
-      <c r="R70" t="s">
+      <c r="S70" s="9" t="s">
         <v>273</v>
-      </c>
-      <c r="S70" s="9" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="71" spans="14:19" x14ac:dyDescent="0.3">
       <c r="P71" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="R71" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="72" spans="14:19" x14ac:dyDescent="0.3">
       <c r="P72" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="R72" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="73" spans="14:19" x14ac:dyDescent="0.3">
       <c r="P73" s="16" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="74" spans="14:19" x14ac:dyDescent="0.3">
@@ -1853,68 +1850,68 @@
     </row>
     <row r="77" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N77" t="s">
+        <v>276</v>
+      </c>
+      <c r="O77" t="s">
+        <v>269</v>
+      </c>
+      <c r="P77" t="s">
         <v>277</v>
       </c>
-      <c r="O77" t="s">
-        <v>270</v>
-      </c>
-      <c r="P77" t="s">
+      <c r="Q77" t="s">
         <v>278</v>
-      </c>
-      <c r="Q77" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="85" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N85" t="s">
+        <v>279</v>
+      </c>
+      <c r="O85" t="s">
         <v>280</v>
       </c>
-      <c r="O85" t="s">
+      <c r="P85" t="s">
+        <v>244</v>
+      </c>
+      <c r="Q85" t="s">
         <v>281</v>
       </c>
-      <c r="P85" t="s">
-        <v>245</v>
-      </c>
-      <c r="Q85" t="s">
+      <c r="R85" t="s">
         <v>282</v>
       </c>
-      <c r="R85" t="s">
+      <c r="S85" t="s">
         <v>283</v>
-      </c>
-      <c r="S85" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="86" spans="14:19" x14ac:dyDescent="0.3">
       <c r="O86" t="s">
+        <v>284</v>
+      </c>
+      <c r="P86" t="s">
         <v>285</v>
       </c>
-      <c r="P86" t="s">
+      <c r="R86" t="s">
         <v>286</v>
-      </c>
-      <c r="R86" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="87" spans="14:19" x14ac:dyDescent="0.3">
       <c r="P87" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="R87" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="88" spans="14:19" x14ac:dyDescent="0.3">
       <c r="P88" t="s">
+        <v>288</v>
+      </c>
+      <c r="R88" t="s">
         <v>289</v>
-      </c>
-      <c r="R88" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="89" spans="14:19" x14ac:dyDescent="0.3">
       <c r="P89" s="17" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="90" spans="14:19" x14ac:dyDescent="0.3">
@@ -1922,46 +1919,46 @@
     </row>
     <row r="94" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N94" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="O94" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="P94" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="95" spans="14:19" x14ac:dyDescent="0.3">
       <c r="O95" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="100" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N100" t="s">
+        <v>292</v>
+      </c>
+      <c r="O100" t="s">
+        <v>280</v>
+      </c>
+      <c r="Q100" t="s">
         <v>293</v>
       </c>
-      <c r="O100" t="s">
-        <v>281</v>
-      </c>
-      <c r="Q100" t="s">
+      <c r="R100" t="s">
         <v>294</v>
-      </c>
-      <c r="R100" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="101" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N101" t="s">
+        <v>295</v>
+      </c>
+      <c r="O101" s="15" t="s">
         <v>296</v>
       </c>
-      <c r="O101" s="15" t="s">
+      <c r="P101" t="s">
         <v>297</v>
       </c>
-      <c r="P101" t="s">
-        <v>298</v>
-      </c>
       <c r="Q101" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="102" spans="14:19" x14ac:dyDescent="0.3">
@@ -1969,113 +1966,113 @@
     </row>
     <row r="104" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N104" t="s">
+        <v>298</v>
+      </c>
+      <c r="O104" t="s">
+        <v>280</v>
+      </c>
+      <c r="P104" t="s">
         <v>299</v>
       </c>
-      <c r="O104" t="s">
-        <v>281</v>
-      </c>
-      <c r="P104" t="s">
+      <c r="R104" t="s">
+        <v>294</v>
+      </c>
+      <c r="S104" t="s">
         <v>300</v>
-      </c>
-      <c r="R104" t="s">
-        <v>295</v>
-      </c>
-      <c r="S104" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="105" spans="14:19" x14ac:dyDescent="0.3">
       <c r="O105" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R105" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="106" spans="14:19" x14ac:dyDescent="0.3">
       <c r="R106" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="107" spans="14:19" x14ac:dyDescent="0.3">
       <c r="R107" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="109" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N109" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="O109" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="110" spans="14:19" x14ac:dyDescent="0.3">
       <c r="O110" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="P110" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="116" spans="14:18" x14ac:dyDescent="0.3">
       <c r="N116" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="O116" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="P116" t="s">
+        <v>306</v>
+      </c>
+      <c r="Q116" t="s">
         <v>307</v>
       </c>
-      <c r="Q116" t="s">
-        <v>308</v>
-      </c>
       <c r="R116" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="117" spans="14:18" x14ac:dyDescent="0.3">
       <c r="O117" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="122" spans="14:18" x14ac:dyDescent="0.3">
       <c r="N122" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O122" t="s">
+        <v>309</v>
+      </c>
+      <c r="P122" t="s">
         <v>310</v>
-      </c>
-      <c r="P122" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="123" spans="14:18" x14ac:dyDescent="0.3">
       <c r="N123" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="O123" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="P123" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="124" spans="14:18" x14ac:dyDescent="0.3">
       <c r="N124" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="O124" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="125" spans="14:18" x14ac:dyDescent="0.3">
       <c r="N125" t="s">
+        <v>312</v>
+      </c>
+      <c r="O125" t="s">
         <v>313</v>
-      </c>
-      <c r="O125" t="s">
-        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -2391,7 +2388,7 @@
         <v>160</v>
       </c>
       <c r="D15" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -2514,7 +2511,7 @@
   <dimension ref="A2:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2538,49 +2535,49 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B3" s="11">
         <v>100</v>
       </c>
       <c r="C3" t="s">
+        <v>319</v>
+      </c>
+      <c r="D3" t="s">
         <v>320</v>
-      </c>
-      <c r="D3" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B4" s="12">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C4" t="s">
-        <v>331</v>
+        <v>319</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B6">
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -2751,10 +2748,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{489F410F-4873-4D81-A8B1-2DDFA51D15D5}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2763,12 +2760,12 @@
     <col min="2" max="2" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2782,7 +2779,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>164</v>
       </c>
@@ -2791,31 +2788,27 @@
         <v>1.5E-3</v>
       </c>
       <c r="C3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>169</v>
+      </c>
+      <c r="B4" s="3">
+        <v>2E-3</v>
+      </c>
+      <c r="C4" t="s">
         <v>170</v>
       </c>
-      <c r="B4" s="1">
-        <f>1*10^-3</f>
-        <v>1E-3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>171</v>
-      </c>
       <c r="D4" t="s">
-        <v>169</v>
-      </c>
-      <c r="H4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>168</v>
       </c>
@@ -2824,9 +2817,9 @@
         <v>1.5E-3</v>
       </c>
       <c r="C5" t="s">
-        <v>171</v>
-      </c>
-      <c r="H5" t="s">
+        <v>170</v>
+      </c>
+      <c r="D5" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2841,7 +2834,7 @@
   <dimension ref="A2:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2855,16 +2848,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E2" t="s">
         <v>70</v>
       </c>
       <c r="F2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -2900,6 +2893,9 @@
         <v>42</v>
       </c>
       <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5">
         <v>20</v>
       </c>
       <c r="D5" t="s">
@@ -2923,7 +2919,7 @@
         <v>95</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -2945,7 +2941,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B8">
         <v>0.17</v>
@@ -2957,12 +2953,12 @@
         <v>95</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B9">
         <f>30/45</f>
@@ -2976,10 +2972,10 @@
         <v>95</v>
       </c>
       <c r="E9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -3028,142 +3024,142 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C2" t="s">
         <v>225</v>
-      </c>
-      <c r="C2" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B3">
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="C3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B4">
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B5">
         <v>0.1</v>
       </c>
       <c r="C5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B6">
         <v>0.25</v>
       </c>
       <c r="C6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B7">
         <v>0.02</v>
       </c>
       <c r="C7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B8">
         <v>0.02</v>
       </c>
       <c r="C8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B9">
         <v>0.22</v>
       </c>
       <c r="C9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B10">
         <v>0.5</v>
       </c>
       <c r="C10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B11">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="C11" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B12">
         <v>0.13500000000000001</v>
       </c>
       <c r="C12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B13">
         <v>0.08</v>
       </c>
       <c r="C13" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B14">
         <v>5.7500000000000002E-2</v>
       </c>
       <c r="C14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -3200,7 +3196,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B3">
         <v>81890</v>
@@ -3228,40 +3224,40 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B6">
         <v>0.2</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B7">
         <v>0.2</v>
       </c>
       <c r="D7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B8">
         <v>2.7E-2</v>
       </c>
       <c r="D8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -3277,7 +3273,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0624EAC2-56E2-4337-8D5D-42EAA0559452}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
@@ -3310,10 +3306,10 @@
         <v>48</v>
       </c>
       <c r="E2" t="s">
+        <v>327</v>
+      </c>
+      <c r="F2" t="s">
         <v>328</v>
-      </c>
-      <c r="F2" t="s">
-        <v>329</v>
       </c>
       <c r="G2" t="s">
         <v>7</v>
@@ -3330,7 +3326,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B3">
         <v>37500</v>
@@ -3359,7 +3355,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B4">
         <v>230000</v>
@@ -3388,7 +3384,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B5">
         <v>63000</v>
@@ -3417,7 +3413,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B6">
         <v>380000</v>
@@ -3440,7 +3436,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B7">
         <v>22000</v>
@@ -3469,7 +3465,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B8">
         <v>37500</v>
@@ -3498,7 +3494,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B9">
         <v>230000</v>
@@ -3527,7 +3523,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B10">
         <v>75000</v>
@@ -3556,7 +3552,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B11">
         <v>100000</v>
@@ -3565,7 +3561,7 @@
         <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E11">
         <v>30</v>
@@ -3577,7 +3573,7 @@
         <v>47</v>
       </c>
       <c r="H11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I11">
         <v>0.67</v>
@@ -3585,7 +3581,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B12">
         <v>32.5</v>
@@ -3594,7 +3590,7 @@
         <v>29</v>
       </c>
       <c r="D12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -3614,7 +3610,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B13">
         <v>238000</v>
@@ -3623,7 +3619,7 @@
         <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E13">
         <v>10</v>
@@ -3635,7 +3631,7 @@
         <v>15</v>
       </c>
       <c r="H13" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I13">
         <v>0.65</v>
@@ -3643,7 +3639,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B14">
         <v>9500</v>
@@ -3672,7 +3668,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B15">
         <v>4800</v>
@@ -3701,7 +3697,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B16">
         <v>80</v>
@@ -3736,7 +3732,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B17">
         <v>21000</v>
@@ -3745,7 +3741,7 @@
         <v>29</v>
       </c>
       <c r="D17" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E17">
         <f>10^6</f>
@@ -3753,10 +3749,10 @@
       </c>
       <c r="F17">
         <f>(standard_belt_conveyor!B6*(standard_belt_conveyor!B4*0.3048)^2.5)</f>
-        <v>435214.799238206</v>
+        <v>76935.833953519264</v>
       </c>
       <c r="G17" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="I17">
         <v>0.2</v>
@@ -3764,7 +3760,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B19">
         <v>650</v>
@@ -3886,10 +3882,10 @@
         <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D10" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -3931,109 +3927,109 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C2" t="s">
         <v>225</v>
-      </c>
-      <c r="C2" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B3">
         <v>0.7</v>
       </c>
       <c r="C3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B4">
         <v>0.18</v>
       </c>
       <c r="C4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B5">
         <v>0.1</v>
       </c>
       <c r="C5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B6">
         <v>0.38</v>
       </c>
       <c r="C6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B7">
         <v>0.4</v>
       </c>
       <c r="C7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B8">
         <v>0.06</v>
       </c>
       <c r="C8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B9">
         <v>0.1</v>
       </c>
       <c r="C9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B10">
         <v>0.25</v>
       </c>
       <c r="C10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B11">
         <v>0.2</v>
       </c>
       <c r="C11" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -4149,7 +4145,7 @@
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -4176,7 +4172,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9896EE1E-7F56-45CB-B0FF-A4EB36B766F1}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixed errors in LC processing, LC purification, Reactant flow, LDH energy, Q Reactors and adjusted assumptions in LDH attributes
</commit_message>
<xml_diff>
--- a/data/LDH_attributes.xlsx
+++ b/data/LDH_attributes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chant\PycharmProjects\FUSE-V2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F4A90FB-A27F-4678-AE41-B1CF1C764BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AA90BB8-5E4B-4E79-BFAA-843315B2FFBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{9D386D14-BB1A-49FB-A5CB-94A6FCCCA1F9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="12" activeTab="15" xr2:uid="{9D386D14-BB1A-49FB-A5CB-94A6FCCCA1F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Process overview" sheetId="23" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="335">
   <si>
     <t>key</t>
   </si>
@@ -334,9 +334,6 @@
     <t>$/kg</t>
   </si>
   <si>
-    <t>https://www.alibaba.com/product-detail/Battery-Grade-Lioh-Lithium-Hydroxide-Lithium_62267896947.html?spm=a2700.galleryofferlist.normal_offer.d_title.b1a0469axvBcL2&amp;s=p</t>
-  </si>
-  <si>
     <t>https://www.alibaba.com/product-detail/Exporter-hot-sale-Hydrochloric-Acid-Factory_1600289913553.html?spm=a2700.galleryofferlist.normal_offer.d_title.3a8e2c51jUtwul&amp;s=p</t>
   </si>
   <si>
@@ -524,9 +521,6 @@
   </si>
   <si>
     <t>dryer_efficiency</t>
-  </si>
-  <si>
-    <t>t</t>
   </si>
   <si>
     <t>mass_difference_evaporation</t>
@@ -1092,9 +1086,6 @@
     <t>Li 2018 (Lithium Recovery from Aqueous Resources and Batteries: A Brief Review)</t>
   </si>
   <si>
-    <t xml:space="preserve">guess </t>
-  </si>
-  <si>
     <t>tonnes/year</t>
   </si>
   <si>
@@ -1105,6 +1096,12 @@
   </si>
   <si>
     <t>20 wt% soda ash sol (Ehren, Patent no: WO 2013/036983 Al)</t>
+  </si>
+  <si>
+    <t>guess (water content left after filtration)</t>
+  </si>
+  <si>
+    <t>https://www.alibaba.com/product-detail/Industrial-Grade-57-LiOH-Manufacturer-Price_1600137601702.html?spm=a2700.galleryofferlist.normal_offer.d_title.2655469a48IhKh</t>
   </si>
 </sst>
 </file>
@@ -1646,62 +1643,62 @@
   <sheetData>
     <row r="2" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N2" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="P2" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="Q2" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="R2" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="S2" s="4" t="s">
         <v>240</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="12" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N12" t="s">
+        <v>241</v>
+      </c>
+      <c r="O12" t="s">
+        <v>110</v>
+      </c>
+      <c r="P12" t="s">
+        <v>242</v>
+      </c>
+      <c r="Q12" t="s">
         <v>243</v>
       </c>
-      <c r="O12" t="s">
-        <v>111</v>
-      </c>
-      <c r="P12" t="s">
+      <c r="S12" t="s">
         <v>244</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>245</v>
-      </c>
-      <c r="S12" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="13" spans="14:20" x14ac:dyDescent="0.3">
       <c r="P13" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="S13" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="14" spans="14:20" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="P14" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="R14" s="6"/>
       <c r="S14" s="13" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="T14" s="6"/>
     </row>
     <row r="15" spans="14:20" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="P15" s="16" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="R15" s="6"/>
       <c r="S15" s="14"/>
@@ -1711,63 +1708,63 @@
       <c r="P16" s="16"/>
       <c r="R16" s="7"/>
       <c r="S16" s="8" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="T16" s="7"/>
     </row>
     <row r="19" spans="14:17" x14ac:dyDescent="0.3">
       <c r="N19" t="s">
+        <v>250</v>
+      </c>
+      <c r="O19" t="s">
+        <v>110</v>
+      </c>
+      <c r="P19" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q19" t="s">
         <v>252</v>
-      </c>
-      <c r="O19" t="s">
-        <v>111</v>
-      </c>
-      <c r="P19" t="s">
-        <v>253</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="25" spans="14:17" x14ac:dyDescent="0.3">
       <c r="N25" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="O25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P25" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="26" spans="14:17" x14ac:dyDescent="0.3">
       <c r="P26" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="Q26" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="39" spans="14:18" x14ac:dyDescent="0.3">
       <c r="N39" t="s">
+        <v>256</v>
+      </c>
+      <c r="O39" t="s">
+        <v>257</v>
+      </c>
+      <c r="P39" t="s">
         <v>258</v>
-      </c>
-      <c r="O39" t="s">
-        <v>259</v>
-      </c>
-      <c r="P39" t="s">
-        <v>260</v>
       </c>
       <c r="Q39">
         <v>12</v>
       </c>
       <c r="R39" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="40" spans="14:18" x14ac:dyDescent="0.3">
       <c r="P40" s="17" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="41" spans="14:18" x14ac:dyDescent="0.3">
@@ -1776,73 +1773,73 @@
     <row r="42" spans="14:18" x14ac:dyDescent="0.3">
       <c r="P42" s="10"/>
       <c r="R42" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="52" spans="14:18" x14ac:dyDescent="0.3">
       <c r="N52" t="s">
+        <v>261</v>
+      </c>
+      <c r="O52" t="s">
+        <v>257</v>
+      </c>
+      <c r="P52" t="s">
+        <v>262</v>
+      </c>
+      <c r="Q52" t="s">
         <v>263</v>
       </c>
-      <c r="O52" t="s">
-        <v>259</v>
-      </c>
-      <c r="P52" t="s">
+      <c r="R52" t="s">
         <v>264</v>
-      </c>
-      <c r="Q52" t="s">
-        <v>265</v>
-      </c>
-      <c r="R52" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="53" spans="14:18" x14ac:dyDescent="0.3">
       <c r="P53" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="R53" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="70" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N70" t="s">
+        <v>266</v>
+      </c>
+      <c r="O70" t="s">
+        <v>267</v>
+      </c>
+      <c r="P70" t="s">
         <v>268</v>
       </c>
-      <c r="O70" t="s">
+      <c r="Q70" t="s">
         <v>269</v>
       </c>
-      <c r="P70" t="s">
+      <c r="R70" t="s">
         <v>270</v>
       </c>
-      <c r="Q70" t="s">
+      <c r="S70" s="9" t="s">
         <v>271</v>
-      </c>
-      <c r="R70" t="s">
-        <v>272</v>
-      </c>
-      <c r="S70" s="9" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="71" spans="14:19" x14ac:dyDescent="0.3">
       <c r="P71" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="R71" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="72" spans="14:19" x14ac:dyDescent="0.3">
       <c r="P72" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="R72" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="73" spans="14:19" x14ac:dyDescent="0.3">
       <c r="P73" s="16" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="74" spans="14:19" x14ac:dyDescent="0.3">
@@ -1850,68 +1847,68 @@
     </row>
     <row r="77" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N77" t="s">
+        <v>274</v>
+      </c>
+      <c r="O77" t="s">
+        <v>267</v>
+      </c>
+      <c r="P77" t="s">
+        <v>275</v>
+      </c>
+      <c r="Q77" t="s">
         <v>276</v>
-      </c>
-      <c r="O77" t="s">
-        <v>269</v>
-      </c>
-      <c r="P77" t="s">
-        <v>277</v>
-      </c>
-      <c r="Q77" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="85" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N85" t="s">
+        <v>277</v>
+      </c>
+      <c r="O85" t="s">
+        <v>278</v>
+      </c>
+      <c r="P85" t="s">
+        <v>242</v>
+      </c>
+      <c r="Q85" t="s">
         <v>279</v>
       </c>
-      <c r="O85" t="s">
+      <c r="R85" t="s">
         <v>280</v>
       </c>
-      <c r="P85" t="s">
-        <v>244</v>
-      </c>
-      <c r="Q85" t="s">
+      <c r="S85" t="s">
         <v>281</v>
-      </c>
-      <c r="R85" t="s">
-        <v>282</v>
-      </c>
-      <c r="S85" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="86" spans="14:19" x14ac:dyDescent="0.3">
       <c r="O86" t="s">
+        <v>282</v>
+      </c>
+      <c r="P86" t="s">
+        <v>283</v>
+      </c>
+      <c r="R86" t="s">
         <v>284</v>
-      </c>
-      <c r="P86" t="s">
-        <v>285</v>
-      </c>
-      <c r="R86" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="87" spans="14:19" x14ac:dyDescent="0.3">
       <c r="P87" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="R87" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="88" spans="14:19" x14ac:dyDescent="0.3">
       <c r="P88" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="R88" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="89" spans="14:19" x14ac:dyDescent="0.3">
       <c r="P89" s="17" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="90" spans="14:19" x14ac:dyDescent="0.3">
@@ -1919,46 +1916,46 @@
     </row>
     <row r="94" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N94" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="O94" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="P94" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="95" spans="14:19" x14ac:dyDescent="0.3">
       <c r="O95" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="100" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N100" t="s">
+        <v>290</v>
+      </c>
+      <c r="O100" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q100" t="s">
+        <v>291</v>
+      </c>
+      <c r="R100" t="s">
         <v>292</v>
-      </c>
-      <c r="O100" t="s">
-        <v>280</v>
-      </c>
-      <c r="Q100" t="s">
-        <v>293</v>
-      </c>
-      <c r="R100" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="101" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N101" t="s">
+        <v>293</v>
+      </c>
+      <c r="O101" s="15" t="s">
+        <v>294</v>
+      </c>
+      <c r="P101" t="s">
         <v>295</v>
       </c>
-      <c r="O101" s="15" t="s">
-        <v>296</v>
-      </c>
-      <c r="P101" t="s">
-        <v>297</v>
-      </c>
       <c r="Q101" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="102" spans="14:19" x14ac:dyDescent="0.3">
@@ -1966,113 +1963,113 @@
     </row>
     <row r="104" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N104" t="s">
+        <v>296</v>
+      </c>
+      <c r="O104" t="s">
+        <v>278</v>
+      </c>
+      <c r="P104" t="s">
+        <v>297</v>
+      </c>
+      <c r="R104" t="s">
+        <v>292</v>
+      </c>
+      <c r="S104" t="s">
         <v>298</v>
-      </c>
-      <c r="O104" t="s">
-        <v>280</v>
-      </c>
-      <c r="P104" t="s">
-        <v>299</v>
-      </c>
-      <c r="R104" t="s">
-        <v>294</v>
-      </c>
-      <c r="S104" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="105" spans="14:19" x14ac:dyDescent="0.3">
       <c r="O105" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="R105" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="106" spans="14:19" x14ac:dyDescent="0.3">
       <c r="R106" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="107" spans="14:19" x14ac:dyDescent="0.3">
       <c r="R107" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="109" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N109" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="O109" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="110" spans="14:19" x14ac:dyDescent="0.3">
       <c r="O110" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="P110" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="116" spans="14:18" x14ac:dyDescent="0.3">
       <c r="N116" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="O116" t="s">
+        <v>278</v>
+      </c>
+      <c r="P116" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q116" t="s">
+        <v>305</v>
+      </c>
+      <c r="R116" t="s">
         <v>280</v>
-      </c>
-      <c r="P116" t="s">
-        <v>306</v>
-      </c>
-      <c r="Q116" t="s">
-        <v>307</v>
-      </c>
-      <c r="R116" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="117" spans="14:18" x14ac:dyDescent="0.3">
       <c r="O117" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="122" spans="14:18" x14ac:dyDescent="0.3">
       <c r="N122" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="O122" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="P122" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="123" spans="14:18" x14ac:dyDescent="0.3">
       <c r="N123" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="O123" t="s">
+        <v>307</v>
+      </c>
+      <c r="P123" t="s">
         <v>309</v>
-      </c>
-      <c r="P123" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="124" spans="14:18" x14ac:dyDescent="0.3">
       <c r="N124" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="O124" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="125" spans="14:18" x14ac:dyDescent="0.3">
       <c r="N125" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="O125" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
   </sheetData>
@@ -2104,7 +2101,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -2117,7 +2114,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B3">
         <v>0.7</v>
@@ -2136,7 +2133,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B5" s="1">
         <v>2</v>
@@ -2200,7 +2197,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2210,7 +2207,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -2224,23 +2221,23 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B4" s="1">
         <v>0.9</v>
@@ -2251,7 +2248,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B5" s="1">
         <v>0.8</v>
@@ -2262,32 +2259,32 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B6">
         <v>298.14999999999998</v>
       </c>
       <c r="C6" t="s">
+        <v>141</v>
+      </c>
+      <c r="D6" t="s">
         <v>142</v>
-      </c>
-      <c r="D6" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B7">
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B8" s="1">
         <v>2</v>
@@ -2301,7 +2298,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B9">
         <v>353</v>
@@ -2312,18 +2309,18 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
@@ -2379,21 +2376,21 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B15" s="1">
-        <v>5000</v>
+        <v>50000</v>
       </c>
       <c r="C15" t="s">
-        <v>160</v>
+        <v>23</v>
       </c>
       <c r="D15" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B16">
         <v>0.8</v>
@@ -2401,13 +2398,16 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B17">
         <v>313.14999999999998</v>
       </c>
+      <c r="C17" t="s">
+        <v>1</v>
+      </c>
       <c r="D17" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -2535,49 +2535,49 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B3" s="11">
         <v>100</v>
       </c>
       <c r="C3" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D3" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B4" s="12">
         <v>100</v>
       </c>
       <c r="C4" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B6">
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -2776,19 +2776,19 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B3">
         <f xml:space="preserve"> 1.5 * 10^(-3)</f>
         <v>1.5E-3</v>
       </c>
       <c r="C3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D3" t="s">
         <v>55</v>
@@ -2796,28 +2796,28 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B4" s="3">
         <v>2E-3</v>
       </c>
       <c r="C4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D4" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B5" s="1">
         <f>1.5*10^-3</f>
         <v>1.5E-3</v>
       </c>
       <c r="C5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D5" t="s">
         <v>40</v>
@@ -2833,8 +2833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F37A8F43-ECBD-4243-988B-AAA9A59B3D22}">
   <dimension ref="A2:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2848,21 +2848,21 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E2" t="s">
         <v>70</v>
       </c>
       <c r="F2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B3">
         <v>6.6600000000000006E-2</v>
@@ -2879,7 +2879,7 @@
         <v>93</v>
       </c>
       <c r="B4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="D4" t="s">
         <v>94</v>
@@ -2893,16 +2893,16 @@
         <v>42</v>
       </c>
       <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5">
         <v>8</v>
-      </c>
-      <c r="C5">
-        <v>20</v>
       </c>
       <c r="D5" t="s">
         <v>95</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>96</v>
+        <v>334</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -2919,7 +2919,7 @@
         <v>95</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -2936,12 +2936,12 @@
         <v>95</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B8">
         <v>0.17</v>
@@ -2953,12 +2953,12 @@
         <v>95</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B9">
         <f>30/45</f>
@@ -2972,10 +2972,10 @@
         <v>95</v>
       </c>
       <c r="E9" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -3005,7 +3005,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3024,142 +3024,142 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B3">
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="C3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B4">
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B5">
         <v>0.1</v>
       </c>
       <c r="C5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B6">
         <v>0.25</v>
       </c>
       <c r="C6" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B7">
         <v>0.02</v>
       </c>
       <c r="C7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B8">
         <v>0.02</v>
       </c>
       <c r="C8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B9">
         <v>0.22</v>
       </c>
       <c r="C9" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B10">
         <v>0.5</v>
       </c>
       <c r="C10" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B11">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="C11" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B12">
         <v>0.13500000000000001</v>
       </c>
       <c r="C12" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B13">
         <v>0.08</v>
       </c>
       <c r="C13" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B14">
         <v>5.7500000000000002E-2</v>
       </c>
       <c r="C14" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -3188,7 +3188,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -3196,7 +3196,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B3">
         <v>81890</v>
@@ -3205,59 +3205,59 @@
         <v>29</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B4" s="3">
         <v>45</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B6">
         <v>0.2</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B7">
         <v>0.2</v>
       </c>
       <c r="D7" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B8">
         <v>2.7E-2</v>
       </c>
       <c r="D8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -3306,10 +3306,10 @@
         <v>48</v>
       </c>
       <c r="E2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="F2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="G2" t="s">
         <v>7</v>
@@ -3326,7 +3326,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B3">
         <v>37500</v>
@@ -3355,7 +3355,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B4">
         <v>230000</v>
@@ -3384,7 +3384,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B5">
         <v>63000</v>
@@ -3413,7 +3413,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B6">
         <v>380000</v>
@@ -3436,7 +3436,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B7">
         <v>22000</v>
@@ -3445,7 +3445,7 @@
         <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E7">
         <v>1600</v>
@@ -3465,7 +3465,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B8">
         <v>37500</v>
@@ -3494,7 +3494,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B9">
         <v>230000</v>
@@ -3523,7 +3523,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B10">
         <v>75000</v>
@@ -3552,7 +3552,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B11">
         <v>100000</v>
@@ -3561,7 +3561,7 @@
         <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E11">
         <v>30</v>
@@ -3573,7 +3573,7 @@
         <v>47</v>
       </c>
       <c r="H11" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I11">
         <v>0.67</v>
@@ -3581,7 +3581,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B12">
         <v>32.5</v>
@@ -3590,7 +3590,7 @@
         <v>29</v>
       </c>
       <c r="D12" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -3602,7 +3602,7 @@
         <v>47</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I12">
         <v>0.95</v>
@@ -3610,7 +3610,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B13">
         <v>238000</v>
@@ -3619,7 +3619,7 @@
         <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E13">
         <v>10</v>
@@ -3631,7 +3631,7 @@
         <v>15</v>
       </c>
       <c r="H13" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I13">
         <v>0.65</v>
@@ -3639,7 +3639,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B14">
         <v>9500</v>
@@ -3668,7 +3668,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B15">
         <v>4800</v>
@@ -3697,7 +3697,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B16">
         <v>80</v>
@@ -3732,7 +3732,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B17">
         <v>21000</v>
@@ -3741,7 +3741,7 @@
         <v>29</v>
       </c>
       <c r="D17" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="E17">
         <f>10^6</f>
@@ -3752,7 +3752,7 @@
         <v>76935.833953519264</v>
       </c>
       <c r="G17" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="I17">
         <v>0.2</v>
@@ -3760,7 +3760,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B19">
         <v>650</v>
@@ -3792,7 +3792,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3803,7 +3803,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -3882,15 +3882,15 @@
         <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D10" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B11">
         <v>0.9</v>
@@ -3907,7 +3907,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3927,109 +3927,109 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B3">
         <v>0.7</v>
       </c>
       <c r="C3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B4">
         <v>0.18</v>
       </c>
       <c r="C4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B5">
         <v>0.1</v>
       </c>
       <c r="C5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B6">
         <v>0.38</v>
       </c>
       <c r="C6" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B7">
         <v>0.4</v>
       </c>
       <c r="C7" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B8">
         <v>0.06</v>
       </c>
       <c r="C8" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B9">
         <v>0.1</v>
       </c>
       <c r="C9" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B10">
         <v>0.25</v>
       </c>
       <c r="C10" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B11">
         <v>0.2</v>
       </c>
       <c r="C11" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -4072,7 +4072,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D3" t="s">
         <v>46</v>
@@ -4145,7 +4145,7 @@
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -4172,7 +4172,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9896EE1E-7F56-45CB-B0FF-A4EB36B766F1}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -4199,35 +4199,35 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B3">
         <v>35000</v>
       </c>
       <c r="C3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B4">
         <v>7920</v>
       </c>
       <c r="C4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B5">
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -4269,41 +4269,41 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B3">
         <v>0.19400000000000001</v>
       </c>
       <c r="C3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B4">
         <v>1204.67</v>
       </c>
       <c r="C4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -4326,7 +4326,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -4345,7 +4345,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B3">
         <v>2.5</v>
@@ -4354,7 +4354,7 @@
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -4368,12 +4368,12 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B5">
         <v>0.9</v>
@@ -4381,43 +4381,43 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B7">
         <v>8</v>
       </c>
       <c r="C7" t="s">
+        <v>126</v>
+      </c>
+      <c r="D7" t="s">
         <v>127</v>
-      </c>
-      <c r="D7" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B8">
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -4459,46 +4459,46 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B3">
         <v>0.19400000000000001</v>
       </c>
       <c r="C3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B4">
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B5">
         <v>50</v>
       </c>
       <c r="C5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" t="s">
         <v>106</v>
-      </c>
-      <c r="D5" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -4551,18 +4551,18 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B3">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -4570,24 +4570,24 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B5">
         <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B6">
         <v>1.71</v>
       </c>
       <c r="C6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -4634,24 +4634,24 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B4">
         <v>174</v>
       </c>
       <c r="C4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B5">
         <v>1.54</v>
       </c>
       <c r="C5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implementation of function description in QMachines and, small corrections to LDH energy, LDH capex, LDH opex and reactant flow, adjustments in LDH attributes
</commit_message>
<xml_diff>
--- a/data/LDH_attributes.xlsx
+++ b/data/LDH_attributes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chant\PycharmProjects\FUSE-V2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AA90BB8-5E4B-4E79-BFAA-843315B2FFBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C956B0A3-EBB9-4700-BBD2-5CAB3E2B065D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="12" activeTab="15" xr2:uid="{9D386D14-BB1A-49FB-A5CB-94A6FCCCA1F9}"/>
   </bookViews>
@@ -1050,18 +1050,12 @@
     <t>Sheets: plant, brine, column, washing, stripping</t>
   </si>
   <si>
-    <t>ft/min</t>
-  </si>
-  <si>
     <t>assumption</t>
   </si>
   <si>
     <t>gradient</t>
   </si>
   <si>
-    <t>°</t>
-  </si>
-  <si>
     <t>output</t>
   </si>
   <si>
@@ -1102,6 +1096,12 @@
   </si>
   <si>
     <t>https://www.alibaba.com/product-detail/Industrial-Grade-57-LiOH-Manufacturer-Price_1600137601702.html?spm=a2700.galleryofferlist.normal_offer.d_title.2655469a48IhKh</t>
+  </si>
+  <si>
+    <t>m/min</t>
+  </si>
+  <si>
+    <t>%</t>
   </si>
 </sst>
 </file>
@@ -2385,7 +2385,7 @@
         <v>23</v>
       </c>
       <c r="D15" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -2511,7 +2511,7 @@
   <dimension ref="A2:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2535,49 +2535,49 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B3" s="11">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
+        <v>333</v>
+      </c>
+      <c r="D3" t="s">
         <v>317</v>
-      </c>
-      <c r="D3" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B4" s="12">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>317</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>320</v>
+        <v>334</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B6">
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -2805,7 +2805,7 @@
         <v>168</v>
       </c>
       <c r="D4" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -2834,7 +2834,7 @@
   <dimension ref="A2:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2902,7 +2902,7 @@
         <v>95</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -3005,7 +3005,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3172,7 +3172,7 @@
   <dimension ref="A2:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3213,7 +3213,7 @@
         <v>136</v>
       </c>
       <c r="B4" s="3">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>134</v>
@@ -3266,6 +3266,7 @@
     <hyperlink ref="D3" r:id="rId2" location="(1)" xr:uid="{8BD7CCF6-289D-4454-B231-B17DF4EE5224}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -3306,10 +3307,10 @@
         <v>48</v>
       </c>
       <c r="E2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="F2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G2" t="s">
         <v>7</v>
@@ -3741,7 +3742,7 @@
         <v>29</v>
       </c>
       <c r="D17" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="E17">
         <f>10^6</f>
@@ -3749,10 +3750,10 @@
       </c>
       <c r="F17">
         <f>(standard_belt_conveyor!B6*(standard_belt_conveyor!B4*0.3048)^2.5)</f>
-        <v>76935.833953519264</v>
+        <v>13600.462476193932</v>
       </c>
       <c r="G17" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="I17">
         <v>0.2</v>
@@ -3760,7 +3761,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B19">
         <v>650</v>
@@ -3882,10 +3883,10 @@
         <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D10" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -4240,7 +4241,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Upscaling of water used for column washing and stripping for 25 tonnes of sorbent, implementation of usage time to belt conveyor to get kWh
</commit_message>
<xml_diff>
--- a/data/LDH_attributes.xlsx
+++ b/data/LDH_attributes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chant\PycharmProjects\FUSE-V2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C956B0A3-EBB9-4700-BBD2-5CAB3E2B065D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59ECE559-4848-4A5A-8D0D-E28A7C0F0D55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="12" activeTab="15" xr2:uid="{9D386D14-BB1A-49FB-A5CB-94A6FCCCA1F9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="7" xr2:uid="{9D386D14-BB1A-49FB-A5CB-94A6FCCCA1F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Process overview" sheetId="23" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="335">
   <si>
     <t>key</t>
   </si>
@@ -355,9 +355,6 @@
     <t>H2O_washing</t>
   </si>
   <si>
-    <t>per washing cycle</t>
-  </si>
-  <si>
     <t>NaCl_conc</t>
   </si>
   <si>
@@ -367,15 +364,9 @@
     <t>5 wt% solution</t>
   </si>
   <si>
-    <t>No_washing_cycles</t>
-  </si>
-  <si>
     <t>H2O_stripping</t>
   </si>
   <si>
-    <t>No_stripping_cycles</t>
-  </si>
-  <si>
     <t>Sorbent Synthesis</t>
   </si>
   <si>
@@ -521,9 +512,6 @@
   </si>
   <si>
     <t>dryer_efficiency</t>
-  </si>
-  <si>
-    <t>mass_difference_evaporation</t>
   </si>
   <si>
     <t>washing_temperature</t>
@@ -1092,9 +1080,6 @@
     <t>20 wt% soda ash sol (Ehren, Patent no: WO 2013/036983 Al)</t>
   </si>
   <si>
-    <t>guess (water content left after filtration)</t>
-  </si>
-  <si>
     <t>https://www.alibaba.com/product-detail/Industrial-Grade-57-LiOH-Manufacturer-Price_1600137601702.html?spm=a2700.galleryofferlist.normal_offer.d_title.2655469a48IhKh</t>
   </si>
   <si>
@@ -1102,13 +1087,28 @@
   </si>
   <si>
     <t>%</t>
+  </si>
+  <si>
+    <t>hours_operation</t>
+  </si>
+  <si>
+    <t>water_content_filtration</t>
+  </si>
+  <si>
+    <t>from Huang 2021</t>
+  </si>
+  <si>
+    <t>upscaled from Huang 2021 (40l for 70g sorbent)</t>
+  </si>
+  <si>
+    <t>upscaled from Huang 2021 30l for 70g sorbent)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1156,6 +1156,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1216,7 +1224,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -1253,6 +1261,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1643,62 +1652,62 @@
   <sheetData>
     <row r="2" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N2" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="R2" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="S2" s="4" t="s">
         <v>236</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="12" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N12" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="O12" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="P12" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="Q12" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="S12" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" spans="14:20" x14ac:dyDescent="0.3">
       <c r="P13" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="S13" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="14" spans="14:20" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="P14" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="R14" s="6"/>
       <c r="S14" s="13" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="T14" s="6"/>
     </row>
     <row r="15" spans="14:20" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="P15" s="16" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="R15" s="6"/>
       <c r="S15" s="14"/>
@@ -1708,63 +1717,63 @@
       <c r="P16" s="16"/>
       <c r="R16" s="7"/>
       <c r="S16" s="8" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="T16" s="7"/>
     </row>
     <row r="19" spans="14:17" x14ac:dyDescent="0.3">
       <c r="N19" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="O19" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="P19" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="Q19" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="25" spans="14:17" x14ac:dyDescent="0.3">
       <c r="N25" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="O25" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="P25" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="26" spans="14:17" x14ac:dyDescent="0.3">
       <c r="P26" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="Q26" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="39" spans="14:18" x14ac:dyDescent="0.3">
       <c r="N39" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="O39" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="P39" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="Q39">
         <v>12</v>
       </c>
       <c r="R39" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="40" spans="14:18" x14ac:dyDescent="0.3">
       <c r="P40" s="17" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="41" spans="14:18" x14ac:dyDescent="0.3">
@@ -1773,73 +1782,73 @@
     <row r="42" spans="14:18" x14ac:dyDescent="0.3">
       <c r="P42" s="10"/>
       <c r="R42" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="52" spans="14:18" x14ac:dyDescent="0.3">
       <c r="N52" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="O52" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="P52" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="Q52" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="R52" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="53" spans="14:18" x14ac:dyDescent="0.3">
       <c r="P53" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="R53" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="70" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N70" t="s">
+        <v>262</v>
+      </c>
+      <c r="O70" t="s">
+        <v>263</v>
+      </c>
+      <c r="P70" t="s">
+        <v>264</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>265</v>
+      </c>
+      <c r="R70" t="s">
         <v>266</v>
       </c>
-      <c r="O70" t="s">
+      <c r="S70" s="9" t="s">
         <v>267</v>
-      </c>
-      <c r="P70" t="s">
-        <v>268</v>
-      </c>
-      <c r="Q70" t="s">
-        <v>269</v>
-      </c>
-      <c r="R70" t="s">
-        <v>270</v>
-      </c>
-      <c r="S70" s="9" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="71" spans="14:19" x14ac:dyDescent="0.3">
       <c r="P71" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="R71" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="72" spans="14:19" x14ac:dyDescent="0.3">
       <c r="P72" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="R72" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="73" spans="14:19" x14ac:dyDescent="0.3">
       <c r="P73" s="16" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="74" spans="14:19" x14ac:dyDescent="0.3">
@@ -1847,68 +1856,68 @@
     </row>
     <row r="77" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N77" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="O77" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="P77" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="Q77" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="85" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N85" t="s">
+        <v>273</v>
+      </c>
+      <c r="O85" t="s">
+        <v>274</v>
+      </c>
+      <c r="P85" t="s">
+        <v>238</v>
+      </c>
+      <c r="Q85" t="s">
+        <v>275</v>
+      </c>
+      <c r="R85" t="s">
+        <v>276</v>
+      </c>
+      <c r="S85" t="s">
         <v>277</v>
-      </c>
-      <c r="O85" t="s">
-        <v>278</v>
-      </c>
-      <c r="P85" t="s">
-        <v>242</v>
-      </c>
-      <c r="Q85" t="s">
-        <v>279</v>
-      </c>
-      <c r="R85" t="s">
-        <v>280</v>
-      </c>
-      <c r="S85" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="86" spans="14:19" x14ac:dyDescent="0.3">
       <c r="O86" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="P86" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="R86" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="87" spans="14:19" x14ac:dyDescent="0.3">
       <c r="P87" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="R87" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="88" spans="14:19" x14ac:dyDescent="0.3">
       <c r="P88" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="R88" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="89" spans="14:19" x14ac:dyDescent="0.3">
       <c r="P89" s="17" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="90" spans="14:19" x14ac:dyDescent="0.3">
@@ -1916,46 +1925,46 @@
     </row>
     <row r="94" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N94" t="s">
+        <v>270</v>
+      </c>
+      <c r="O94" t="s">
         <v>274</v>
       </c>
-      <c r="O94" t="s">
-        <v>278</v>
-      </c>
       <c r="P94" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="95" spans="14:19" x14ac:dyDescent="0.3">
       <c r="O95" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="100" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N100" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="O100" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="Q100" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="R100" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="101" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N101" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="O101" s="15" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="P101" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="Q101" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="102" spans="14:19" x14ac:dyDescent="0.3">
@@ -1963,113 +1972,113 @@
     </row>
     <row r="104" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N104" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="O104" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="P104" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="R104" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="S104" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="105" spans="14:19" x14ac:dyDescent="0.3">
       <c r="O105" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="R105" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="106" spans="14:19" x14ac:dyDescent="0.3">
       <c r="R106" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="107" spans="14:19" x14ac:dyDescent="0.3">
       <c r="R107" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="109" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N109" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="O109" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="110" spans="14:19" x14ac:dyDescent="0.3">
       <c r="O110" t="s">
+        <v>295</v>
+      </c>
+      <c r="P110" t="s">
         <v>299</v>
-      </c>
-      <c r="P110" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="116" spans="14:18" x14ac:dyDescent="0.3">
       <c r="N116" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="O116" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="P116" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="Q116" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="R116" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="117" spans="14:18" x14ac:dyDescent="0.3">
       <c r="O117" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="122" spans="14:18" x14ac:dyDescent="0.3">
       <c r="N122" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="O122" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="P122" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="123" spans="14:18" x14ac:dyDescent="0.3">
       <c r="N123" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="O123" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="P123" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="124" spans="14:18" x14ac:dyDescent="0.3">
       <c r="N124" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="O124" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="125" spans="14:18" x14ac:dyDescent="0.3">
       <c r="N125" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="O125" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
   </sheetData>
@@ -2101,7 +2110,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -2133,7 +2142,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B5" s="1">
         <v>2</v>
@@ -2197,7 +2206,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2207,7 +2216,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -2221,23 +2230,23 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B4" s="1">
         <v>0.9</v>
@@ -2248,7 +2257,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B5" s="1">
         <v>0.8</v>
@@ -2259,32 +2268,32 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B6">
         <v>298.14999999999998</v>
       </c>
       <c r="C6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D6" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>143</v>
-      </c>
-      <c r="B7">
+      <c r="A7" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="B7" s="18">
         <v>10</v>
       </c>
-      <c r="C7" t="s">
-        <v>139</v>
+      <c r="C7" s="18" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B8" s="1">
         <v>2</v>
@@ -2298,7 +2307,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B9">
         <v>353</v>
@@ -2308,19 +2317,19 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>145</v>
-      </c>
-      <c r="B10">
+      <c r="A10" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="B10" s="18">
         <v>1</v>
       </c>
-      <c r="C10" t="s">
-        <v>139</v>
+      <c r="C10" s="18" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
@@ -2376,21 +2385,18 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="B15" s="1">
-        <v>50000</v>
-      </c>
-      <c r="C15" t="s">
-        <v>23</v>
+        <v>331</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0.35</v>
       </c>
       <c r="D15" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B16">
         <v>0.8</v>
@@ -2398,7 +2404,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B17">
         <v>313.14999999999998</v>
@@ -2407,7 +2413,7 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -2508,15 +2514,15 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39F5853C-7EBD-44C3-B44F-35BFE47CA7B2}">
-  <dimension ref="A2:D7"/>
+  <dimension ref="A2:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.109375" customWidth="1"/>
+    <col min="1" max="1" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -2535,21 +2541,21 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B3" s="11">
         <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="D3" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B4" s="12">
         <v>50</v>
@@ -2560,24 +2566,24 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B6">
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -2586,6 +2592,17 @@
       </c>
       <c r="B7">
         <v>0.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>330</v>
+      </c>
+      <c r="B8">
+        <v>7920</v>
+      </c>
+      <c r="C8" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -2781,14 +2798,14 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B3">
         <f xml:space="preserve"> 1.5 * 10^(-3)</f>
         <v>1.5E-3</v>
       </c>
       <c r="C3" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D3" t="s">
         <v>55</v>
@@ -2796,28 +2813,28 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B4" s="3">
         <v>2E-3</v>
       </c>
       <c r="C4" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D4" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B5" s="1">
         <f>1.5*10^-3</f>
         <v>1.5E-3</v>
       </c>
       <c r="C5" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D5" t="s">
         <v>40</v>
@@ -2833,7 +2850,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F37A8F43-ECBD-4243-988B-AAA9A59B3D22}">
   <dimension ref="A2:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -2848,16 +2865,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E2" t="s">
         <v>70</v>
       </c>
       <c r="F2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -2902,7 +2919,7 @@
         <v>95</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -2919,7 +2936,7 @@
         <v>95</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -2941,7 +2958,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B8">
         <v>0.17</v>
@@ -2953,12 +2970,12 @@
         <v>95</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B9">
         <f>30/45</f>
@@ -2972,10 +2989,10 @@
         <v>95</v>
       </c>
       <c r="E9" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -3024,142 +3041,142 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C2" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B3">
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="C3" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B4">
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C4" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B5">
         <v>0.1</v>
       </c>
       <c r="C5" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B6">
         <v>0.25</v>
       </c>
       <c r="C6" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B7">
         <v>0.02</v>
       </c>
       <c r="C7" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B8">
         <v>0.02</v>
       </c>
       <c r="C8" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B9">
         <v>0.22</v>
       </c>
       <c r="C9" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B10">
         <v>0.5</v>
       </c>
       <c r="C10" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B11">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="C11" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B12">
         <v>0.13500000000000001</v>
       </c>
       <c r="C12" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B13">
         <v>0.08</v>
       </c>
       <c r="C13" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B14">
         <v>5.7500000000000002E-2</v>
       </c>
       <c r="C14" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -3188,7 +3205,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -3196,7 +3213,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B3">
         <v>81890</v>
@@ -3205,59 +3222,59 @@
         <v>29</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B4" s="3">
         <v>20</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="H4" t="s">
         <v>134</v>
-      </c>
-      <c r="H4" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B6">
         <v>0.2</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B7">
         <v>0.2</v>
       </c>
       <c r="D7" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B8">
         <v>2.7E-2</v>
       </c>
       <c r="D8" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -3307,10 +3324,10 @@
         <v>48</v>
       </c>
       <c r="E2" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="F2" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="G2" t="s">
         <v>7</v>
@@ -3327,7 +3344,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B3">
         <v>37500</v>
@@ -3356,7 +3373,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B4">
         <v>230000</v>
@@ -3385,7 +3402,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B5">
         <v>63000</v>
@@ -3414,7 +3431,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B6">
         <v>380000</v>
@@ -3437,7 +3454,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B7">
         <v>22000</v>
@@ -3446,7 +3463,7 @@
         <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E7">
         <v>1600</v>
@@ -3466,7 +3483,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B8">
         <v>37500</v>
@@ -3495,7 +3512,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B9">
         <v>230000</v>
@@ -3524,7 +3541,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B10">
         <v>75000</v>
@@ -3553,7 +3570,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B11">
         <v>100000</v>
@@ -3562,7 +3579,7 @@
         <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E11">
         <v>30</v>
@@ -3574,7 +3591,7 @@
         <v>47</v>
       </c>
       <c r="H11" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="I11">
         <v>0.67</v>
@@ -3582,7 +3599,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B12">
         <v>32.5</v>
@@ -3591,7 +3608,7 @@
         <v>29</v>
       </c>
       <c r="D12" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -3603,7 +3620,7 @@
         <v>47</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="I12">
         <v>0.95</v>
@@ -3611,7 +3628,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B13">
         <v>238000</v>
@@ -3620,7 +3637,7 @@
         <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E13">
         <v>10</v>
@@ -3632,7 +3649,7 @@
         <v>15</v>
       </c>
       <c r="H13" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="I13">
         <v>0.65</v>
@@ -3640,7 +3657,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B14">
         <v>9500</v>
@@ -3669,7 +3686,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B15">
         <v>4800</v>
@@ -3698,7 +3715,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B16">
         <v>80</v>
@@ -3733,7 +3750,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B17">
         <v>21000</v>
@@ -3742,7 +3759,7 @@
         <v>29</v>
       </c>
       <c r="D17" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="E17">
         <f>10^6</f>
@@ -3753,7 +3770,7 @@
         <v>13600.462476193932</v>
       </c>
       <c r="G17" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="I17">
         <v>0.2</v>
@@ -3761,7 +3778,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B19">
         <v>650</v>
@@ -3793,7 +3810,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3883,10 +3900,10 @@
         <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="D10" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -3928,109 +3945,109 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C2" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B3">
         <v>0.7</v>
       </c>
       <c r="C3" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B4">
         <v>0.18</v>
       </c>
       <c r="C4" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B5">
         <v>0.1</v>
       </c>
       <c r="C5" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B6">
         <v>0.38</v>
       </c>
       <c r="C6" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B7">
         <v>0.4</v>
       </c>
       <c r="C7" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B8">
         <v>0.06</v>
       </c>
       <c r="C8" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B9">
         <v>0.1</v>
       </c>
       <c r="C9" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B10">
         <v>0.25</v>
       </c>
       <c r="C10" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B11">
         <v>0.2</v>
       </c>
       <c r="C11" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -4073,7 +4090,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D3" t="s">
         <v>46</v>
@@ -4146,7 +4163,7 @@
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -4200,35 +4217,35 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B3">
         <v>35000</v>
       </c>
       <c r="C3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B4">
         <v>7920</v>
       </c>
       <c r="C4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B5">
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -4270,41 +4287,41 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B3">
         <v>0.19400000000000001</v>
       </c>
       <c r="C3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B4">
         <v>1204.67</v>
       </c>
       <c r="C4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D5" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -4317,7 +4334,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4327,7 +4344,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -4346,7 +4363,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B3">
         <v>2.5</v>
@@ -4355,7 +4372,7 @@
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -4369,12 +4386,12 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B5">
         <v>0.9</v>
@@ -4382,43 +4399,43 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B7">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D7" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B8">
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -4428,15 +4445,16 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{057E51FA-16AA-4EDB-95D7-E76738AA23C5}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.44140625" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -4460,62 +4478,43 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="B3">
-        <v>0.19400000000000001</v>
+        <v>14285714.300000001</v>
       </c>
       <c r="C3" t="s">
-        <v>105</v>
+        <v>101</v>
+      </c>
+      <c r="D3" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B4">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B5">
-        <v>50</v>
+        <v>20</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.5</v>
       </c>
       <c r="C5" t="s">
-        <v>105</v>
+        <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>107</v>
-      </c>
-      <c r="B6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" t="s">
         <v>40</v>
       </c>
     </row>
@@ -4526,23 +4525,24 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4E9EB40-91BA-4B28-833D-B3DB1EE1EE78}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.77734375" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4550,45 +4550,29 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4">
+        <v>10714285.699999999</v>
+      </c>
+      <c r="C4" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>119</v>
-      </c>
-      <c r="B5">
-        <v>40</v>
-      </c>
-      <c r="C5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>120</v>
-      </c>
-      <c r="B6">
-        <v>1.71</v>
-      </c>
-      <c r="C6" t="s">
-        <v>101</v>
+      <c r="D4" t="s">
+        <v>334</v>
       </c>
     </row>
   </sheetData>
@@ -4635,18 +4619,18 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B4">
         <v>174</v>
       </c>
       <c r="C4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B5">
         <v>1.54</v>

</xml_diff>

<commit_message>
Correction of conc. in brine, stripping sol and FO sol for Li instead of LiCl, implementation of plot for LDH opex
</commit_message>
<xml_diff>
--- a/data/LDH_attributes.xlsx
+++ b/data/LDH_attributes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chant\PycharmProjects\FUSE-V2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59ECE559-4848-4A5A-8D0D-E28A7C0F0D55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7034B639-7FFC-4A44-BE7C-6F01C83B51DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="7" xr2:uid="{9D386D14-BB1A-49FB-A5CB-94A6FCCCA1F9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="8" xr2:uid="{9D386D14-BB1A-49FB-A5CB-94A6FCCCA1F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Process overview" sheetId="23" r:id="rId1"/>
@@ -34,17 +34,26 @@
     <sheet name="equipment" sheetId="6" r:id="rId19"/>
     <sheet name="capex" sheetId="21" r:id="rId20"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="334">
   <si>
     <t>key</t>
   </si>
@@ -389,18 +398,6 @@
   </si>
   <si>
     <t>years</t>
-  </si>
-  <si>
-    <t>LiCl_conc_brine</t>
-  </si>
-  <si>
-    <t>LiCl_conc_stripping</t>
-  </si>
-  <si>
-    <t>LiCl_sol_output</t>
-  </si>
-  <si>
-    <t>LiCl_conc_FO</t>
   </si>
   <si>
     <t>plant_lifetime</t>
@@ -1102,6 +1099,15 @@
   </si>
   <si>
     <t>upscaled from Huang 2021 30l for 70g sorbent)</t>
+  </si>
+  <si>
+    <t>Li_conc_brine</t>
+  </si>
+  <si>
+    <t>Li_conc_stripping</t>
+  </si>
+  <si>
+    <t>Li_conc_FO</t>
   </si>
 </sst>
 </file>
@@ -1246,6 +1252,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1261,7 +1268,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1652,433 +1658,433 @@
   <sheetData>
     <row r="2" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N2" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="R2" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="S2" s="4" t="s">
         <v>232</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="12" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N12" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="O12" t="s">
         <v>107</v>
       </c>
       <c r="P12" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="Q12" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="S12" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="13" spans="14:20" x14ac:dyDescent="0.3">
       <c r="P13" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="S13" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="14" spans="14:20" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="P14" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="R14" s="6"/>
-      <c r="S14" s="13" t="s">
-        <v>244</v>
+      <c r="S14" s="14" t="s">
+        <v>240</v>
       </c>
       <c r="T14" s="6"/>
     </row>
     <row r="15" spans="14:20" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="P15" s="16" t="s">
-        <v>308</v>
+      <c r="P15" s="17" t="s">
+        <v>304</v>
       </c>
       <c r="R15" s="6"/>
-      <c r="S15" s="14"/>
+      <c r="S15" s="15"/>
       <c r="T15" s="6"/>
     </row>
     <row r="16" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="P16" s="16"/>
+      <c r="P16" s="17"/>
       <c r="R16" s="7"/>
       <c r="S16" s="8" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="T16" s="7"/>
     </row>
     <row r="19" spans="14:17" x14ac:dyDescent="0.3">
       <c r="N19" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="O19" t="s">
         <v>107</v>
       </c>
       <c r="P19" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="Q19" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="25" spans="14:17" x14ac:dyDescent="0.3">
       <c r="N25" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="O25" t="s">
         <v>107</v>
       </c>
       <c r="P25" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="26" spans="14:17" x14ac:dyDescent="0.3">
       <c r="P26" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="Q26" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="39" spans="14:18" x14ac:dyDescent="0.3">
       <c r="N39" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="O39" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="P39" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="Q39">
         <v>12</v>
       </c>
       <c r="R39" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="40" spans="14:18" x14ac:dyDescent="0.3">
-      <c r="P40" s="17" t="s">
-        <v>312</v>
+      <c r="P40" s="18" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="41" spans="14:18" x14ac:dyDescent="0.3">
-      <c r="P41" s="17"/>
+      <c r="P41" s="18"/>
     </row>
     <row r="42" spans="14:18" x14ac:dyDescent="0.3">
       <c r="P42" s="10"/>
       <c r="R42" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="52" spans="14:18" x14ac:dyDescent="0.3">
       <c r="N52" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="O52" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="P52" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="Q52" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="R52" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="53" spans="14:18" x14ac:dyDescent="0.3">
       <c r="P53" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="R53" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="70" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N70" t="s">
+        <v>258</v>
+      </c>
+      <c r="O70" t="s">
+        <v>259</v>
+      </c>
+      <c r="P70" t="s">
+        <v>260</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>261</v>
+      </c>
+      <c r="R70" t="s">
         <v>262</v>
       </c>
-      <c r="O70" t="s">
+      <c r="S70" s="9" t="s">
         <v>263</v>
-      </c>
-      <c r="P70" t="s">
-        <v>264</v>
-      </c>
-      <c r="Q70" t="s">
-        <v>265</v>
-      </c>
-      <c r="R70" t="s">
-        <v>266</v>
-      </c>
-      <c r="S70" s="9" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="71" spans="14:19" x14ac:dyDescent="0.3">
       <c r="P71" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="R71" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="72" spans="14:19" x14ac:dyDescent="0.3">
       <c r="P72" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="R72" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="73" spans="14:19" x14ac:dyDescent="0.3">
-      <c r="P73" s="16" t="s">
-        <v>310</v>
+      <c r="P73" s="17" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="74" spans="14:19" x14ac:dyDescent="0.3">
-      <c r="P74" s="16"/>
+      <c r="P74" s="17"/>
     </row>
     <row r="77" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N77" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="O77" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="P77" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="Q77" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="85" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N85" t="s">
+        <v>269</v>
+      </c>
+      <c r="O85" t="s">
+        <v>270</v>
+      </c>
+      <c r="P85" t="s">
+        <v>234</v>
+      </c>
+      <c r="Q85" t="s">
+        <v>271</v>
+      </c>
+      <c r="R85" t="s">
+        <v>272</v>
+      </c>
+      <c r="S85" t="s">
         <v>273</v>
-      </c>
-      <c r="O85" t="s">
-        <v>274</v>
-      </c>
-      <c r="P85" t="s">
-        <v>238</v>
-      </c>
-      <c r="Q85" t="s">
-        <v>275</v>
-      </c>
-      <c r="R85" t="s">
-        <v>276</v>
-      </c>
-      <c r="S85" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="86" spans="14:19" x14ac:dyDescent="0.3">
       <c r="O86" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="P86" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="R86" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="87" spans="14:19" x14ac:dyDescent="0.3">
       <c r="P87" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="R87" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="88" spans="14:19" x14ac:dyDescent="0.3">
       <c r="P88" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="R88" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="89" spans="14:19" x14ac:dyDescent="0.3">
-      <c r="P89" s="17" t="s">
-        <v>311</v>
+      <c r="P89" s="18" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="90" spans="14:19" x14ac:dyDescent="0.3">
-      <c r="P90" s="17"/>
+      <c r="P90" s="18"/>
     </row>
     <row r="94" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N94" t="s">
+        <v>266</v>
+      </c>
+      <c r="O94" t="s">
         <v>270</v>
       </c>
-      <c r="O94" t="s">
-        <v>274</v>
-      </c>
       <c r="P94" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="95" spans="14:19" x14ac:dyDescent="0.3">
       <c r="O95" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="100" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N100" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="O100" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="Q100" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="R100" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="101" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N101" t="s">
-        <v>289</v>
-      </c>
-      <c r="O101" s="15" t="s">
-        <v>290</v>
+        <v>285</v>
+      </c>
+      <c r="O101" s="16" t="s">
+        <v>286</v>
       </c>
       <c r="P101" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="Q101" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="102" spans="14:19" x14ac:dyDescent="0.3">
-      <c r="O102" s="15"/>
+      <c r="O102" s="16"/>
     </row>
     <row r="104" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N104" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="O104" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="P104" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="R104" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="S104" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="105" spans="14:19" x14ac:dyDescent="0.3">
       <c r="O105" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="R105" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="106" spans="14:19" x14ac:dyDescent="0.3">
       <c r="R106" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="107" spans="14:19" x14ac:dyDescent="0.3">
       <c r="R107" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="109" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N109" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="O109" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="110" spans="14:19" x14ac:dyDescent="0.3">
       <c r="O110" t="s">
+        <v>291</v>
+      </c>
+      <c r="P110" t="s">
         <v>295</v>
-      </c>
-      <c r="P110" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="116" spans="14:18" x14ac:dyDescent="0.3">
       <c r="N116" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="O116" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="P116" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="Q116" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="R116" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="117" spans="14:18" x14ac:dyDescent="0.3">
       <c r="O117" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="122" spans="14:18" x14ac:dyDescent="0.3">
       <c r="N122" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="O122" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="P122" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="123" spans="14:18" x14ac:dyDescent="0.3">
       <c r="N123" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="O123" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="P123" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="124" spans="14:18" x14ac:dyDescent="0.3">
       <c r="N124" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="O124" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="125" spans="14:18" x14ac:dyDescent="0.3">
       <c r="N125" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="O125" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -2110,7 +2116,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -2142,7 +2148,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B5" s="1">
         <v>2</v>
@@ -2216,7 +2222,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -2230,23 +2236,23 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B4" s="1">
         <v>0.9</v>
@@ -2257,7 +2263,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B5" s="1">
         <v>0.8</v>
@@ -2268,32 +2274,32 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B6">
         <v>298.14999999999998</v>
       </c>
       <c r="C6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D6" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="B7" s="18">
+      <c r="A7" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B7" s="13">
         <v>10</v>
       </c>
-      <c r="C7" s="18" t="s">
-        <v>136</v>
+      <c r="C7" s="13" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B8" s="1">
         <v>2</v>
@@ -2307,7 +2313,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B9">
         <v>353</v>
@@ -2317,19 +2323,19 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="B10" s="18">
+      <c r="A10" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="B10" s="13">
         <v>1</v>
       </c>
-      <c r="C10" s="18" t="s">
-        <v>136</v>
+      <c r="C10" s="13" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
@@ -2385,18 +2391,18 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B15" s="3">
         <v>0.35</v>
       </c>
       <c r="D15" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B16">
         <v>0.8</v>
@@ -2404,7 +2410,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B17">
         <v>313.14999999999998</v>
@@ -2413,7 +2419,7 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -2541,21 +2547,21 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B3" s="11">
         <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="D3" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B4" s="12">
         <v>50</v>
@@ -2566,24 +2572,24 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B6">
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -2596,7 +2602,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="B8">
         <v>7920</v>
@@ -2798,14 +2804,14 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B3">
         <f xml:space="preserve"> 1.5 * 10^(-3)</f>
         <v>1.5E-3</v>
       </c>
       <c r="C3" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D3" t="s">
         <v>55</v>
@@ -2813,28 +2819,28 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B4" s="3">
         <v>2E-3</v>
       </c>
       <c r="C4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D4" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B5" s="1">
         <f>1.5*10^-3</f>
         <v>1.5E-3</v>
       </c>
       <c r="C5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D5" t="s">
         <v>40</v>
@@ -2865,16 +2871,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E2" t="s">
         <v>70</v>
       </c>
       <c r="F2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -2919,7 +2925,7 @@
         <v>95</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -2936,7 +2942,7 @@
         <v>95</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -2958,7 +2964,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B8">
         <v>0.17</v>
@@ -2970,12 +2976,12 @@
         <v>95</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B9">
         <f>30/45</f>
@@ -2989,10 +2995,10 @@
         <v>95</v>
       </c>
       <c r="E9" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -3041,142 +3047,142 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C2" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B3">
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="C3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B4">
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="C4" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B5">
         <v>0.1</v>
       </c>
       <c r="C5" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B6">
         <v>0.25</v>
       </c>
       <c r="C6" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B7">
         <v>0.02</v>
       </c>
       <c r="C7" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B8">
         <v>0.02</v>
       </c>
       <c r="C8" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B9">
         <v>0.22</v>
       </c>
       <c r="C9" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B10">
         <v>0.5</v>
       </c>
       <c r="C10" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B11">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="C11" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B12">
         <v>0.13500000000000001</v>
       </c>
       <c r="C12" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B13">
         <v>0.08</v>
       </c>
       <c r="C13" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B14">
         <v>5.7500000000000002E-2</v>
       </c>
       <c r="C14" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -3205,7 +3211,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -3213,7 +3219,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B3">
         <v>81890</v>
@@ -3222,59 +3228,59 @@
         <v>29</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B4" s="3">
         <v>20</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="H4" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B6">
         <v>0.2</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B7">
         <v>0.2</v>
       </c>
       <c r="D7" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B8">
         <v>2.7E-2</v>
       </c>
       <c r="D8" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -3324,10 +3330,10 @@
         <v>48</v>
       </c>
       <c r="E2" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="F2" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="G2" t="s">
         <v>7</v>
@@ -3344,7 +3350,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B3">
         <v>37500</v>
@@ -3373,7 +3379,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B4">
         <v>230000</v>
@@ -3402,7 +3408,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B5">
         <v>63000</v>
@@ -3431,7 +3437,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B6">
         <v>380000</v>
@@ -3454,7 +3460,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B7">
         <v>22000</v>
@@ -3463,7 +3469,7 @@
         <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E7">
         <v>1600</v>
@@ -3483,7 +3489,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B8">
         <v>37500</v>
@@ -3512,7 +3518,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B9">
         <v>230000</v>
@@ -3541,7 +3547,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B10">
         <v>75000</v>
@@ -3570,7 +3576,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B11">
         <v>100000</v>
@@ -3579,7 +3585,7 @@
         <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E11">
         <v>30</v>
@@ -3591,7 +3597,7 @@
         <v>47</v>
       </c>
       <c r="H11" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="I11">
         <v>0.67</v>
@@ -3599,7 +3605,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B12">
         <v>32.5</v>
@@ -3608,7 +3614,7 @@
         <v>29</v>
       </c>
       <c r="D12" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -3620,7 +3626,7 @@
         <v>47</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I12">
         <v>0.95</v>
@@ -3628,7 +3634,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B13">
         <v>238000</v>
@@ -3637,7 +3643,7 @@
         <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E13">
         <v>10</v>
@@ -3649,7 +3655,7 @@
         <v>15</v>
       </c>
       <c r="H13" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="I13">
         <v>0.65</v>
@@ -3657,7 +3663,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B14">
         <v>9500</v>
@@ -3686,7 +3692,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B15">
         <v>4800</v>
@@ -3715,7 +3721,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B16">
         <v>80</v>
@@ -3750,7 +3756,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B17">
         <v>21000</v>
@@ -3759,7 +3765,7 @@
         <v>29</v>
       </c>
       <c r="D17" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="E17">
         <f>10^6</f>
@@ -3770,7 +3776,7 @@
         <v>13600.462476193932</v>
       </c>
       <c r="G17" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="I17">
         <v>0.2</v>
@@ -3778,7 +3784,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B19">
         <v>650</v>
@@ -3900,10 +3906,10 @@
         <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="D10" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -3945,109 +3951,109 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C2" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B3">
         <v>0.7</v>
       </c>
       <c r="C3" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B4">
         <v>0.18</v>
       </c>
       <c r="C4" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B5">
         <v>0.1</v>
       </c>
       <c r="C5" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B6">
         <v>0.38</v>
       </c>
       <c r="C6" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B7">
         <v>0.4</v>
       </c>
       <c r="C7" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B8">
         <v>0.06</v>
       </c>
       <c r="C8" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B9">
         <v>0.1</v>
       </c>
       <c r="C9" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B10">
         <v>0.25</v>
       </c>
       <c r="C10" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B11">
         <v>0.2</v>
       </c>
       <c r="C11" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -4163,7 +4169,7 @@
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -4228,7 +4234,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B4">
         <v>7920</v>
@@ -4239,7 +4245,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B5">
         <v>20</v>
@@ -4258,7 +4264,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4287,7 +4293,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>331</v>
       </c>
       <c r="B3">
         <v>0.19400000000000001</v>
@@ -4312,16 +4318,16 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D5" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -4344,7 +4350,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -4363,7 +4369,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B3">
         <v>2.5</v>
@@ -4372,7 +4378,7 @@
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -4386,12 +4392,12 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B5">
         <v>0.9</v>
@@ -4399,43 +4405,43 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B7">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D7" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B8">
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -4487,7 +4493,7 @@
         <v>101</v>
       </c>
       <c r="D3" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -4527,8 +4533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4E9EB40-91BA-4B28-833D-B3DB1EE1EE78}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4552,7 +4558,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>116</v>
+        <v>332</v>
       </c>
       <c r="B3">
         <v>40</v>
@@ -4572,7 +4578,7 @@
         <v>101</v>
       </c>
       <c r="D4" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -4582,10 +4588,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{285FC4B4-1D25-4960-A894-56724304077E}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4619,24 +4625,13 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>118</v>
+        <v>333</v>
       </c>
       <c r="B4">
         <v>174</v>
       </c>
       <c r="C4" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>117</v>
-      </c>
-      <c r="B5">
-        <v>1.54</v>
-      </c>
-      <c r="C5" t="s">
-        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor changes to LDH attributes
</commit_message>
<xml_diff>
--- a/data/LDH_attributes.xlsx
+++ b/data/LDH_attributes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chant\PycharmProjects\FUSE-V2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7034B639-7FFC-4A44-BE7C-6F01C83B51DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8002B34-264B-4E4B-9A1B-104AC4DCFDC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="8" xr2:uid="{9D386D14-BB1A-49FB-A5CB-94A6FCCCA1F9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="11" xr2:uid="{9D386D14-BB1A-49FB-A5CB-94A6FCCCA1F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Process overview" sheetId="23" r:id="rId1"/>
@@ -2212,7 +2212,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2266,7 +2266,7 @@
         <v>150</v>
       </c>
       <c r="B5" s="1">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="D5" t="s">
         <v>40</v>
@@ -2432,7 +2432,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A0F109E-90BE-42A5-8DFF-EE3A7F8215F0}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -4590,8 +4590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{285FC4B4-1D25-4960-A894-56724304077E}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
changes to LDH.opex to adjust dtype of all opex_df columns to float, changes to labels in LDH.plots
</commit_message>
<xml_diff>
--- a/data/LDH_attributes.xlsx
+++ b/data/LDH_attributes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chant\PycharmProjects\FUSE-V2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8002B34-264B-4E4B-9A1B-104AC4DCFDC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D7F95E-1904-4733-BF9E-263D16CFD188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="11" xr2:uid="{9D386D14-BB1A-49FB-A5CB-94A6FCCCA1F9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="12" activeTab="17" xr2:uid="{9D386D14-BB1A-49FB-A5CB-94A6FCCCA1F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Process overview" sheetId="23" r:id="rId1"/>
@@ -2432,7 +2432,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A0F109E-90BE-42A5-8DFF-EE3A7F8215F0}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -3028,7 +3028,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3194,8 +3194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1330EF6F-438D-41F9-93CA-537B5AFAC263}">
   <dimension ref="A2:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>